<commit_message>
added April 8th and July 19th
</commit_message>
<xml_diff>
--- a/LUO.xlsx
+++ b/LUO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="377">
   <si>
     <t>Jii 7 jowito ngimagi e masira mar apaya yoo Kisian e County ma Kisumu</t>
   </si>
@@ -926,6 +926,234 @@
   </si>
   <si>
     <t>Jalup apisa maduong’ e rito lee mag bunge e county ma Kisumu gi Siaya Joseph Nyingesa wacho ni chenro mar chudono nyalo bedo ni gwaro to kata kamano piny owacho to gikone nyaka chudi.</t>
+  </si>
+  <si>
+    <t>Jadolo Muheria mar Catholic okwayo kuonde lamo duto mapachoka mondo joyie oluu chike duto mane oketi mag kedo gi Covid-19</t>
+  </si>
+  <si>
+    <t>Jakom komiti mar jotend dinde mane ochuogi mag rango kaka kuonde lamo chopo chike mag kedo gi Coronavirus kapok oyau kuonde lamogo , jadolo mar kanisa mar Catholic mapachoka Anthony Muheria koro kwayo jotend dinde duto mathurka mondo jotemie neno ni chike ma oketi mag kedo gi Coronavirusgo dhano oluwo e kuonde lamogo kaka duarore</t>
+  </si>
+  <si>
+    <t>Kanomedowuoyo ewii wachno jadolo Muheria mabende e jatend diocese mar Catholic ma gwenge mag Nyeri ne owacho ni en gima ochuno mondo jolemo duto joluu chike moketi gi sirikalgo mondo okonygi e geng’o gamo midusi mar Covid-19no</t>
+  </si>
+  <si>
+    <t>Magi ne owacho ni esechegi makoro ne iyawoe kanise mapachoka ei kawuononi</t>
+  </si>
+  <si>
+    <t>To kumachielo bende jadolo Muheria bende ne okwayo jolemo duto mathurka mondo joket lamo ewii tuo mar Coronavirusni mondo mi Nyasaye orie bade kendo golo tuono e kind oganda – ma ochwe odhi chutho</t>
+  </si>
+  <si>
+    <t>Kanise ma County ma Kisumu ne oyepo ei odiechieng makoro ne oyawie kanise e thurkani</t>
+  </si>
+  <si>
+    <t>Kanise ma County ma Kisumu kawuono ne jonie odiechieng mar ariyo mar yuoro e weche mag alam bang yepo mag kanise e pachoka</t>
+  </si>
+  <si>
+    <t>Nonro mane otim gi Radio Ramogi ne oyango ni jolemo ne joyuoro e alam e kanise buora kaka kanisa mar Catholic , Anglican kod Deliverence Church kuom mamoko</t>
+  </si>
+  <si>
+    <t>Arch Bishop Joel Ofuna mar kanisa mar Ruwe Holy Ghost Church of East Africa ne oyango ni ne gichopo chike duto mane migao mochungne yoore mag thieth e pachoka ne duaro ni giluu mar neno ni jolemo mane odhi kuno ok jonyal gamo tuo mar Coronavirus</t>
+  </si>
+  <si>
+    <t>Kanomedowuoyo ewii wachno Bishop Ofuna nowacho ni giduaro temo neno ni onge ng’ata ng’ata magamo tuono e kuonde mag lamogo</t>
+  </si>
+  <si>
+    <t>Kanowuoyo gi Radio Ramogi , jadolono katakamano nowacho ni pod nitie kanise modhuro mapod nigi sida mar ng’iewo rapim liet mar del mabende ong’ere gi dho ngere kaka thermo gun ma iwacho ni nengone nimalo</t>
+  </si>
+  <si>
+    <t>Katakamano ne owacho ni kanise duaroee mondo jotemie luwo tir chike duto mane oketi gi piny owacho mag rakruok gi tuono</t>
+  </si>
+  <si>
+    <t>Midhiero mag kanisni</t>
+  </si>
+  <si>
+    <t>Jotelo mag county ma Siaya ojiwu mondo mii josir kanisni kendo neno ni gibedo gi nyalo mar yawo chenro mag alam kagiluwore gi okenge ma oketi mag geng’o landruok mar midhusi mar coronavirus.</t>
+  </si>
+  <si>
+    <t>MCA ma ward ma Usonga e kar chung od bura ma Alego Usonga migosi Silvestre Madialo wacho ni nitie kanisni ma dhii rem yawo chenro mag alam nimar gionge kod nyalo mar chopo dwaro ma piny owacho oketo</t>
+  </si>
+  <si>
+    <t>Kwan jii maromo 688 ne oyudi ei kawuononi ni nigi Coronavirus e pachoka</t>
+  </si>
+  <si>
+    <t>Kwan jii maromo 688 mane oyudi kawuononi ni nikod tuo mar Coronavirus makoro kelo kwan duto mag jogo man kod midusi magalagalano e pachoka chopo jii alufu 12 gi 750</t>
+  </si>
+  <si>
+    <t>Magi ne oyangi gi jatend migao mochungne yoore mag thieth e pachoka migosi Mutahi Kagwe mane owacho ni kuom jii 688 go ng’ama hike ne tin mogik ne en nyathi moro ma ja dweche 7 ka mane hike duong mogik ne ja higni 95</t>
+  </si>
+  <si>
+    <t>Kanowuoyo gi jopiny kachiel kachiel e tipo mar telebisen kowuok e County ma Embu migosi Kagwe bende ne oyango ni jii 3 moko ne tuono olal gi ngimagi kawuononi makoro ne kelo kwan jogo duto ma tuono osenego e pachoka chopo jii 225 kod bende lero ni nitie jii 457 mane ochango ma owe odhi pacho ei kawuononi makoro kelo kwan jogo duto ma osechango e thurka chopo jii alufu 4 gi 440</t>
+  </si>
+  <si>
+    <t>Katakamano ne odhi nyime gi kwayo oganda jokenya duto mondo joyie okau lwenj kedo gi tuo mar Covid-19no ka margi giwegi maok weye ne mana piny owacho kende</t>
+  </si>
+  <si>
+    <t>DICHUO ODERE KA POLIS BANG’ NEGO WUON MARE</t>
+  </si>
+  <si>
+    <t>Dichuo moro ma ja higni 41 ma nyocha omaki kuom nego wuongi  ka gilaro wach  bando, okaw ngimane e cell mar obila. OCPD ma Ikolomani Joseph Chesire, oyango wachno kolero ni Raytone Luhombo mawuok e gweng ma Matundu  yoo Kakamega, nodere  kotiyo gi sati manorwako e cell mar tesend obila ma Malinya , kama osebed kolorne nyaka noneg wuon mare ma ja higni 68 no alfred isutsi.</t>
+  </si>
+  <si>
+    <t>Joyuak noyudo osechako chenro mar iko jaduongno kawuono e seche manokelnegi wach ni rawuoyino bende odere.</t>
+  </si>
+  <si>
+    <t>Riuruok mar bisobe mag oganda jokopere koro dhi nyime gi kedo gi tuo mar kahera e County ma Kisumu</t>
+  </si>
+  <si>
+    <t>Riuruok mar bisobe mag oganda jokopere mong’ere kaka Kenye Conference of Catholic Bishops kokalo kuom chenro manyochane gichako mar kedo kod landruok mar tuo mar kahera mong’ere kaka Komesha TB Program sani jodhi nyime gi puonjo jopiny e County ma Kisumu ewii wach dhi e pim mar ng’eyo chal mari ne tuo mar kaherano</t>
+  </si>
+  <si>
+    <t>Maendi koro ne gichako kaluwore kod wach kwan matin mag jii mawuok oko mar dhi e kuonde thieth nikech giluoro wach tuo mar Coronavirus masani koro landore ka maa tiang e piny Kenyani</t>
+  </si>
+  <si>
+    <t>Kanowuoyo e Sub County ma Nyakach laktar Sam Oduor Muga maen manager mar chenro mar Komesha TB no mabende osir gi USaid nowacho ni githiedho tuo mar kaherano nono maonge chudo e osiptende mag misen ka gisiro chenro mag thieth nonogo</t>
+  </si>
+  <si>
+    <t>Zipporrah Orucho maen Coordinator mar weche mag kedo gi tuo mar kaherano e Sub County ma Nyakach kuno nowacho ni gikedo mar golo luoro ma dhano nigo e weche mag thieth mar tuo mar kaherano kaachiel gi golo akwede moko ma dhano jokwedogo joma giwinjo ni nigi tuo mar kaherano</t>
+  </si>
+  <si>
+    <t>George Oliech maen jatij kar thieth ma Nyabondo Mission Hospital nowacho ni osebedo ka otiyo tij wuoyo gi jogweng mondo joyie odhi e pim mar kahera mondo mi ging’e chal margi koluwore gi tuono kanowacho ni tuo mar kahera en tuo migamo gie yamo ma kaok ong’i wachne maber to yot mondo mi oket ngima oganda kamarach</t>
+  </si>
+  <si>
+    <t>SENETA SAKAJA ORAMO NI NE OK OMAKE</t>
+  </si>
+  <si>
+    <t>Kata kamano andike mare e mbui mar twitter omedo mana jimbo wach ka jokenya mathoth medo kwede  kuom rocho chike mag curfew  moketi gi piny owacho  to en e jakom mar kamati mar senate e wi midhusi mar corona.</t>
+  </si>
+  <si>
+    <t>Senator ma Nairobi Johnson Sakaja koro okwedo lipode ni nomake  monindo e tesend obila ma Kilimani otieno mokalo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kokalo e mbui mare mar twitter,  Sakaja wacho ni jok ma lando meko mare onego ochiw namba mar OB manondikne kobila kaka yoo mar bedo gi adiera e wi meko mare.</t>
+  </si>
+  <si>
+    <t>OPAMO DWARO RATIRO MARGI</t>
+  </si>
+  <si>
+    <t>Piny owacho mag Counties okwa mondo oket thenge kwan omenda moro mar konyo opamo mae Counties go ma sani kaloe kinde matek mokalo kaluwore gi midhiero mokel gi mucoh mar midhusi mar corona.</t>
+  </si>
+  <si>
+    <t>Riwruok moro ni sauti ya wanawake bade ma ka nam chumbi kokalo kuok jakomgi Dorcas Jibran, owacho ni andwayogo ok nyal yudo kaka chiemo wira ni chike moketi gi piny owacho oridore negi mokalo.</t>
+  </si>
+  <si>
+    <t>Nowacho ni counties onego omigi kony mar yudo kaka ginyalo medo dago ngima maber.</t>
+  </si>
+  <si>
+    <t>LADY MAUREEN POK OIKI</t>
+  </si>
+  <si>
+    <t>Kata kamano jopiny ok odewo wach mdhusi mar Corona wira ni dhano odhugni malich mokalo e kama inene ringre jangolono.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ringre jangolo mar ohangla lady Maureen pod ni e alak  mar sikul ma Kopanga kama jopiny pod nene ringre kapok okowe kar yueyo mare mogik. </t>
+  </si>
+  <si>
+    <t>Motelo noseter ringre pacho mak mana ni johera mage noyudho ringre motero e sikund primar ma Kopanga kama jopiny nene e yor kwe.</t>
+  </si>
+  <si>
+    <t>DOHO MA KISUMU OPUODHO OMBARA</t>
+  </si>
+  <si>
+    <t>Doho wacho ni Ombara kuom mano ne ok obalo gi chik mar doho.</t>
+  </si>
+  <si>
+    <t>Go ma Kisumo owacho ni City manager Doris Ombara ne ok otimo keth moro amora kaluwore gi okang mare mar  muko chiro ma kibuye e okang mar bero chirono.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jangad bura wacho ni winjruok ne obedo kendo jo ohalago nodar modhi kamachielo  mane gidhi use ka girito tiek gedo mar chirono.</t>
+  </si>
+  <si>
+    <t>OLORNE RINGRE WUODGI NIKECH GOWI MADUONG’.</t>
+  </si>
+  <si>
+    <t>Familia moro e gweng ma Malela ei West Kabuoch  location e Sub County ma Ndhiwa sani jokwayo kony mondo mi giyud ringre wuodgi moselorne kuom kinde buora e kar kano ringruok moro ma eldoret e wi bill mar siling 759,000</t>
+  </si>
+  <si>
+    <t>Anyuolano wacho ni wuodgi ma ja higni 44 no osebet e osiptal ma Eldoretno kuom jumbe ariyo kane en gi Cancer mar remo ema kaeto bangé nowito ngimane.</t>
+  </si>
+  <si>
+    <t>Weg osiptal mar jii giwegino olero ni ok ginyal chiwo ringre jalo nyaka chul bill go duto.</t>
+  </si>
+  <si>
+    <t>Ng’ur e od bura ma Homabay</t>
+  </si>
+  <si>
+    <t>Lemo mar jatend kweth mathoth ne omii MCA ma Kanyaluo ward Jeff Ongoro ka lemo mar spika ne omii MCA ma Kabondo West migosi Godfrey Anyango ma ongere kaka Goody Goody.</t>
+  </si>
+  <si>
+    <t>MCA ma Kanyadoto ward Walter Were Muok manyo omaa lemo mar jetend kweth mathoth e od burano nyoro, ywak ni yierruok ne obedo kendo nitie gwenge ma ok omii thuolo mar telo.</t>
+  </si>
+  <si>
+    <t>Jatuo maja piny China oketi e ward e kar kende e hopspital ma Agakhan hospital Kisumu kaluwore gio luoro marni onyalo bedogi midhusi mar Corona Virus</t>
+  </si>
+  <si>
+    <t>Ja Chinano matiyo e kambi magero apaya e boma ma Ugunja county ma Siaya wachore ni nyoro oter e kar thiethno otieno manyoro gi miyo moro kendo esache mane irwake ei od thieth to ne orwakne leuni mag arita ma pononi ne onyalo bedogi midhusino to ne ok onyal landore kuom jok mamoko</t>
+  </si>
+  <si>
+    <t>Laktere wachoni jatuono ne okuong othiedhi gi tuo mar pneumonia ka katakamno ne oduog okete ei ward maentie kar kende kama osekawie ranyisi mar timo pim kendo yango kadiponi onyalo bedogi midhusi mar Coronano kata ooyo.</t>
+  </si>
+  <si>
+    <t>Katakamano kane odwar pache ewi wachni to directa mochungne chenro mag thieth e kar thieth ma Aghakan Dr. Patrick Eshiwani ne okoni ne entie e romo moro kendo ne ok oduogo oyua tol machiwo ler ewi wachno</t>
+  </si>
+  <si>
+    <t>Jagoro maduong mar duond bura mar Jubilee Raphael Tuju ne oter gi ndege nyaka epinje maoko dhi yudo thieth moyiedhi kaluwore gi masira mar apaya mane ojuke e apaya maduong mawuok Nairobika nyaka Nakuru.</t>
+  </si>
+  <si>
+    <t>Duond bura mar Jubilee e ote makende ne ute fuambo gi keyo kokalo kuom directa mochungne yore tudruok Albert Nemusi, wachoni familia mar tuju ema okawo okang’ mar tere e pinje maoko bang lalruok giu laktare mane thiedhe e pachoka</t>
+  </si>
+  <si>
+    <t>Tuju kaluwore gi memusi nyo osegol e kar thieth mar jotuo mangimagi nitie kama rach kendoni nyo osepiele e ward mapile kaluwore gi kaka ngimane nyo osechako bedogi lokruok</t>
+  </si>
+  <si>
+    <t>Tuju ne oromo gi masira mar apaya makamano tarik 12 dweni kane oriko entie e safar kane odhi e hiiko mar ker mar 2 mapachoka jaduong Daniel Arap Moi Kabarak.</t>
+  </si>
+  <si>
+    <t>Kaluwore gi ripord obila nyamburko mar tuju ne otuomore gi matatu mane temo kalo nyamburko mamoko e apayano ka tije manyocha ne Tuju timo e duond bura mar jubilee itimo gi apisa maduong james waweru makonyore gi apisas mamoko nyaka chop Tuju bii duogi kowuok e hospital.</t>
+  </si>
+  <si>
+    <t>Manyaloromo familia 10 sani jodong maonge kuma chuoyee wigi bang mach maratipo wang’o utegi e dho wath ma Sena Beach , Mfang’ano East location , Suba North e County ma Homa Bay</t>
+  </si>
+  <si>
+    <t>Majno nyo owang’o udigi ei otieno mane piny oruugo kawuononi</t>
+  </si>
+  <si>
+    <t>Majno mabende nyo omuoch kar saa adek mar otieno mane piny oruugo kawuononi ne owang’o udi 6 mag apanga ma odong mana mirni olilo nyaka mwandu mane nie igi duto bende</t>
+  </si>
+  <si>
+    <t>Kanowuoyo ewii wachno jatend obila ma County ma Homa Bay Esther Seroney nowacho ni majno nyo omuoch e achiel kuom udigo ni ema kaeto nyo olandoree ma odhi e udi mamoko ma owang’o duto gi mwandu e igi ma oweyo weg udigo ka jodong chwata gi lwetgi nono makata gima digiwachi ni gidonggo onge</t>
+  </si>
+  <si>
+    <t>Kanomedowuoyo ewii wachno Seroney nowacho ni majno ne owang’o udigo kod mwandu duto manyo nie igi makoro nyo ochuno weg udigo mondo jonind oko e koyo</t>
+  </si>
+  <si>
+    <t>Obila mawuok e tesend obila ma Sena Patrol Base mane joringo odhi e kama nyo masirano otimoreeno nyo jotemo konyo e nego majno ka jotenore kod jopiny to katakamano nyo nego majno otamore nikech nyo oselandore ma omako udigo duto</t>
+  </si>
+  <si>
+    <t>Jatend obilano nowacho ni gisechako timo nonro mar yango gima dinyo kel majno</t>
+  </si>
+  <si>
+    <t>Katakamano onge ng’ata ng’ata manyo ohinyore kata tho e masirano</t>
+  </si>
+  <si>
+    <t>Obila e kaunti ma Mombasa pedho achije moko angwen  mane omonjo wuon duka moro e gweng ma Chaani eodbura ma Changamwe Mombasa kuma ne gikwale kwan omwom mapok oyangi eotieno mane piny ruugo kawuono.</t>
+  </si>
+  <si>
+    <t>Kaneoyango wachnoendo komanda mar obila ma Changamwe Ali Ndiema wacho achijego mane jomanore gi musdhola ne jotingore e apiko achiel esche mag monjno mane gitimo kar saa angwen motieno.</t>
+  </si>
+  <si>
+    <t>Wachore ni achijego ne owuodho musdhola to kae to gichikone wuon dukane kagike ni oywa dhot kuna ne gidonje kae to gichoko pesa duto mane giyudo.</t>
+  </si>
+  <si>
+    <t>Ne ochuno jonjorego muocho magina ariyo e kor yamo kakoro giwuok mar keyo moko kuom jopiny mane oseyuoro modino negi bang winjo nduru mar wuon dukanoendo makatakamano ne otony maonge hinyruok.</t>
+  </si>
+  <si>
+    <t>Jochiwu thieth e osiptal ma mine ma pumwani jong’anyo tich kagibandho chudo mar osara ma giywak ni pok ochulgi kuom dweche 4.</t>
+  </si>
+  <si>
+    <t>Ma ok tin ne jochiwu thieth 70 ma ondiki e yor kojolo kata contract odagi donjo e tich kendo gibago ng’anyo kagikoo ne jatend osiptandno Geoffrey Mosira ochulgi osara ma osekunore kochakore dwee mar 11 higa mokalo.</t>
+  </si>
+  <si>
+    <t>Peter Mwangi gi Judith Adongo ma otelo ne kweth jochiwu thieth ma ng’anyogo ywakni gikadhe midhiero mathoth e osiptandno ma Pumwani.</t>
   </si>
 </sst>
 </file>
@@ -2822,10 +3050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B284"/>
+  <dimension ref="A1:B360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268"/>
+    <sheetView tabSelected="1" topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="B357" sqref="B357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3690,7 +3918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="45">
+    <row r="108" spans="1:2">
       <c r="A108" s="10" t="s">
         <v>138</v>
       </c>
@@ -3698,7 +3926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="45">
+    <row r="109" spans="1:2" ht="30">
       <c r="A109" s="11" t="s">
         <v>132</v>
       </c>
@@ -3706,7 +3934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="45">
+    <row r="110" spans="1:2" ht="30">
       <c r="A110" s="11" t="s">
         <v>133</v>
       </c>
@@ -3714,7 +3942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="45">
+    <row r="111" spans="1:2" ht="30">
       <c r="A111" s="11" t="s">
         <v>134</v>
       </c>
@@ -3722,7 +3950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="45">
+    <row r="112" spans="1:2" ht="30">
       <c r="A112" s="11" t="s">
         <v>135</v>
       </c>
@@ -3730,7 +3958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="45">
+    <row r="113" spans="1:2" ht="30">
       <c r="A113" s="11" t="s">
         <v>136</v>
       </c>
@@ -3738,7 +3966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="45">
+    <row r="114" spans="1:2" ht="30">
       <c r="A114" s="11" t="s">
         <v>137</v>
       </c>
@@ -3746,7 +3974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="75">
+    <row r="115" spans="1:2" ht="30">
       <c r="A115" s="10" t="s">
         <v>139</v>
       </c>
@@ -3754,7 +3982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="75">
+    <row r="116" spans="1:2" ht="30">
       <c r="A116" s="11" t="s">
         <v>140</v>
       </c>
@@ -3762,7 +3990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="75">
+    <row r="117" spans="1:2" ht="30">
       <c r="A117" s="11" t="s">
         <v>141</v>
       </c>
@@ -3770,7 +3998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="75">
+    <row r="118" spans="1:2" ht="30">
       <c r="A118" s="11" t="s">
         <v>142</v>
       </c>
@@ -3778,7 +4006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="75">
+    <row r="119" spans="1:2">
       <c r="A119" s="11" t="s">
         <v>143</v>
       </c>
@@ -3786,7 +4014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="75">
+    <row r="120" spans="1:2" ht="30">
       <c r="A120" s="11" t="s">
         <v>144</v>
       </c>
@@ -3794,7 +4022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="75">
+    <row r="121" spans="1:2" ht="30">
       <c r="A121" s="11" t="s">
         <v>145</v>
       </c>
@@ -3938,7 +4166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="60">
+    <row r="139" spans="1:2">
       <c r="A139" s="10" t="s">
         <v>163</v>
       </c>
@@ -3946,7 +4174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="60">
+    <row r="140" spans="1:2" ht="45">
       <c r="A140" s="11" t="s">
         <v>164</v>
       </c>
@@ -3954,7 +4182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="60">
+    <row r="141" spans="1:2" ht="45">
       <c r="A141" s="11" t="s">
         <v>165</v>
       </c>
@@ -3962,7 +4190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="60">
+    <row r="142" spans="1:2" ht="45">
       <c r="A142" s="11" t="s">
         <v>166</v>
       </c>
@@ -3970,7 +4198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="60">
+    <row r="143" spans="1:2" ht="45">
       <c r="A143" s="11" t="s">
         <v>167</v>
       </c>
@@ -4034,7 +4262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="45">
+    <row r="151" spans="1:2">
       <c r="A151" s="10" t="s">
         <v>175</v>
       </c>
@@ -4042,7 +4270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="45">
+    <row r="152" spans="1:2" ht="30">
       <c r="A152" s="11" t="s">
         <v>176</v>
       </c>
@@ -4050,7 +4278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="45">
+    <row r="153" spans="1:2" ht="30">
       <c r="A153" s="11" t="s">
         <v>177</v>
       </c>
@@ -4066,7 +4294,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="45">
+    <row r="155" spans="1:2" ht="30">
       <c r="A155" s="11" t="s">
         <v>179</v>
       </c>
@@ -4082,7 +4310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="45">
+    <row r="157" spans="1:2" ht="30">
       <c r="A157" s="11" t="s">
         <v>181</v>
       </c>
@@ -4122,7 +4350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="75">
+    <row r="162" spans="1:2">
       <c r="A162" s="10" t="s">
         <v>186</v>
       </c>
@@ -4130,7 +4358,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="75">
+    <row r="163" spans="1:2" ht="30">
       <c r="A163" s="11" t="s">
         <v>187</v>
       </c>
@@ -4138,7 +4366,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="75">
+    <row r="164" spans="1:2" ht="30">
       <c r="A164" s="11" t="s">
         <v>188</v>
       </c>
@@ -4146,7 +4374,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="75">
+    <row r="165" spans="1:2" ht="30">
       <c r="A165" s="11" t="s">
         <v>189</v>
       </c>
@@ -4154,7 +4382,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="75">
+    <row r="166" spans="1:2" ht="30">
       <c r="A166" s="12" t="s">
         <v>190</v>
       </c>
@@ -4162,7 +4390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="75">
+    <row r="167" spans="1:2" ht="45">
       <c r="A167" s="11" t="s">
         <v>191</v>
       </c>
@@ -4170,7 +4398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="75">
+    <row r="168" spans="1:2" ht="45">
       <c r="A168" s="11" t="s">
         <v>192</v>
       </c>
@@ -4178,7 +4406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="75">
+    <row r="169" spans="1:2" ht="30">
       <c r="A169" s="11" t="s">
         <v>193</v>
       </c>
@@ -4186,7 +4414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="75">
+    <row r="170" spans="1:2" ht="45">
       <c r="A170" s="11" t="s">
         <v>194</v>
       </c>
@@ -4194,7 +4422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="75">
+    <row r="171" spans="1:2" ht="30">
       <c r="A171" s="11" t="s">
         <v>195</v>
       </c>
@@ -4202,7 +4430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="75">
+    <row r="172" spans="1:2" ht="45">
       <c r="A172" s="11" t="s">
         <v>196</v>
       </c>
@@ -4210,7 +4438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="75">
+    <row r="173" spans="1:2" ht="30">
       <c r="A173" s="11" t="s">
         <v>197</v>
       </c>
@@ -4306,7 +4534,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="45">
+    <row r="185" spans="1:2" ht="30">
       <c r="A185" s="11" t="s">
         <v>210</v>
       </c>
@@ -4322,7 +4550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="45">
+    <row r="187" spans="1:2" ht="30">
       <c r="A187" s="11" t="s">
         <v>212</v>
       </c>
@@ -4330,7 +4558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="60">
+    <row r="188" spans="1:2" ht="45">
       <c r="A188" s="11" t="s">
         <v>213</v>
       </c>
@@ -4338,7 +4566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="60">
+    <row r="189" spans="1:2" ht="30">
       <c r="A189" s="11" t="s">
         <v>214</v>
       </c>
@@ -4346,7 +4574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="60">
+    <row r="190" spans="1:2" ht="45">
       <c r="A190" s="11" t="s">
         <v>215</v>
       </c>
@@ -4354,7 +4582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="60">
+    <row r="191" spans="1:2" ht="45">
       <c r="A191" s="11" t="s">
         <v>216</v>
       </c>
@@ -4386,7 +4614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="60">
+    <row r="195" spans="1:2" ht="45">
       <c r="A195" s="11" t="s">
         <v>220</v>
       </c>
@@ -4394,7 +4622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="60">
+    <row r="196" spans="1:2" ht="30">
       <c r="A196" s="11" t="s">
         <v>221</v>
       </c>
@@ -4402,7 +4630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="60">
+    <row r="197" spans="1:2" ht="45">
       <c r="A197" s="11" t="s">
         <v>222</v>
       </c>
@@ -4538,7 +4766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="75">
+    <row r="214" spans="1:2">
       <c r="A214" s="11" t="s">
         <v>239</v>
       </c>
@@ -4546,7 +4774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="75">
+    <row r="215" spans="1:2" ht="30">
       <c r="A215" s="11" t="s">
         <v>240</v>
       </c>
@@ -4554,7 +4782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="75">
+    <row r="216" spans="1:2" ht="30">
       <c r="A216" s="11" t="s">
         <v>241</v>
       </c>
@@ -4562,7 +4790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="75">
+    <row r="217" spans="1:2" ht="30">
       <c r="A217" s="11" t="s">
         <v>242</v>
       </c>
@@ -4570,7 +4798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="75">
+    <row r="218" spans="1:2" ht="45">
       <c r="A218" s="11" t="s">
         <v>243</v>
       </c>
@@ -4578,7 +4806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="60">
+    <row r="219" spans="1:2" ht="45">
       <c r="A219" s="11" t="s">
         <v>244</v>
       </c>
@@ -4586,7 +4814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="60">
+    <row r="220" spans="1:2" ht="45">
       <c r="A220" s="11" t="s">
         <v>245</v>
       </c>
@@ -4594,7 +4822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="60">
+    <row r="221" spans="1:2" ht="45">
       <c r="A221" s="11" t="s">
         <v>246</v>
       </c>
@@ -4602,7 +4830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="45">
+    <row r="222" spans="1:2">
       <c r="A222" s="10" t="s">
         <v>1</v>
       </c>
@@ -4610,7 +4838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="45">
+    <row r="223" spans="1:2" ht="30">
       <c r="A223" s="11" t="s">
         <v>247</v>
       </c>
@@ -4618,7 +4846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="45">
+    <row r="224" spans="1:2" ht="30">
       <c r="A224" s="11" t="s">
         <v>248</v>
       </c>
@@ -4650,7 +4878,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="45">
+    <row r="228" spans="1:2" ht="30">
       <c r="A228" s="11" t="s">
         <v>252</v>
       </c>
@@ -4658,7 +4886,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="45">
+    <row r="229" spans="1:2" ht="30">
       <c r="A229" s="11" t="s">
         <v>253</v>
       </c>
@@ -4666,7 +4894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="75">
+    <row r="230" spans="1:2">
       <c r="A230" s="10" t="s">
         <v>0</v>
       </c>
@@ -4674,7 +4902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="75">
+    <row r="231" spans="1:2" ht="30">
       <c r="A231" s="11" t="s">
         <v>254</v>
       </c>
@@ -4682,7 +4910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="75">
+    <row r="232" spans="1:2" ht="30">
       <c r="A232" s="11" t="s">
         <v>255</v>
       </c>
@@ -4690,7 +4918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="75">
+    <row r="233" spans="1:2" ht="30">
       <c r="A233" s="11" t="s">
         <v>256</v>
       </c>
@@ -4698,7 +4926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="75">
+    <row r="234" spans="1:2" ht="45">
       <c r="A234" s="11" t="s">
         <v>257</v>
       </c>
@@ -4706,7 +4934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="75">
+    <row r="235" spans="1:2" ht="30">
       <c r="A235" s="11" t="s">
         <v>258</v>
       </c>
@@ -4714,7 +4942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="75">
+    <row r="236" spans="1:2" ht="30">
       <c r="A236" s="11" t="s">
         <v>259</v>
       </c>
@@ -4722,7 +4950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="75">
+    <row r="237" spans="1:2" ht="45">
       <c r="A237" s="11" t="s">
         <v>260</v>
       </c>
@@ -5104,6 +5332,614 @@
       </c>
       <c r="B284" s="5" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="30">
+      <c r="A285" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B285" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="60">
+      <c r="A286" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="45">
+      <c r="A287" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="A288" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B288" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="45">
+      <c r="A289" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="B289" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="A290" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="30">
+      <c r="A291" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="B291" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" ht="30">
+      <c r="A292" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B292" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="45">
+      <c r="A293" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="B293" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="30">
+      <c r="A294" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B294" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" ht="45">
+      <c r="A295" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B295" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" ht="30">
+      <c r="A296" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B296" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="A297" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B297" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" ht="30">
+      <c r="A298" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="B298" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" ht="45">
+      <c r="A299" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B299" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="B300" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" ht="30">
+      <c r="A301" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B301" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" ht="45">
+      <c r="A302" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" ht="60">
+      <c r="A303" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B303" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="30">
+      <c r="A304" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B304" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2">
+      <c r="A305" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="B305" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" ht="60">
+      <c r="A306" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="B306" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" ht="30">
+      <c r="A307" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="B307" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" ht="30">
+      <c r="A308" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="B308" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" ht="60">
+      <c r="A309" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="B309" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" ht="30">
+      <c r="A310" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="B310" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" ht="45">
+      <c r="A311" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="B311" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" ht="45">
+      <c r="A312" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="B312" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" ht="60">
+      <c r="A313" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="B313" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2">
+      <c r="A314" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" ht="30">
+      <c r="A315" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" ht="30">
+      <c r="A316" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" ht="45">
+      <c r="A317" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2">
+      <c r="A318" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" ht="45">
+      <c r="A319" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" ht="45">
+      <c r="A320" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2">
+      <c r="A321" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2">
+      <c r="A322" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" ht="30">
+      <c r="A323" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" ht="30">
+      <c r="A324" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" ht="30">
+      <c r="A325" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2">
+      <c r="A326" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" ht="30">
+      <c r="A327" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" ht="30">
+      <c r="A328" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2">
+      <c r="A329" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2">
+      <c r="A330" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" ht="45">
+      <c r="A331" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" ht="30">
+      <c r="A332" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
+      <c r="A333" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="B334" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" ht="30">
+      <c r="A335" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" ht="30">
+      <c r="A336" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" ht="30">
+      <c r="A337" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="B337" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" ht="45">
+      <c r="A338" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="B338" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" ht="45">
+      <c r="A339" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="B339" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" ht="45">
+      <c r="A340" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="B340" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" ht="45">
+      <c r="A341" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="B341" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" ht="45">
+      <c r="A342" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" ht="30">
+      <c r="A343" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="B343" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" ht="30">
+      <c r="A344" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="B344" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" ht="45">
+      <c r="A345" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="B345" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" ht="30">
+      <c r="A346" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="B346" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2">
+      <c r="A347" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="B347" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" ht="30">
+      <c r="A348" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="B348" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" ht="60">
+      <c r="A349" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="B349" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" ht="30">
+      <c r="A350" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="B350" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" ht="45">
+      <c r="A351" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="B351" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2">
+      <c r="A352" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="B352" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2">
+      <c r="A353" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B353" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" ht="45">
+      <c r="A354" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="B354" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" ht="45">
+      <c r="A355" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B355" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" ht="30">
+      <c r="A356" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="B356" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" ht="45">
+      <c r="A357" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B357" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" ht="30">
+      <c r="A358" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B358" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" ht="45">
+      <c r="A359" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B359" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" ht="30">
+      <c r="A360" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="B360" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added from week of August 10th
</commit_message>
<xml_diff>
--- a/LUO.xlsx
+++ b/LUO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="13335" windowHeight="2850" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="13335" windowHeight="2850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Combined_text" sheetId="9" r:id="rId1"/>
@@ -13,14 +13,14 @@
   </sheets>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2876" uniqueCount="1233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2914" uniqueCount="1252">
   <si>
     <t>Jii 7 jowito ngimagi e masira mar apaya yoo Kisian e County ma Kisumu</t>
   </si>
@@ -3721,13 +3721,71 @@
   </si>
   <si>
     <t>Count of ANYUOLA KAJEMBE YUAK NE KAGWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OD BUCH SENATE KINY NOROM KENDO E WI WACH POK OMENDA MAG COUNTIES.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KUOM THUOLO MAR OCHIKO OD BUCH SENATE KINY NOROM MAR TEMO MANYO WINJRUOK E YOO MAKARE MIBIRO TIYO GODO E POGO OMENDA MADHI E COUNTIES. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROMO MA KAMANO KINY NOTIMRE E KINDENI MA MOK KUOM SENATORS WACHO NI IBUOGOGI MONDO MI GIGOL PARO KALUWORE GI DWARO MAR PINY OWACHO. </t>
+  </si>
+  <si>
+    <t>SENATOR MA ELGEIYO MARAKWET KIPCHUMBA MURKOMEN, WACHO NI SAMORO KA WINJRUOK OK OYUDORE TO BIRO CHUNO NI MONDO OCHAK OCHWAL MBELE TWAK MA KAMANO.</t>
+  </si>
+  <si>
+    <t>SENATORS MALUNGORE NI TEAM KENYA TO SEYO JAGOOO OPORO MAR KWETH MATHOTH IRUNGU KANGATA MA GIWACHO NI NIGI DWARO MAR CHWALO KENDO TWAK MA KAMANO NYIME.</t>
+  </si>
+  <si>
+    <t>JO PAU NYUKA DWARO OLALO</t>
+  </si>
+  <si>
+    <t>JODAK MA PAU NYUKA EI KAKRAO WARD E SUB COUNTY MA SUNA EAST DWARO NI PINY OWACHO MA COUNTY MA MIGORI MONDO OGERNEGI OLALO MABIRO RINGO E WI AORA NYASARARA MONDO MI OTIEK MIDHIERO MA NYITHINDO MASOMO NYIKENDO PRIMARY SCHOOL THORO KALE E KINDE KOTH.</t>
+  </si>
+  <si>
+    <t>KOTELNEGI KOD ISMAIL AKEDE, JOPUONJRE MA NYIKENDO PRIMARY MANIE BATH AORANO KOMACHIELO THORO BEDO GI MDHIERO KA GIWACHO NI GISEGOO LIPORT MA KAMANO TIELO MANG’ENY KENDO NI LIPORT MARGI SEBEDO KA LWAR MANA E IT MODINO.</t>
+  </si>
+  <si>
+    <t>DICHUO MORO YUAGO RATIRO MVITA</t>
+  </si>
+  <si>
+    <t>DICHUO MORO MANTIE E KAR DAK MONGOHORE MA AMAZON EOD BURA MVITA MOMBASA KORO YWAGO RATICHE BANG OBILA WEYO THUOLO JARIEMBO MORO MANYOCHA OGWEYO MONEGO NYATHINE MAJAHIGNI APAR JUMBE ARIYO MOSEKALO.</t>
+  </si>
+  <si>
+    <t>WUON NYATHINO KONI NYAKA SANI POK GIWINJO WACH MORO AMORO KUWUOK KUOM OBILA KATA JAGO MANYOCHA ONEKONO, KA EN BENDE POD RINGERE NYATHINE POD OKWAMO E MORTUARY MAONGE KAKA OTER DALA ODHI OYIKI.</t>
+  </si>
+  <si>
+    <t>JAL MAONONEG NYATHINE ODAK GI LUORO</t>
+  </si>
+  <si>
+    <t>PINY OWACHO OLERO NI GISETIMO MATHOTH NE JOTHIETH</t>
+  </si>
+  <si>
+    <t>BAD MIGAO MAR THIETH OWACHO NI MOKO KUOM NGÚR MA LAKTACHE MA COUNTY MA NAIROBI NYOGOLO KANYO GICHIWO NOTICE MAR CHAKO NGANY GIN GIGO MA PINY OWACHO DHI NYIME GI LOSO MA BENDE MOKO KUOMGI OSELOSI.</t>
+  </si>
+  <si>
+    <t>JALUP JATEND MIGAO MAR THIETH DR MERCY MWANGANGI OLERO NI BAD MIGAONO OSEGOO OKANG E NENO NI GICHOPO YUAK MAG JOTHIETH MA THURKA.</t>
+  </si>
+  <si>
+    <t>E TWAK MA PILE KA PILE GI UTE FWAMBO MAR CHIWO LER E WI MIDHUSI MAR CORONA, DR MWANGANGI  NYOWACHO NI LAKTACHE DUTO MMA COUNTY MA NAIROBI NOSECHUL MBALANG MAGGI MOTUDORE GI WCAH MIDHUSI MAR KORONA.</t>
+  </si>
+  <si>
+    <t>OKWACH KICH OTHO E AORA KIPKELION</t>
+  </si>
+  <si>
+    <t>NYO EN LIT KOD KUYO YOO KIPKELION BANG APISA MORO MAR OKWACH KICH MA KIPKELION KOD MIYO MORO THO E PII ODHIAMBO MA NYORO BANG OHULA YUEROGI.</t>
+  </si>
+  <si>
+    <t>MCA MA KIPKELION ANTHONY RUTO, OYANGO NI JATEND OKWACH KICHNO MANOCHUNG’NE KIPKELION, NYOTHO E SECHE MA NYAMBURKO MARE MATIN MANYOTINGE KOD NYANO  NYO OHULA OYUAYO KANYO GITEMO NGÁDO NDARA MANYO PII OPONGÓ EMA NYO OYUA GARINO NYAKA EI AORA.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3912,6 +3970,12 @@
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -4264,7 +4328,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4317,10 +4381,13 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4839,7 +4906,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G17:H25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
@@ -4896,7 +4963,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A17:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
@@ -10250,7 +10317,7 @@
       </c>
     </row>
     <row r="1002" spans="1:1" ht="21">
-      <c r="A1002" s="21" t="s">
+      <c r="A1002" s="20" t="s">
         <v>1178</v>
       </c>
     </row>
@@ -10280,7 +10347,7 @@
       </c>
     </row>
     <row r="1008" spans="1:1" ht="21">
-      <c r="A1008" s="21" t="s">
+      <c r="A1008" s="20" t="s">
         <v>1184</v>
       </c>
     </row>
@@ -10310,7 +10377,7 @@
       </c>
     </row>
     <row r="1014" spans="1:1" ht="21">
-      <c r="A1014" s="21" t="s">
+      <c r="A1014" s="20" t="s">
         <v>1192</v>
       </c>
     </row>
@@ -10380,7 +10447,7 @@
       </c>
     </row>
     <row r="1028" spans="1:1" ht="21">
-      <c r="A1028" s="21" t="s">
+      <c r="A1028" s="20" t="s">
         <v>1205</v>
       </c>
     </row>
@@ -10400,7 +10467,7 @@
       </c>
     </row>
     <row r="1032" spans="1:1" ht="21">
-      <c r="A1032" s="21" t="s">
+      <c r="A1032" s="20" t="s">
         <v>1209</v>
       </c>
     </row>
@@ -10445,7 +10512,7 @@
       </c>
     </row>
     <row r="1041" spans="1:1" ht="21">
-      <c r="A1041" s="21" t="s">
+      <c r="A1041" s="20" t="s">
         <v>1218</v>
       </c>
     </row>
@@ -10465,7 +10532,7 @@
       </c>
     </row>
     <row r="1045" spans="1:1" ht="21">
-      <c r="A1045" s="21" t="s">
+      <c r="A1045" s="20" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -10485,7 +10552,7 @@
       </c>
     </row>
     <row r="1049" spans="1:1" ht="21">
-      <c r="A1049" s="21" t="s">
+      <c r="A1049" s="20" t="s">
         <v>1226</v>
       </c>
     </row>
@@ -10521,10 +10588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B891"/>
+  <dimension ref="A1:B910"/>
   <sheetViews>
-    <sheetView topLeftCell="A886" workbookViewId="0">
-      <selection activeCell="A895" sqref="A895"/>
+    <sheetView tabSelected="1" topLeftCell="A906" workbookViewId="0">
+      <selection activeCell="A909" sqref="A909"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17225,7 +17292,7 @@
       </c>
     </row>
     <row r="839" spans="1:2" ht="21">
-      <c r="A839" s="21" t="s">
+      <c r="A839" s="20" t="s">
         <v>1178</v>
       </c>
       <c r="B839" s="2" t="s">
@@ -17273,7 +17340,7 @@
       </c>
     </row>
     <row r="845" spans="1:2" ht="21">
-      <c r="A845" s="21" t="s">
+      <c r="A845" s="20" t="s">
         <v>1184</v>
       </c>
       <c r="B845" s="2" t="s">
@@ -17321,7 +17388,7 @@
       </c>
     </row>
     <row r="851" spans="1:2" ht="21">
-      <c r="A851" s="21" t="s">
+      <c r="A851" s="20" t="s">
         <v>1192</v>
       </c>
       <c r="B851" s="2" t="s">
@@ -17433,7 +17500,7 @@
       </c>
     </row>
     <row r="865" spans="1:2" ht="21">
-      <c r="A865" s="21" t="s">
+      <c r="A865" s="20" t="s">
         <v>1205</v>
       </c>
       <c r="B865" s="2" t="s">
@@ -17465,7 +17532,7 @@
       </c>
     </row>
     <row r="869" spans="1:2" ht="21">
-      <c r="A869" s="21" t="s">
+      <c r="A869" s="20" t="s">
         <v>1209</v>
       </c>
       <c r="B869" s="2" t="s">
@@ -17537,7 +17604,7 @@
       </c>
     </row>
     <row r="878" spans="1:2" ht="21">
-      <c r="A878" s="21" t="s">
+      <c r="A878" s="20" t="s">
         <v>1218</v>
       </c>
       <c r="B878" s="2" t="s">
@@ -17569,7 +17636,7 @@
       </c>
     </row>
     <row r="882" spans="1:2" ht="21">
-      <c r="A882" s="21" t="s">
+      <c r="A882" s="20" t="s">
         <v>1222</v>
       </c>
       <c r="B882" s="2" t="s">
@@ -17601,7 +17668,7 @@
       </c>
     </row>
     <row r="886" spans="1:2" ht="21">
-      <c r="A886" s="21" t="s">
+      <c r="A886" s="20" t="s">
         <v>1226</v>
       </c>
       <c r="B886" s="2" t="s">
@@ -17646,6 +17713,158 @@
       </c>
       <c r="B891" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" ht="30">
+      <c r="A892" s="9" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B892" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" ht="30">
+      <c r="A893" s="9" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B893" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2" ht="30">
+      <c r="A894" s="9" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B894" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" ht="30">
+      <c r="A895" s="9" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B895" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2" ht="30">
+      <c r="A896" s="9" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B896" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2" ht="21">
+      <c r="A897" s="22" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B897" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" ht="105">
+      <c r="A898" s="11" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B898" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2" ht="84">
+      <c r="A899" s="11" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B899" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" ht="21">
+      <c r="A900" s="22" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B900" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2" ht="84">
+      <c r="A901" s="11" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B901" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="902" spans="1:2" ht="84">
+      <c r="A902" s="11" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B902" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2" ht="21">
+      <c r="A903" s="22" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B903" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2" ht="21">
+      <c r="A904" s="22" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B904" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2" ht="84">
+      <c r="A905" s="11" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B905" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2" ht="63">
+      <c r="A906" s="11" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B906" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2" ht="84">
+      <c r="A907" s="11" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B907" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="908" spans="1:2" ht="21">
+      <c r="A908" s="22" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B908" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" ht="63">
+      <c r="A909" s="11" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B909" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2" ht="105">
+      <c r="A910" s="11" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B910" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -17658,7 +17877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2:M12"/>
     </sheetView>
   </sheetViews>
@@ -17940,8 +18159,8 @@
       <c r="M11">
         <v>29</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
added Feb 26th 2021
</commit_message>
<xml_diff>
--- a/LUO.xlsx
+++ b/LUO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELOHOME\OneDrive\Desktop\Masakhane\Luo-News-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6621471D-8F59-421F-9D3A-A4195F3CACE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992A0DE4-A32C-458D-95EA-D9A4BB72B0DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3232" uniqueCount="1401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3310" uniqueCount="1440">
   <si>
     <t>Jii 7 jowito ngimagi e masira mar apaya yoo Kisian e County ma Kisumu</t>
   </si>
@@ -4234,13 +4234,151 @@
   </si>
   <si>
     <t>Kanowuoyo e kanisa mar Moore Catholic Church Kairuri Parish mabende ne odhi yuagoe familia mar jatend oganda jokopere mapachoka Cardinal John Njue kuom tho mar nyamin Njue nogono laktar Ruto nowacho ni wach sieko mar BBIno osemono piny owacho mar Jubilee e timo chenro meke mag dongruok ne jopiny kabende ne osingo ne oganda ma Embu kuno ni piny owacho ohikore mar biro tieko wach gedo mag apaya makono</t>
+  </si>
+  <si>
+    <t>Jopur niang dwaro ni mondo kembe marego niang ochulgi omenda ma wuok kuom molases</t>
+  </si>
+  <si>
+    <t>Jagoro mar riuruok jopur niang migosi Ezra Okoth Olodi dwaro ni kembe marego niang ochul jopur go mwandu mamoko mabende wuok kuom niang kaka molasses kod mamoko.</t>
+  </si>
+  <si>
+    <t>Okoth wacho ni kembe marego niang loso omenda mathoth kuom mwandu mamaoko mabende wuoke niang mabende on’gere kaka by products.</t>
+  </si>
+  <si>
+    <t>Okoth wacho ni jopur bende onego oyud ber kowuok kuom mwandugo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chenro mar dwaro loko pend chike ma pachoka okao okang achiel nyime bang counties mohewo 24 kadho paro mar chik mar bbi </t>
+  </si>
+  <si>
+    <t>Koro en ayanga ni chenro mar dwaro loko pend chike ma pachoka okao okang achiel nyime bang counties mohewo 24 kadho paro mar chik mar bbi</t>
+  </si>
+  <si>
+    <t>Odiochineg ma kawuono counties 26  ne okadho paro ongo mar chik kaka ne igeno ka jogo masiro paro Onogo mar chik wacho ni mano nyiso ni chenro mar loko pend chike ma pachoka biro yudo sir kowuok kuom oganda jokenya .</t>
+  </si>
+  <si>
+    <t>Giesani wenge koro ochom ne od bura maamalo to kod mano mar senate mar twak e wii paro onogo kapok gibiro gichwale ne duol matayo weche yiero to kod tomg e pachoka iebc mar bago ombulu mago mar referendum.</t>
+  </si>
+  <si>
+    <t>Japuonj moro madichuo mapuonjo  St Pius Uriri boys sec  school  e subcounty ma  Uriri olalo ngimane e masira mar apaya</t>
+  </si>
+  <si>
+    <t>Japuonj moro madichuo mapuonjo  St Pius Uriri boys sec  school  e subcounty ma  Uriri olalo ngimane e masira mar apaya  mane ojuko lory mar tipa mar kambi jochina matimo gedo mar apaya kod apiko  ecenter mar Garage mantie Ururi e apaya maduong mar Migori Rongo.</t>
+  </si>
+  <si>
+    <t>Comanda mar obila  esub county ma Uriri Peter Njoroge owacho ni japuonj no maja igni 40 ne riembo apikone kadhi school  emane lory mar tipano otuome gi  yoka toke ma otho kanyo gi kanyo kendo ringre noter  e kar kano ringre ma Migori level 4 hospital</t>
+  </si>
+  <si>
+    <t>Njoroge owacho ni jopiny mane igi owang ne dwa wan’go lorry mar tipano kata kamano obila ne ogen’gogi.</t>
+  </si>
+  <si>
+    <t>BBI ochomo ng’iende</t>
+  </si>
+  <si>
+    <t>Geno mar jogo ma siro paro mar chik mar BBI kawuono ni kuom ute bura ma ikore mar dhii goyo ombulu mar yie kata kwedo parono odiechieng’ ma kawuono.</t>
+  </si>
+  <si>
+    <t>Nyaka sani ute bura mag counties 12 osekadho paro mar chikno ka kwan ma dwarore mondo mii puodhe ne dhii e ombulu mar paro en ute bura mag counties 24.</t>
+  </si>
+  <si>
+    <t>Counties ma ute bura maggi igeno ni dhii tiekore gi wach bbi kawuono oriwo koda ka county ma Migori, county ma Nyamira, Mombasa, Kilifi, Nakuru, Nyeri, Embu, Kirinyaga, Makueni, Machakos, Kitui, Isiolo, Garissa, kod Taita-Taveta.</t>
+  </si>
+  <si>
+    <t>Raila ogolo siem ewii keto chik makumo tiyo gi dhok mar hustler</t>
+  </si>
+  <si>
+    <t>Ogai mar ODM migosi Raila Amolo Odinga ogolo siem ewii mar kumo tiyo gi dhok moro ni hustler manyochane jalup jatend piny Kenya laktar William Ruto ochako kaka ngero mare mar campaign e thurka kowacho ni keto chik makumo tiyo gi dhok machalo kamano romre gi ketho ratich oganda mar wacho dwachgi e pachoka</t>
+  </si>
+  <si>
+    <t>Kanomedowuoyo ewii wachno migosi Raila nowacho ni kata obedo ni kit siasa ailano sigande ok osebedo ka ber ahinya e pachoka kamano to nowacho ni paro kumo tiyo gi dhok moro ni hustler e campainno en gino manyaloketho weche mag demokrasia ma piny Kenyaka kod bende ketho thuolo ma onegobed ni imiyo oganda mar wacho pachgi kagin thuolo</t>
+  </si>
+  <si>
+    <t>Paro nyochane osebedo e thurka mar kalo chik moro mane birokumo tiyo gi dhokno kendo keto fuai maduong ne joma oyud katiyo gi dhok mar hustlerno kata tweyogi mondo gidhi gicham oganda iye</t>
+  </si>
+  <si>
+    <t>Doho ma Rongo on’gadone jago moro maike niediere buch twech mar igni 5 kod keth mar bambo rawera moro manyako maja igni 13</t>
+  </si>
+  <si>
+    <t>Doho ma Rongo  on’gado ne jago moro ma ike nie diere  buch twech mar igni 5 bang yie kod  keth mar bambo rawera moro  manyako maja igni 13.</t>
+  </si>
+  <si>
+    <t>Evance Onyango mane otere nyim  jan’gad  buche  Rymond  Lan’gat ne oyie ni ne otimo keth maka mano kendo ne on’gadne buch twech mar igni 5.</t>
+  </si>
+  <si>
+    <r>
+      <t>Onyango ne oketho chik mar  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13.2"/>
+        <color rgb="FF212529"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Sexual offences act  2006</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <color rgb="FF212529"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, kare no 3.</t>
+    </r>
+  </si>
+  <si>
+    <t>Onyango ne oketho chikno  ekind tarik 10 dwe mar achiel igani  gi tarik 19 dwe mar achiel igani egweng ma Nyarombo , Dede location Awendo sub county  kendo ne omake tarik 19 mar dwe mar achiel , kabende ne otere edoho mokuongo tarik 22 dwe mar achiel igani.</t>
+  </si>
+  <si>
+    <t>Doho ma malo ma Kisumo ogolo chik mondo piny owacho ma county ma Kisumo ochul Speaker machon mar countyno Ann Adul sh million 5.2</t>
+  </si>
+  <si>
+    <t>Doho mamalo ma Kisumo ogolo chik ne piny  owacho mar County ma Kisumo mondo mi ochul  Speaker machon mar county assembly ma Kisumono   Anne Adul omenda maromo million 5.2  kuom thuolo mar dweche ariyo.</t>
+  </si>
+  <si>
+    <t>Justice Stephen Radido  ne ochuno  clerk mar assembly Owen Ojuok, county secretary Geoffrey Kigochi  kod jatend migao mar omenda   George Okong’go mondo jondik piny ni gibiro timo chudo maka mano ekidienje ariyo kata two installments.</t>
+  </si>
+  <si>
+    <t>Okil mar Adul ne otero bura edoho tarik 4 dwe mar 8 iga mokalo mar donjone jii adek go kaluore kod tamruok luwo chik doho mane doho ogolo mondo mi ne chul Ann Adul  kaluore kod kaka ne odhiche oko ekom mar Speaker mar county assembly no eiga mar 2014.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piny owacho mar countyno osingo ni biro timo chudo ne Speaker machon no omenda maromo million 2.5 kochopo tarik 3 dwe mar adek  igani kendo omenda modon’g million 2.9 ibiro chulo tarik 19 mar dwe mar 4 igani. </t>
+  </si>
+  <si>
+    <t>Justice Radido  omedo ni burano ibiro winjo kendo tarik 21 mar dwe mar 4 mar rango kabende singo go ochopi.</t>
+  </si>
+  <si>
+    <t>Chudo mar spika machon ma Kisumu pod okwamo</t>
+  </si>
+  <si>
+    <t>Karan mar od bura ma Kisumu owen ojuok to kod jatend migao mar omenda e countnyno ongo george okongo, to kod jagoro mar county Geoffrey Kigochi igeno e doho kawuono mondo mii gidhi gichiwu ler mar gimomiyo giserem chulo omenda maromo silingis milion 5.2 ne spika machon ma Kisumu Anne Adul.</t>
+  </si>
+  <si>
+    <t>Jayal bura mar doho ma Kisumu ma winjo buche mag jotich stephen radido ogolo chik ne apisas 3go mondo mii jochop e nyim doho kawuono.</t>
+  </si>
+  <si>
+    <t>Doho dwaro ni giluok nyinggi mar gimomiyo ok nyal kawnegi okang’ mar chik kuom rem luwo chik mane doho osegolo ni chul mikayi Anne Adul.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruodhi gi jolupgi ecounty ma Siaya omi siem mondo owe tudore kod wede mamoko mar mayo mond liete gi nyithi kiye mwandu
+</t>
+  </si>
+  <si>
+    <t>Ruodhi gi jolupgi ecounty ma siaya omi siem mager kaluore kod tim moro mar timo tudruok mar mayo mond liete gi nyithi kiye mwandu ma owenegi.</t>
+  </si>
+  <si>
+    <t>Jalup County  Commissioner ma Siaya Enock Nyarango owacho ni giseyudo  buche moko ma ruodhi gi jolupgi tudore kod wede moko mar mayo mond liete gi nyithi kiye mwandu ma owenegi.</t>
+  </si>
+  <si>
+    <t>Migosi  Nyarango  mane owacho magi esach romo mar rango arita kwe mane otimore e apise mag IEBC  ma Siaya owacho ni tend nango ma osebedo katimo tim maka mano mondo owe mapiyo piyo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4452,6 +4590,18 @@
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.2"/>
+      <color rgb="FF212529"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="33">
@@ -4795,7 +4945,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4854,9 +5004,6 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4865,6 +5012,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -11129,10 +11282,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B1070"/>
+  <dimension ref="A1:B1109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1065" workbookViewId="0">
-      <selection activeCell="A1070" sqref="A1070"/>
+    <sheetView tabSelected="1" topLeftCell="A1104" workbookViewId="0">
+      <selection activeCell="A1109" sqref="A1109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -18409,7 +18562,7 @@
       </c>
     </row>
     <row r="911" spans="1:2" ht="20.399999999999999">
-      <c r="A911" s="23" t="s">
+      <c r="A911" s="22" t="s">
         <v>1252</v>
       </c>
       <c r="B911" s="6" t="s">
@@ -18417,7 +18570,7 @@
       </c>
     </row>
     <row r="912" spans="1:2" ht="15">
-      <c r="A912" s="24" t="s">
+      <c r="A912" s="23" t="s">
         <v>1253</v>
       </c>
       <c r="B912" s="6" t="s">
@@ -18433,7 +18586,7 @@
       </c>
     </row>
     <row r="914" spans="1:2" ht="15">
-      <c r="A914" s="24" t="s">
+      <c r="A914" s="23" t="s">
         <v>1255</v>
       </c>
       <c r="B914" s="6" t="s">
@@ -18457,7 +18610,7 @@
       </c>
     </row>
     <row r="917" spans="1:2" ht="15">
-      <c r="A917" s="24" t="s">
+      <c r="A917" s="23" t="s">
         <v>1258</v>
       </c>
       <c r="B917" s="6" t="s">
@@ -18473,7 +18626,7 @@
       </c>
     </row>
     <row r="919" spans="1:2" ht="15">
-      <c r="A919" s="24" t="s">
+      <c r="A919" s="23" t="s">
         <v>1260</v>
       </c>
       <c r="B919" s="6" t="s">
@@ -18481,7 +18634,7 @@
       </c>
     </row>
     <row r="920" spans="1:2" ht="20.399999999999999">
-      <c r="A920" s="23" t="s">
+      <c r="A920" s="22" t="s">
         <v>1261</v>
       </c>
       <c r="B920" s="6" t="s">
@@ -18489,7 +18642,7 @@
       </c>
     </row>
     <row r="921" spans="1:2" ht="79.2">
-      <c r="A921" s="25" t="s">
+      <c r="A921" s="24" t="s">
         <v>1262</v>
       </c>
       <c r="B921" s="6" t="s">
@@ -18497,7 +18650,7 @@
       </c>
     </row>
     <row r="922" spans="1:2" ht="39.6">
-      <c r="A922" s="25" t="s">
+      <c r="A922" s="24" t="s">
         <v>1263</v>
       </c>
       <c r="B922" s="6" t="s">
@@ -18505,7 +18658,7 @@
       </c>
     </row>
     <row r="923" spans="1:2" ht="20.399999999999999">
-      <c r="A923" s="23" t="s">
+      <c r="A923" s="22" t="s">
         <v>1264</v>
       </c>
       <c r="B923" s="6" t="s">
@@ -18513,7 +18666,7 @@
       </c>
     </row>
     <row r="924" spans="1:2" ht="59.4">
-      <c r="A924" s="25" t="s">
+      <c r="A924" s="24" t="s">
         <v>1265</v>
       </c>
       <c r="B924" s="6" t="s">
@@ -18521,7 +18674,7 @@
       </c>
     </row>
     <row r="925" spans="1:2" ht="59.4">
-      <c r="A925" s="25" t="s">
+      <c r="A925" s="24" t="s">
         <v>1266</v>
       </c>
       <c r="B925" s="6" t="s">
@@ -18529,7 +18682,7 @@
       </c>
     </row>
     <row r="926" spans="1:2" ht="79.2">
-      <c r="A926" s="25" t="s">
+      <c r="A926" s="24" t="s">
         <v>1267</v>
       </c>
       <c r="B926" s="6" t="s">
@@ -18537,7 +18690,7 @@
       </c>
     </row>
     <row r="927" spans="1:2" ht="79.2">
-      <c r="A927" s="25" t="s">
+      <c r="A927" s="24" t="s">
         <v>1268</v>
       </c>
       <c r="B927" s="6" t="s">
@@ -18553,7 +18706,7 @@
       </c>
     </row>
     <row r="929" spans="1:2" ht="39.6">
-      <c r="A929" s="25" t="s">
+      <c r="A929" s="24" t="s">
         <v>1271</v>
       </c>
       <c r="B929" s="6" t="s">
@@ -18569,7 +18722,7 @@
       </c>
     </row>
     <row r="931" spans="1:2" ht="79.2">
-      <c r="A931" s="25" t="s">
+      <c r="A931" s="24" t="s">
         <v>1270</v>
       </c>
       <c r="B931" s="6" t="s">
@@ -18577,7 +18730,7 @@
       </c>
     </row>
     <row r="932" spans="1:2" ht="20.399999999999999">
-      <c r="A932" s="23" t="s">
+      <c r="A932" s="22" t="s">
         <v>1273</v>
       </c>
       <c r="B932" s="6" t="s">
@@ -18585,7 +18738,7 @@
       </c>
     </row>
     <row r="933" spans="1:2" ht="59.4">
-      <c r="A933" s="25" t="s">
+      <c r="A933" s="24" t="s">
         <v>1274</v>
       </c>
       <c r="B933" s="6" t="s">
@@ -18593,7 +18746,7 @@
       </c>
     </row>
     <row r="934" spans="1:2" ht="79.2">
-      <c r="A934" s="25" t="s">
+      <c r="A934" s="24" t="s">
         <v>1275</v>
       </c>
       <c r="B934" s="6" t="s">
@@ -18601,7 +18754,7 @@
       </c>
     </row>
     <row r="935" spans="1:2" ht="79.2">
-      <c r="A935" s="25" t="s">
+      <c r="A935" s="24" t="s">
         <v>1276</v>
       </c>
       <c r="B935" s="6" t="s">
@@ -18609,7 +18762,7 @@
       </c>
     </row>
     <row r="936" spans="1:2" ht="20.399999999999999">
-      <c r="A936" s="23" t="s">
+      <c r="A936" s="22" t="s">
         <v>1277</v>
       </c>
       <c r="B936" s="6" t="s">
@@ -18617,7 +18770,7 @@
       </c>
     </row>
     <row r="937" spans="1:2" ht="59.4">
-      <c r="A937" s="25" t="s">
+      <c r="A937" s="24" t="s">
         <v>1278</v>
       </c>
       <c r="B937" s="6" t="s">
@@ -18625,7 +18778,7 @@
       </c>
     </row>
     <row r="938" spans="1:2" ht="59.4">
-      <c r="A938" s="25" t="s">
+      <c r="A938" s="24" t="s">
         <v>1279</v>
       </c>
       <c r="B938" s="6" t="s">
@@ -18633,7 +18786,7 @@
       </c>
     </row>
     <row r="939" spans="1:2" ht="59.4">
-      <c r="A939" s="25" t="s">
+      <c r="A939" s="24" t="s">
         <v>1280</v>
       </c>
       <c r="B939" s="6" t="s">
@@ -18641,7 +18794,7 @@
       </c>
     </row>
     <row r="940" spans="1:2" ht="79.2">
-      <c r="A940" s="25" t="s">
+      <c r="A940" s="24" t="s">
         <v>1281</v>
       </c>
       <c r="B940" s="6" t="s">
@@ -18649,7 +18802,7 @@
       </c>
     </row>
     <row r="941" spans="1:2" ht="40.799999999999997">
-      <c r="A941" s="23" t="s">
+      <c r="A941" s="22" t="s">
         <v>1282</v>
       </c>
       <c r="B941" s="6" t="s">
@@ -18657,7 +18810,7 @@
       </c>
     </row>
     <row r="942" spans="1:2" ht="59.4">
-      <c r="A942" s="25" t="s">
+      <c r="A942" s="24" t="s">
         <v>1283</v>
       </c>
       <c r="B942" s="6" t="s">
@@ -18673,7 +18826,7 @@
       </c>
     </row>
     <row r="944" spans="1:2" ht="59.4">
-      <c r="A944" s="25" t="s">
+      <c r="A944" s="24" t="s">
         <v>1236</v>
       </c>
       <c r="B944" s="6" t="s">
@@ -18681,7 +18834,7 @@
       </c>
     </row>
     <row r="945" spans="1:2" ht="59.4">
-      <c r="A945" s="25" t="s">
+      <c r="A945" s="24" t="s">
         <v>1237</v>
       </c>
       <c r="B945" s="6" t="s">
@@ -18697,7 +18850,7 @@
       </c>
     </row>
     <row r="947" spans="1:2" ht="79.2">
-      <c r="A947" s="25" t="s">
+      <c r="A947" s="24" t="s">
         <v>1239</v>
       </c>
       <c r="B947" s="6" t="s">
@@ -18705,7 +18858,7 @@
       </c>
     </row>
     <row r="948" spans="1:2" ht="79.2">
-      <c r="A948" s="25" t="s">
+      <c r="A948" s="24" t="s">
         <v>1240</v>
       </c>
       <c r="B948" s="6" t="s">
@@ -18713,7 +18866,7 @@
       </c>
     </row>
     <row r="949" spans="1:2" ht="20.399999999999999">
-      <c r="A949" s="23" t="s">
+      <c r="A949" s="22" t="s">
         <v>1241</v>
       </c>
       <c r="B949" s="6" t="s">
@@ -18721,7 +18874,7 @@
       </c>
     </row>
     <row r="950" spans="1:2" ht="79.2">
-      <c r="A950" s="25" t="s">
+      <c r="A950" s="24" t="s">
         <v>1242</v>
       </c>
       <c r="B950" s="6" t="s">
@@ -18729,7 +18882,7 @@
       </c>
     </row>
     <row r="951" spans="1:2" ht="79.2">
-      <c r="A951" s="25" t="s">
+      <c r="A951" s="24" t="s">
         <v>1243</v>
       </c>
       <c r="B951" s="6" t="s">
@@ -18745,7 +18898,7 @@
       </c>
     </row>
     <row r="953" spans="1:2" ht="79.2">
-      <c r="A953" s="25" t="s">
+      <c r="A953" s="24" t="s">
         <v>1286</v>
       </c>
       <c r="B953" s="6" t="s">
@@ -18753,7 +18906,7 @@
       </c>
     </row>
     <row r="954" spans="1:2" ht="59.4">
-      <c r="A954" s="25" t="s">
+      <c r="A954" s="24" t="s">
         <v>1287</v>
       </c>
       <c r="B954" s="6" t="s">
@@ -18761,7 +18914,7 @@
       </c>
     </row>
     <row r="955" spans="1:2" ht="79.2">
-      <c r="A955" s="25" t="s">
+      <c r="A955" s="24" t="s">
         <v>1288</v>
       </c>
       <c r="B955" s="6" t="s">
@@ -18769,7 +18922,7 @@
       </c>
     </row>
     <row r="956" spans="1:2" ht="79.2">
-      <c r="A956" s="25" t="s">
+      <c r="A956" s="24" t="s">
         <v>1289</v>
       </c>
       <c r="B956" s="6" t="s">
@@ -18777,7 +18930,7 @@
       </c>
     </row>
     <row r="957" spans="1:2" ht="40.799999999999997">
-      <c r="A957" s="23" t="s">
+      <c r="A957" s="22" t="s">
         <v>1290</v>
       </c>
       <c r="B957" s="6" t="s">
@@ -18785,7 +18938,7 @@
       </c>
     </row>
     <row r="958" spans="1:2" ht="59.4">
-      <c r="A958" s="25" t="s">
+      <c r="A958" s="24" t="s">
         <v>1291</v>
       </c>
       <c r="B958" s="6" t="s">
@@ -18793,7 +18946,7 @@
       </c>
     </row>
     <row r="959" spans="1:2" ht="59.4">
-      <c r="A959" s="25" t="s">
+      <c r="A959" s="24" t="s">
         <v>1292</v>
       </c>
       <c r="B959" s="6" t="s">
@@ -18801,7 +18954,7 @@
       </c>
     </row>
     <row r="960" spans="1:2" ht="20.399999999999999">
-      <c r="A960" s="23" t="s">
+      <c r="A960" s="22" t="s">
         <v>1293</v>
       </c>
       <c r="B960" s="6" t="s">
@@ -18809,7 +18962,7 @@
       </c>
     </row>
     <row r="961" spans="1:2" ht="59.4">
-      <c r="A961" s="25" t="s">
+      <c r="A961" s="24" t="s">
         <v>1294</v>
       </c>
       <c r="B961" s="6" t="s">
@@ -18817,7 +18970,7 @@
       </c>
     </row>
     <row r="962" spans="1:2" ht="59.4">
-      <c r="A962" s="25" t="s">
+      <c r="A962" s="24" t="s">
         <v>1295</v>
       </c>
       <c r="B962" s="6" t="s">
@@ -18825,7 +18978,7 @@
       </c>
     </row>
     <row r="963" spans="1:2" ht="59.4">
-      <c r="A963" s="25" t="s">
+      <c r="A963" s="24" t="s">
         <v>1296</v>
       </c>
       <c r="B963" s="6" t="s">
@@ -18833,7 +18986,7 @@
       </c>
     </row>
     <row r="964" spans="1:2" ht="40.799999999999997">
-      <c r="A964" s="23" t="s">
+      <c r="A964" s="22" t="s">
         <v>1297</v>
       </c>
       <c r="B964" s="6" t="s">
@@ -18841,7 +18994,7 @@
       </c>
     </row>
     <row r="965" spans="1:2" ht="15">
-      <c r="A965" s="24" t="s">
+      <c r="A965" s="23" t="s">
         <v>1298</v>
       </c>
       <c r="B965" s="6" t="s">
@@ -18849,7 +19002,7 @@
       </c>
     </row>
     <row r="966" spans="1:2" ht="15">
-      <c r="A966" s="24" t="s">
+      <c r="A966" s="23" t="s">
         <v>1299</v>
       </c>
       <c r="B966" s="6" t="s">
@@ -18857,7 +19010,7 @@
       </c>
     </row>
     <row r="967" spans="1:2" ht="20.399999999999999">
-      <c r="A967" s="23" t="s">
+      <c r="A967" s="22" t="s">
         <v>1300</v>
       </c>
       <c r="B967" s="6" t="s">
@@ -18865,7 +19018,7 @@
       </c>
     </row>
     <row r="968" spans="1:2" ht="33.6">
-      <c r="A968" s="26" t="s">
+      <c r="A968" s="25" t="s">
         <v>1301</v>
       </c>
       <c r="B968" s="6" t="s">
@@ -18873,7 +19026,7 @@
       </c>
     </row>
     <row r="969" spans="1:2" ht="33.6">
-      <c r="A969" s="26" t="s">
+      <c r="A969" s="25" t="s">
         <v>1302</v>
       </c>
       <c r="B969" s="6" t="s">
@@ -18881,7 +19034,7 @@
       </c>
     </row>
     <row r="970" spans="1:2" ht="50.4">
-      <c r="A970" s="26" t="s">
+      <c r="A970" s="25" t="s">
         <v>1303</v>
       </c>
       <c r="B970" s="6" t="s">
@@ -18889,7 +19042,7 @@
       </c>
     </row>
     <row r="971" spans="1:2" ht="67.2">
-      <c r="A971" s="26" t="s">
+      <c r="A971" s="25" t="s">
         <v>1304</v>
       </c>
       <c r="B971" s="6" t="s">
@@ -18897,7 +19050,7 @@
       </c>
     </row>
     <row r="972" spans="1:2" ht="40.799999999999997">
-      <c r="A972" s="23" t="s">
+      <c r="A972" s="22" t="s">
         <v>1305</v>
       </c>
       <c r="B972" s="6" t="s">
@@ -18905,7 +19058,7 @@
       </c>
     </row>
     <row r="973" spans="1:2" ht="15">
-      <c r="A973" s="24" t="s">
+      <c r="A973" s="23" t="s">
         <v>1306</v>
       </c>
       <c r="B973" s="6" t="s">
@@ -18913,7 +19066,7 @@
       </c>
     </row>
     <row r="974" spans="1:2" ht="15">
-      <c r="A974" s="24" t="s">
+      <c r="A974" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="B974" s="6" t="s">
@@ -18921,7 +19074,7 @@
       </c>
     </row>
     <row r="975" spans="1:2" ht="15">
-      <c r="A975" s="24" t="s">
+      <c r="A975" s="23" t="s">
         <v>1308</v>
       </c>
       <c r="B975" s="6" t="s">
@@ -18929,7 +19082,7 @@
       </c>
     </row>
     <row r="976" spans="1:2" ht="15">
-      <c r="A976" s="24" t="s">
+      <c r="A976" s="23" t="s">
         <v>1309</v>
       </c>
       <c r="B976" s="6" t="s">
@@ -18937,7 +19090,7 @@
       </c>
     </row>
     <row r="977" spans="1:2" ht="40.799999999999997">
-      <c r="A977" s="23" t="s">
+      <c r="A977" s="22" t="s">
         <v>1310</v>
       </c>
       <c r="B977" s="6" t="s">
@@ -18945,7 +19098,7 @@
       </c>
     </row>
     <row r="978" spans="1:2" ht="15">
-      <c r="A978" s="24" t="s">
+      <c r="A978" s="23" t="s">
         <v>1311</v>
       </c>
       <c r="B978" s="6" t="s">
@@ -18953,7 +19106,7 @@
       </c>
     </row>
     <row r="979" spans="1:2" ht="15">
-      <c r="A979" s="24" t="s">
+      <c r="A979" s="23" t="s">
         <v>1312</v>
       </c>
       <c r="B979" s="6" t="s">
@@ -18961,7 +19114,7 @@
       </c>
     </row>
     <row r="980" spans="1:2" ht="40.799999999999997">
-      <c r="A980" s="23" t="s">
+      <c r="A980" s="22" t="s">
         <v>1313</v>
       </c>
       <c r="B980" s="6" t="s">
@@ -18969,7 +19122,7 @@
       </c>
     </row>
     <row r="981" spans="1:2" ht="15">
-      <c r="A981" s="24" t="s">
+      <c r="A981" s="23" t="s">
         <v>1313</v>
       </c>
       <c r="B981" s="6" t="s">
@@ -18977,7 +19130,7 @@
       </c>
     </row>
     <row r="982" spans="1:2" ht="15">
-      <c r="A982" s="24" t="s">
+      <c r="A982" s="23" t="s">
         <v>1314</v>
       </c>
       <c r="B982" s="6" t="s">
@@ -18985,7 +19138,7 @@
       </c>
     </row>
     <row r="983" spans="1:2" ht="15">
-      <c r="A983" s="24" t="s">
+      <c r="A983" s="23" t="s">
         <v>1315</v>
       </c>
       <c r="B983" s="6" t="s">
@@ -18993,7 +19146,7 @@
       </c>
     </row>
     <row r="984" spans="1:2" ht="15">
-      <c r="A984" s="24" t="s">
+      <c r="A984" s="23" t="s">
         <v>1316</v>
       </c>
       <c r="B984" s="6" t="s">
@@ -19001,7 +19154,7 @@
       </c>
     </row>
     <row r="985" spans="1:2" ht="40.799999999999997">
-      <c r="A985" s="23" t="s">
+      <c r="A985" s="22" t="s">
         <v>1317</v>
       </c>
       <c r="B985" s="6" t="s">
@@ -19009,7 +19162,7 @@
       </c>
     </row>
     <row r="986" spans="1:2" ht="59.4">
-      <c r="A986" s="25" t="s">
+      <c r="A986" s="24" t="s">
         <v>1318</v>
       </c>
       <c r="B986" s="6" t="s">
@@ -19017,7 +19170,7 @@
       </c>
     </row>
     <row r="987" spans="1:2" ht="99">
-      <c r="A987" s="25" t="s">
+      <c r="A987" s="24" t="s">
         <v>1319</v>
       </c>
       <c r="B987" s="6" t="s">
@@ -19025,7 +19178,7 @@
       </c>
     </row>
     <row r="988" spans="1:2" ht="40.799999999999997">
-      <c r="A988" s="23" t="s">
+      <c r="A988" s="22" t="s">
         <v>1320</v>
       </c>
       <c r="B988" s="6" t="s">
@@ -19033,7 +19186,7 @@
       </c>
     </row>
     <row r="989" spans="1:2" ht="99">
-      <c r="A989" s="25" t="s">
+      <c r="A989" s="24" t="s">
         <v>1321</v>
       </c>
       <c r="B989" s="6" t="s">
@@ -19041,7 +19194,7 @@
       </c>
     </row>
     <row r="990" spans="1:2" ht="79.2">
-      <c r="A990" s="25" t="s">
+      <c r="A990" s="24" t="s">
         <v>1322</v>
       </c>
       <c r="B990" s="6" t="s">
@@ -19049,7 +19202,7 @@
       </c>
     </row>
     <row r="991" spans="1:2" ht="39.6">
-      <c r="A991" s="25" t="s">
+      <c r="A991" s="24" t="s">
         <v>1323</v>
       </c>
       <c r="B991" s="6" t="s">
@@ -19057,7 +19210,7 @@
       </c>
     </row>
     <row r="992" spans="1:2" ht="79.2">
-      <c r="A992" s="25" t="s">
+      <c r="A992" s="24" t="s">
         <v>1324</v>
       </c>
       <c r="B992" s="6" t="s">
@@ -19065,7 +19218,7 @@
       </c>
     </row>
     <row r="993" spans="1:2" ht="40.799999999999997">
-      <c r="A993" s="23" t="s">
+      <c r="A993" s="22" t="s">
         <v>1325</v>
       </c>
       <c r="B993" s="6" t="s">
@@ -19073,7 +19226,7 @@
       </c>
     </row>
     <row r="994" spans="1:2" ht="59.4">
-      <c r="A994" s="25" t="s">
+      <c r="A994" s="24" t="s">
         <v>1326</v>
       </c>
       <c r="B994" s="6" t="s">
@@ -19081,7 +19234,7 @@
       </c>
     </row>
     <row r="995" spans="1:2" ht="59.4">
-      <c r="A995" s="25" t="s">
+      <c r="A995" s="24" t="s">
         <v>1327</v>
       </c>
       <c r="B995" s="6" t="s">
@@ -19089,7 +19242,7 @@
       </c>
     </row>
     <row r="996" spans="1:2" ht="79.2">
-      <c r="A996" s="25" t="s">
+      <c r="A996" s="24" t="s">
         <v>1328</v>
       </c>
       <c r="B996" s="6" t="s">
@@ -19105,7 +19258,7 @@
       </c>
     </row>
     <row r="998" spans="1:2" ht="99">
-      <c r="A998" s="25" t="s">
+      <c r="A998" s="24" t="s">
         <v>1330</v>
       </c>
       <c r="B998" s="6" t="s">
@@ -19113,7 +19266,7 @@
       </c>
     </row>
     <row r="999" spans="1:2" ht="59.4">
-      <c r="A999" s="25" t="s">
+      <c r="A999" s="24" t="s">
         <v>1331</v>
       </c>
       <c r="B999" s="6" t="s">
@@ -19121,7 +19274,7 @@
       </c>
     </row>
     <row r="1000" spans="1:2" ht="40.799999999999997">
-      <c r="A1000" s="23" t="s">
+      <c r="A1000" s="22" t="s">
         <v>1332</v>
       </c>
       <c r="B1000" s="6" t="s">
@@ -19129,7 +19282,7 @@
       </c>
     </row>
     <row r="1001" spans="1:2" ht="59.4">
-      <c r="A1001" s="25" t="s">
+      <c r="A1001" s="24" t="s">
         <v>1333</v>
       </c>
       <c r="B1001" s="6" t="s">
@@ -19137,7 +19290,7 @@
       </c>
     </row>
     <row r="1002" spans="1:2" ht="39.6">
-      <c r="A1002" s="25" t="s">
+      <c r="A1002" s="24" t="s">
         <v>1334</v>
       </c>
       <c r="B1002" s="6" t="s">
@@ -19145,7 +19298,7 @@
       </c>
     </row>
     <row r="1003" spans="1:2" ht="59.4">
-      <c r="A1003" s="25" t="s">
+      <c r="A1003" s="24" t="s">
         <v>1335</v>
       </c>
       <c r="B1003" s="6" t="s">
@@ -19153,7 +19306,7 @@
       </c>
     </row>
     <row r="1004" spans="1:2" ht="39.6">
-      <c r="A1004" s="25" t="s">
+      <c r="A1004" s="24" t="s">
         <v>1336</v>
       </c>
       <c r="B1004" s="6" t="s">
@@ -19161,7 +19314,7 @@
       </c>
     </row>
     <row r="1005" spans="1:2" ht="20.399999999999999">
-      <c r="A1005" s="23" t="s">
+      <c r="A1005" s="22" t="s">
         <v>1337</v>
       </c>
       <c r="B1005" s="6" t="s">
@@ -19169,7 +19322,7 @@
       </c>
     </row>
     <row r="1006" spans="1:2" ht="59.4">
-      <c r="A1006" s="25" t="s">
+      <c r="A1006" s="24" t="s">
         <v>1338</v>
       </c>
       <c r="B1006" s="6" t="s">
@@ -19177,7 +19330,7 @@
       </c>
     </row>
     <row r="1007" spans="1:2" ht="59.4">
-      <c r="A1007" s="25" t="s">
+      <c r="A1007" s="24" t="s">
         <v>1339</v>
       </c>
       <c r="B1007" s="6" t="s">
@@ -19185,7 +19338,7 @@
       </c>
     </row>
     <row r="1008" spans="1:2" ht="39.6">
-      <c r="A1008" s="25" t="s">
+      <c r="A1008" s="24" t="s">
         <v>1340</v>
       </c>
       <c r="B1008" s="6" t="s">
@@ -19193,7 +19346,7 @@
       </c>
     </row>
     <row r="1009" spans="1:2" ht="40.799999999999997">
-      <c r="A1009" s="23" t="s">
+      <c r="A1009" s="22" t="s">
         <v>1341</v>
       </c>
       <c r="B1009" s="6" t="s">
@@ -19201,7 +19354,7 @@
       </c>
     </row>
     <row r="1010" spans="1:2" ht="59.4">
-      <c r="A1010" s="25" t="s">
+      <c r="A1010" s="24" t="s">
         <v>1342</v>
       </c>
       <c r="B1010" s="6" t="s">
@@ -19215,7 +19368,7 @@
       </c>
     </row>
     <row r="1012" spans="1:2" ht="79.2">
-      <c r="A1012" s="25" t="s">
+      <c r="A1012" s="24" t="s">
         <v>1343</v>
       </c>
       <c r="B1012" s="6" t="s">
@@ -19223,7 +19376,7 @@
       </c>
     </row>
     <row r="1013" spans="1:2" ht="59.4">
-      <c r="A1013" s="25" t="s">
+      <c r="A1013" s="24" t="s">
         <v>1344</v>
       </c>
       <c r="B1013" s="6" t="s">
@@ -19231,7 +19384,7 @@
       </c>
     </row>
     <row r="1014" spans="1:2" ht="39.6">
-      <c r="A1014" s="25" t="s">
+      <c r="A1014" s="24" t="s">
         <v>1345</v>
       </c>
       <c r="B1014" s="6" t="s">
@@ -19239,7 +19392,7 @@
       </c>
     </row>
     <row r="1015" spans="1:2" ht="59.4">
-      <c r="A1015" s="25" t="s">
+      <c r="A1015" s="24" t="s">
         <v>1346</v>
       </c>
       <c r="B1015" s="6" t="s">
@@ -19247,7 +19400,7 @@
       </c>
     </row>
     <row r="1016" spans="1:2" ht="19.8">
-      <c r="A1016" s="25" t="s">
+      <c r="A1016" s="24" t="s">
         <v>1347</v>
       </c>
       <c r="B1016" s="6" t="s">
@@ -19255,7 +19408,7 @@
       </c>
     </row>
     <row r="1017" spans="1:2" ht="39.6">
-      <c r="A1017" s="25" t="s">
+      <c r="A1017" s="24" t="s">
         <v>1348</v>
       </c>
       <c r="B1017" s="6" t="s">
@@ -19263,7 +19416,7 @@
       </c>
     </row>
     <row r="1018" spans="1:2" ht="20.399999999999999">
-      <c r="A1018" s="23" t="s">
+      <c r="A1018" s="22" t="s">
         <v>1349</v>
       </c>
       <c r="B1018" s="6" t="s">
@@ -19271,7 +19424,7 @@
       </c>
     </row>
     <row r="1019" spans="1:2" ht="39.6">
-      <c r="A1019" s="25" t="s">
+      <c r="A1019" s="24" t="s">
         <v>1350</v>
       </c>
       <c r="B1019" s="6" t="s">
@@ -19279,7 +19432,7 @@
       </c>
     </row>
     <row r="1020" spans="1:2" ht="59.4">
-      <c r="A1020" s="25" t="s">
+      <c r="A1020" s="24" t="s">
         <v>1353</v>
       </c>
       <c r="B1020" s="6" t="s">
@@ -19287,7 +19440,7 @@
       </c>
     </row>
     <row r="1021" spans="1:2" ht="39.6">
-      <c r="A1021" s="25" t="s">
+      <c r="A1021" s="24" t="s">
         <v>1351</v>
       </c>
       <c r="B1021" s="6" t="s">
@@ -19295,7 +19448,7 @@
       </c>
     </row>
     <row r="1022" spans="1:2" ht="19.8">
-      <c r="A1022" s="25" t="s">
+      <c r="A1022" s="24" t="s">
         <v>1352</v>
       </c>
       <c r="B1022" s="6" t="s">
@@ -19303,7 +19456,7 @@
       </c>
     </row>
     <row r="1023" spans="1:2" ht="40.799999999999997">
-      <c r="A1023" s="23" t="s">
+      <c r="A1023" s="22" t="s">
         <v>1354</v>
       </c>
       <c r="B1023" s="6" t="s">
@@ -19311,7 +19464,7 @@
       </c>
     </row>
     <row r="1024" spans="1:2" ht="59.4">
-      <c r="A1024" s="25" t="s">
+      <c r="A1024" s="24" t="s">
         <v>1355</v>
       </c>
       <c r="B1024" s="6" t="s">
@@ -19319,7 +19472,7 @@
       </c>
     </row>
     <row r="1025" spans="1:2" ht="59.4">
-      <c r="A1025" s="25" t="s">
+      <c r="A1025" s="24" t="s">
         <v>1356</v>
       </c>
       <c r="B1025" s="6" t="s">
@@ -19327,7 +19480,7 @@
       </c>
     </row>
     <row r="1026" spans="1:2" ht="59.4">
-      <c r="A1026" s="25" t="s">
+      <c r="A1026" s="24" t="s">
         <v>1357</v>
       </c>
       <c r="B1026" s="6" t="s">
@@ -19335,7 +19488,7 @@
       </c>
     </row>
     <row r="1027" spans="1:2" ht="79.2">
-      <c r="A1027" s="25" t="s">
+      <c r="A1027" s="24" t="s">
         <v>1358</v>
       </c>
       <c r="B1027" s="6" t="s">
@@ -19343,7 +19496,7 @@
       </c>
     </row>
     <row r="1028" spans="1:2" ht="20.399999999999999">
-      <c r="A1028" s="23" t="s">
+      <c r="A1028" s="22" t="s">
         <v>1359</v>
       </c>
       <c r="B1028" s="6" t="s">
@@ -19351,7 +19504,7 @@
       </c>
     </row>
     <row r="1029" spans="1:2" ht="59.4">
-      <c r="A1029" s="25" t="s">
+      <c r="A1029" s="24" t="s">
         <v>1360</v>
       </c>
       <c r="B1029" s="6" t="s">
@@ -19359,7 +19512,7 @@
       </c>
     </row>
     <row r="1030" spans="1:2" ht="39.6">
-      <c r="A1030" s="25" t="s">
+      <c r="A1030" s="24" t="s">
         <v>1361</v>
       </c>
       <c r="B1030" s="6" t="s">
@@ -19367,7 +19520,7 @@
       </c>
     </row>
     <row r="1031" spans="1:2" ht="20.399999999999999">
-      <c r="A1031" s="23" t="s">
+      <c r="A1031" s="22" t="s">
         <v>1362</v>
       </c>
       <c r="B1031" s="6" t="s">
@@ -19375,7 +19528,7 @@
       </c>
     </row>
     <row r="1032" spans="1:2" ht="59.4">
-      <c r="A1032" s="25" t="s">
+      <c r="A1032" s="24" t="s">
         <v>1363</v>
       </c>
       <c r="B1032" s="6" t="s">
@@ -19383,7 +19536,7 @@
       </c>
     </row>
     <row r="1033" spans="1:2" ht="39.6">
-      <c r="A1033" s="25" t="s">
+      <c r="A1033" s="24" t="s">
         <v>1365</v>
       </c>
       <c r="B1033" s="6" t="s">
@@ -19399,7 +19552,7 @@
       </c>
     </row>
     <row r="1035" spans="1:2" ht="39.6">
-      <c r="A1035" s="25" t="s">
+      <c r="A1035" s="24" t="s">
         <v>1364</v>
       </c>
       <c r="B1035" s="6" t="s">
@@ -19407,7 +19560,7 @@
       </c>
     </row>
     <row r="1036" spans="1:2" ht="20.399999999999999">
-      <c r="A1036" s="23" t="s">
+      <c r="A1036" s="22" t="s">
         <v>1367</v>
       </c>
       <c r="B1036" s="6" t="s">
@@ -19415,7 +19568,7 @@
       </c>
     </row>
     <row r="1037" spans="1:2" ht="39.6">
-      <c r="A1037" s="25" t="s">
+      <c r="A1037" s="24" t="s">
         <v>1368</v>
       </c>
       <c r="B1037" s="6" t="s">
@@ -19429,7 +19582,7 @@
       </c>
     </row>
     <row r="1039" spans="1:2" ht="39.6">
-      <c r="A1039" s="25" t="s">
+      <c r="A1039" s="24" t="s">
         <v>1369</v>
       </c>
       <c r="B1039" s="6" t="s">
@@ -19437,7 +19590,7 @@
       </c>
     </row>
     <row r="1040" spans="1:2" ht="59.4">
-      <c r="A1040" s="25" t="s">
+      <c r="A1040" s="24" t="s">
         <v>1370</v>
       </c>
       <c r="B1040" s="6" t="s">
@@ -19445,7 +19598,7 @@
       </c>
     </row>
     <row r="1041" spans="1:2" ht="19.8">
-      <c r="A1041" s="25" t="s">
+      <c r="A1041" s="24" t="s">
         <v>1371</v>
       </c>
       <c r="B1041" s="6" t="s">
@@ -19453,7 +19606,7 @@
       </c>
     </row>
     <row r="1042" spans="1:2" ht="19.8">
-      <c r="A1042" s="25" t="s">
+      <c r="A1042" s="24" t="s">
         <v>1372</v>
       </c>
       <c r="B1042" s="6" t="s">
@@ -19461,7 +19614,7 @@
       </c>
     </row>
     <row r="1043" spans="1:2" ht="20.399999999999999">
-      <c r="A1043" s="23" t="s">
+      <c r="A1043" s="22" t="s">
         <v>1373</v>
       </c>
       <c r="B1043" s="6" t="s">
@@ -19469,7 +19622,7 @@
       </c>
     </row>
     <row r="1044" spans="1:2" ht="39.6">
-      <c r="A1044" s="25" t="s">
+      <c r="A1044" s="24" t="s">
         <v>1374</v>
       </c>
       <c r="B1044" s="6" t="s">
@@ -19477,7 +19630,7 @@
       </c>
     </row>
     <row r="1045" spans="1:2" ht="79.2">
-      <c r="A1045" s="25" t="s">
+      <c r="A1045" s="24" t="s">
         <v>1375</v>
       </c>
       <c r="B1045" s="6" t="s">
@@ -19485,7 +19638,7 @@
       </c>
     </row>
     <row r="1046" spans="1:2" ht="79.2">
-      <c r="A1046" s="25" t="s">
+      <c r="A1046" s="24" t="s">
         <v>1376</v>
       </c>
       <c r="B1046" s="6" t="s">
@@ -19493,7 +19646,7 @@
       </c>
     </row>
     <row r="1047" spans="1:2" ht="79.2">
-      <c r="A1047" s="25" t="s">
+      <c r="A1047" s="24" t="s">
         <v>1377</v>
       </c>
       <c r="B1047" s="6" t="s">
@@ -19501,7 +19654,7 @@
       </c>
     </row>
     <row r="1048" spans="1:2" ht="39.6">
-      <c r="A1048" s="25" t="s">
+      <c r="A1048" s="24" t="s">
         <v>1378</v>
       </c>
       <c r="B1048" s="6" t="s">
@@ -19517,7 +19670,7 @@
       </c>
     </row>
     <row r="1050" spans="1:2" ht="59.4">
-      <c r="A1050" s="25" t="s">
+      <c r="A1050" s="24" t="s">
         <v>1380</v>
       </c>
       <c r="B1050" s="6" t="s">
@@ -19525,7 +19678,7 @@
       </c>
     </row>
     <row r="1051" spans="1:2" ht="118.8">
-      <c r="A1051" s="25" t="s">
+      <c r="A1051" s="24" t="s">
         <v>1381</v>
       </c>
       <c r="B1051" s="6" t="s">
@@ -19533,7 +19686,7 @@
       </c>
     </row>
     <row r="1052" spans="1:2" ht="79.2">
-      <c r="A1052" s="25" t="s">
+      <c r="A1052" s="24" t="s">
         <v>1382</v>
       </c>
       <c r="B1052" s="6" t="s">
@@ -19541,7 +19694,7 @@
       </c>
     </row>
     <row r="1053" spans="1:2" ht="59.4">
-      <c r="A1053" s="25" t="s">
+      <c r="A1053" s="24" t="s">
         <v>1383</v>
       </c>
       <c r="B1053" s="6" t="s">
@@ -19549,7 +19702,7 @@
       </c>
     </row>
     <row r="1054" spans="1:2" ht="59.4">
-      <c r="A1054" s="25" t="s">
+      <c r="A1054" s="24" t="s">
         <v>1384</v>
       </c>
       <c r="B1054" s="6" t="s">
@@ -19557,7 +19710,7 @@
       </c>
     </row>
     <row r="1055" spans="1:2" ht="79.2">
-      <c r="A1055" s="25" t="s">
+      <c r="A1055" s="24" t="s">
         <v>1385</v>
       </c>
       <c r="B1055" s="6" t="s">
@@ -19565,7 +19718,7 @@
       </c>
     </row>
     <row r="1056" spans="1:2" ht="79.2">
-      <c r="A1056" s="25" t="s">
+      <c r="A1056" s="24" t="s">
         <v>1386</v>
       </c>
       <c r="B1056" s="6" t="s">
@@ -19573,7 +19726,7 @@
       </c>
     </row>
     <row r="1057" spans="1:2" ht="20.399999999999999">
-      <c r="A1057" s="23" t="s">
+      <c r="A1057" s="22" t="s">
         <v>1387</v>
       </c>
       <c r="B1057" s="6" t="s">
@@ -19581,7 +19734,7 @@
       </c>
     </row>
     <row r="1058" spans="1:2" ht="59.4">
-      <c r="A1058" s="25" t="s">
+      <c r="A1058" s="24" t="s">
         <v>1388</v>
       </c>
       <c r="B1058" s="6" t="s">
@@ -19589,7 +19742,7 @@
       </c>
     </row>
     <row r="1059" spans="1:2" ht="99">
-      <c r="A1059" s="25" t="s">
+      <c r="A1059" s="24" t="s">
         <v>1389</v>
       </c>
       <c r="B1059" s="6" t="s">
@@ -19597,7 +19750,7 @@
       </c>
     </row>
     <row r="1060" spans="1:2" ht="79.2">
-      <c r="A1060" s="25" t="s">
+      <c r="A1060" s="24" t="s">
         <v>1390</v>
       </c>
       <c r="B1060" s="6" t="s">
@@ -19605,7 +19758,7 @@
       </c>
     </row>
     <row r="1061" spans="1:2" ht="59.4">
-      <c r="A1061" s="25" t="s">
+      <c r="A1061" s="24" t="s">
         <v>1391</v>
       </c>
       <c r="B1061" s="6" t="s">
@@ -19621,7 +19774,7 @@
       </c>
     </row>
     <row r="1063" spans="1:2" ht="39.6">
-      <c r="A1063" s="25" t="s">
+      <c r="A1063" s="24" t="s">
         <v>1393</v>
       </c>
       <c r="B1063" s="6" t="s">
@@ -19629,7 +19782,7 @@
       </c>
     </row>
     <row r="1064" spans="1:2" ht="59.4">
-      <c r="A1064" s="25" t="s">
+      <c r="A1064" s="24" t="s">
         <v>1394</v>
       </c>
       <c r="B1064" s="6" t="s">
@@ -19637,7 +19790,7 @@
       </c>
     </row>
     <row r="1065" spans="1:2" ht="19.8">
-      <c r="A1065" s="25" t="s">
+      <c r="A1065" s="24" t="s">
         <v>1395</v>
       </c>
       <c r="B1065" s="6" t="s">
@@ -19645,7 +19798,7 @@
       </c>
     </row>
     <row r="1066" spans="1:2" ht="20.399999999999999">
-      <c r="A1066" s="23" t="s">
+      <c r="A1066" s="22" t="s">
         <v>1396</v>
       </c>
       <c r="B1066" s="6" t="s">
@@ -19653,7 +19806,7 @@
       </c>
     </row>
     <row r="1067" spans="1:2" ht="39.6">
-      <c r="A1067" s="25" t="s">
+      <c r="A1067" s="24" t="s">
         <v>1397</v>
       </c>
       <c r="B1067" s="6" t="s">
@@ -19661,7 +19814,7 @@
       </c>
     </row>
     <row r="1068" spans="1:2" ht="79.2">
-      <c r="A1068" s="25" t="s">
+      <c r="A1068" s="24" t="s">
         <v>1398</v>
       </c>
       <c r="B1068" s="6" t="s">
@@ -19669,7 +19822,7 @@
       </c>
     </row>
     <row r="1069" spans="1:2" ht="79.2">
-      <c r="A1069" s="25" t="s">
+      <c r="A1069" s="24" t="s">
         <v>1399</v>
       </c>
       <c r="B1069" s="6" t="s">
@@ -19677,10 +19830,322 @@
       </c>
     </row>
     <row r="1070" spans="1:2" ht="118.8">
-      <c r="A1070" s="25" t="s">
+      <c r="A1070" s="24" t="s">
         <v>1400</v>
       </c>
       <c r="B1070" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:2" ht="40.799999999999997">
+      <c r="A1071" s="27" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B1071" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:2" ht="59.4">
+      <c r="A1072" s="24" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B1072" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:2" ht="39.6">
+      <c r="A1073" s="24" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B1073" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:2" ht="19.8">
+      <c r="A1074" s="24" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B1074" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:2" ht="28.8">
+      <c r="A1075" s="5" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1075" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:2" ht="39.6">
+      <c r="A1076" s="24" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1076" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:2" ht="59.4">
+      <c r="A1077" s="24" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1077" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:2" ht="59.4">
+      <c r="A1078" s="24" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B1078" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:2" ht="28.8">
+      <c r="A1079" s="5" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B1079" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:2" ht="79.2">
+      <c r="A1080" s="24" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B1080" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:2" ht="79.2">
+      <c r="A1081" s="24" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B1081" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:2" ht="39.6">
+      <c r="A1082" s="24" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B1082" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:2" ht="20.399999999999999">
+      <c r="A1083" s="27" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B1083" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:2" ht="39.6">
+      <c r="A1084" s="24" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B1084" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:2" ht="59.4">
+      <c r="A1085" s="24" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B1085" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:2" ht="59.4">
+      <c r="A1086" s="24" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B1086" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:2">
+      <c r="A1087" s="5" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B1087" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:2" ht="79.2">
+      <c r="A1088" s="24" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B1088" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:2" ht="99">
+      <c r="A1089" s="24" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B1089" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:2" ht="59.4">
+      <c r="A1090" s="24" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B1090" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:2" ht="40.799999999999997">
+      <c r="A1091" s="27" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B1091" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:2" ht="39.6">
+      <c r="A1092" s="24" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B1092" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:2" ht="39.6">
+      <c r="A1093" s="24" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B1093" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:2" ht="19.8">
+      <c r="A1094" s="24" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B1094" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:2" ht="79.2">
+      <c r="A1095" s="24" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B1095" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:2" ht="40.799999999999997">
+      <c r="A1096" s="27" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B1096" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:2" ht="59.4">
+      <c r="A1097" s="24" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B1097" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:2" ht="79.2">
+      <c r="A1098" s="24" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B1098" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:2" ht="59.4">
+      <c r="A1099" s="24" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B1099" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:2">
+      <c r="A1100" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B1100" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:2" ht="79.2">
+      <c r="A1101" s="24" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B1101" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:2">
+      <c r="A1102" s="5" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B1102" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:2" ht="79.2">
+      <c r="A1103" s="24" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B1103" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:2" ht="39.6">
+      <c r="A1104" s="24" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B1104" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:2" ht="39.6">
+      <c r="A1105" s="24" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B1105" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:2" ht="61.2">
+      <c r="A1106" s="27" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B1106" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:2" ht="39.6">
+      <c r="A1107" s="24" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B1107" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:2" ht="59.4">
+      <c r="A1108" s="24" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B1108" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:2" ht="59.4">
+      <c r="A1109" s="24" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B1109" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -19976,8 +20441,8 @@
       <c r="M11">
         <v>29</v>
       </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
added 414 English from Lolwe Tv
</commit_message>
<xml_diff>
--- a/LUO.xlsx
+++ b/LUO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ogayo\OneDrive\Desktop\Masakhane\Luo-News-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50E211F-FEC8-4B42-A629-66BFEC82FCBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A914A69-DC98-459C-8019-3A951848B717}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined_text" sheetId="9" r:id="rId1"/>
@@ -6459,13 +6459,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -20966,8 +20966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1414"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1157" workbookViewId="0">
-      <selection activeCell="B1411" sqref="B1411:B1414"/>
+    <sheetView topLeftCell="A1157" workbookViewId="0">
+      <selection activeCell="B1157" sqref="B1157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -31227,7 +31227,7 @@
       </c>
     </row>
     <row r="1283" spans="1:2" ht="40.799999999999997">
-      <c r="A1283" s="48" t="s">
+      <c r="A1283" s="47" t="s">
         <v>1786</v>
       </c>
       <c r="B1283" s="21" t="s">
@@ -31251,7 +31251,7 @@
       </c>
     </row>
     <row r="1286" spans="1:2" ht="20.399999999999999">
-      <c r="A1286" s="48" t="s">
+      <c r="A1286" s="47" t="s">
         <v>1789</v>
       </c>
       <c r="B1286" t="s">
@@ -31299,7 +31299,7 @@
       </c>
     </row>
     <row r="1292" spans="1:2" ht="40.799999999999997">
-      <c r="A1292" s="48" t="s">
+      <c r="A1292" s="47" t="s">
         <v>1795</v>
       </c>
       <c r="B1292" s="9" t="s">
@@ -31339,7 +31339,7 @@
       </c>
     </row>
     <row r="1297" spans="1:2" ht="20.399999999999999">
-      <c r="A1297" s="48" t="s">
+      <c r="A1297" s="47" t="s">
         <v>1800</v>
       </c>
       <c r="B1297" t="s">
@@ -31379,7 +31379,7 @@
       </c>
     </row>
     <row r="1302" spans="1:2" ht="20.399999999999999">
-      <c r="A1302" s="48" t="s">
+      <c r="A1302" s="47" t="s">
         <v>1805</v>
       </c>
       <c r="B1302" t="s">
@@ -31387,7 +31387,7 @@
       </c>
     </row>
     <row r="1303" spans="1:2" ht="15">
-      <c r="A1303" s="49" t="s">
+      <c r="A1303" s="48" t="s">
         <v>1806</v>
       </c>
       <c r="B1303" s="9" t="s">
@@ -31395,7 +31395,7 @@
       </c>
     </row>
     <row r="1304" spans="1:2" ht="15">
-      <c r="A1304" s="49" t="s">
+      <c r="A1304" s="48" t="s">
         <v>1807</v>
       </c>
       <c r="B1304" s="9" t="s">
@@ -31403,7 +31403,7 @@
       </c>
     </row>
     <row r="1305" spans="1:2" ht="15">
-      <c r="A1305" s="49" t="s">
+      <c r="A1305" s="48" t="s">
         <v>1808</v>
       </c>
       <c r="B1305" s="9" t="s">
@@ -31411,7 +31411,7 @@
       </c>
     </row>
     <row r="1306" spans="1:2" ht="15">
-      <c r="A1306" s="49" t="s">
+      <c r="A1306" s="48" t="s">
         <v>1809</v>
       </c>
       <c r="B1306" s="9" t="s">
@@ -31419,7 +31419,7 @@
       </c>
     </row>
     <row r="1307" spans="1:2" ht="15">
-      <c r="A1307" s="49" t="s">
+      <c r="A1307" s="48" t="s">
         <v>1810</v>
       </c>
       <c r="B1307" s="9" t="s">
@@ -31427,7 +31427,7 @@
       </c>
     </row>
     <row r="1308" spans="1:2" ht="40.799999999999997">
-      <c r="A1308" s="48" t="s">
+      <c r="A1308" s="47" t="s">
         <v>1811</v>
       </c>
       <c r="B1308" s="4" t="s">
@@ -31435,7 +31435,7 @@
       </c>
     </row>
     <row r="1309" spans="1:2" ht="15">
-      <c r="A1309" s="49" t="s">
+      <c r="A1309" s="48" t="s">
         <v>1812</v>
       </c>
       <c r="B1309" s="15" t="s">
@@ -31443,7 +31443,7 @@
       </c>
     </row>
     <row r="1310" spans="1:2" ht="15">
-      <c r="A1310" s="49" t="s">
+      <c r="A1310" s="48" t="s">
         <v>1813</v>
       </c>
       <c r="B1310" s="15" t="s">
@@ -31451,7 +31451,7 @@
       </c>
     </row>
     <row r="1311" spans="1:2" ht="15">
-      <c r="A1311" s="49" t="s">
+      <c r="A1311" s="48" t="s">
         <v>1814</v>
       </c>
       <c r="B1311" s="15" t="s">
@@ -31459,7 +31459,7 @@
       </c>
     </row>
     <row r="1312" spans="1:2" ht="40.799999999999997">
-      <c r="A1312" s="48" t="s">
+      <c r="A1312" s="47" t="s">
         <v>1815</v>
       </c>
       <c r="B1312" s="4" t="s">
@@ -31467,7 +31467,7 @@
       </c>
     </row>
     <row r="1313" spans="1:2" ht="15">
-      <c r="A1313" s="49" t="s">
+      <c r="A1313" s="48" t="s">
         <v>1815</v>
       </c>
       <c r="B1313" s="15" t="s">
@@ -31475,7 +31475,7 @@
       </c>
     </row>
     <row r="1314" spans="1:2" ht="15">
-      <c r="A1314" s="49" t="s">
+      <c r="A1314" s="48" t="s">
         <v>1816</v>
       </c>
       <c r="B1314" s="15" t="s">
@@ -31483,7 +31483,7 @@
       </c>
     </row>
     <row r="1315" spans="1:2" ht="15">
-      <c r="A1315" s="49" t="s">
+      <c r="A1315" s="48" t="s">
         <v>1817</v>
       </c>
       <c r="B1315" s="15" t="s">
@@ -31491,7 +31491,7 @@
       </c>
     </row>
     <row r="1316" spans="1:2" ht="15">
-      <c r="A1316" s="49" t="s">
+      <c r="A1316" s="48" t="s">
         <v>1818</v>
       </c>
       <c r="B1316" s="15" t="s">
@@ -31499,7 +31499,7 @@
       </c>
     </row>
     <row r="1317" spans="1:2" ht="40.799999999999997">
-      <c r="A1317" s="48" t="s">
+      <c r="A1317" s="47" t="s">
         <v>1819</v>
       </c>
       <c r="B1317" s="15" t="s">
@@ -31507,7 +31507,7 @@
       </c>
     </row>
     <row r="1318" spans="1:2" ht="15">
-      <c r="A1318" s="49" t="s">
+      <c r="A1318" s="48" t="s">
         <v>1820</v>
       </c>
       <c r="B1318" s="15" t="s">
@@ -31515,7 +31515,7 @@
       </c>
     </row>
     <row r="1319" spans="1:2" ht="15">
-      <c r="A1319" s="49" t="s">
+      <c r="A1319" s="48" t="s">
         <v>1821</v>
       </c>
       <c r="B1319" s="15" t="s">
@@ -31523,7 +31523,7 @@
       </c>
     </row>
     <row r="1320" spans="1:2" ht="15">
-      <c r="A1320" s="49" t="s">
+      <c r="A1320" s="48" t="s">
         <v>1822</v>
       </c>
       <c r="B1320" s="15" t="s">
@@ -31531,7 +31531,7 @@
       </c>
     </row>
     <row r="1321" spans="1:2" ht="15">
-      <c r="A1321" s="49" t="s">
+      <c r="A1321" s="48" t="s">
         <v>1823</v>
       </c>
       <c r="B1321" s="15" t="s">
@@ -31539,7 +31539,7 @@
       </c>
     </row>
     <row r="1322" spans="1:2" ht="20.399999999999999">
-      <c r="A1322" s="48" t="s">
+      <c r="A1322" s="47" t="s">
         <v>1824</v>
       </c>
       <c r="B1322" s="4" t="s">
@@ -31571,7 +31571,7 @@
       </c>
     </row>
     <row r="1326" spans="1:2" ht="40.799999999999997">
-      <c r="A1326" s="48" t="s">
+      <c r="A1326" s="47" t="s">
         <v>1828</v>
       </c>
       <c r="B1326" s="15" t="s">
@@ -31627,7 +31627,7 @@
       </c>
     </row>
     <row r="1333" spans="1:2" ht="20.399999999999999">
-      <c r="A1333" s="48" t="s">
+      <c r="A1333" s="47" t="s">
         <v>1835</v>
       </c>
       <c r="B1333" s="4" t="s">
@@ -31675,7 +31675,7 @@
       </c>
     </row>
     <row r="1339" spans="1:2" ht="20.399999999999999">
-      <c r="A1339" s="48" t="s">
+      <c r="A1339" s="47" t="s">
         <v>1841</v>
       </c>
       <c r="B1339" s="15" t="s">
@@ -31723,7 +31723,7 @@
       </c>
     </row>
     <row r="1345" spans="1:2" ht="40.799999999999997">
-      <c r="A1345" s="48" t="s">
+      <c r="A1345" s="47" t="s">
         <v>1847</v>
       </c>
       <c r="B1345" s="4" t="s">
@@ -31731,7 +31731,7 @@
       </c>
     </row>
     <row r="1346" spans="1:2" ht="15">
-      <c r="A1346" s="49" t="s">
+      <c r="A1346" s="48" t="s">
         <v>1848</v>
       </c>
       <c r="B1346" s="15" t="s">
@@ -31739,7 +31739,7 @@
       </c>
     </row>
     <row r="1347" spans="1:2" ht="15">
-      <c r="A1347" s="49" t="s">
+      <c r="A1347" s="48" t="s">
         <v>1850</v>
       </c>
       <c r="B1347" s="15" t="s">
@@ -31747,7 +31747,7 @@
       </c>
     </row>
     <row r="1348" spans="1:2" ht="15">
-      <c r="A1348" s="49" t="s">
+      <c r="A1348" s="48" t="s">
         <v>1851</v>
       </c>
       <c r="B1348" s="15" t="s">
@@ -31755,7 +31755,7 @@
       </c>
     </row>
     <row r="1349" spans="1:2" ht="15">
-      <c r="A1349" s="49" t="s">
+      <c r="A1349" s="48" t="s">
         <v>1849</v>
       </c>
       <c r="B1349" s="15" t="s">
@@ -31763,7 +31763,7 @@
       </c>
     </row>
     <row r="1350" spans="1:2" ht="40.799999999999997">
-      <c r="A1350" s="48" t="s">
+      <c r="A1350" s="47" t="s">
         <v>1852</v>
       </c>
       <c r="B1350" s="4" t="s">
@@ -31771,7 +31771,7 @@
       </c>
     </row>
     <row r="1351" spans="1:2" ht="15">
-      <c r="A1351" s="49" t="s">
+      <c r="A1351" s="48" t="s">
         <v>1853</v>
       </c>
       <c r="B1351" s="15" t="s">
@@ -31779,7 +31779,7 @@
       </c>
     </row>
     <row r="1352" spans="1:2" ht="15">
-      <c r="A1352" s="49" t="s">
+      <c r="A1352" s="48" t="s">
         <v>1854</v>
       </c>
       <c r="B1352" s="15" t="s">
@@ -31787,7 +31787,7 @@
       </c>
     </row>
     <row r="1353" spans="1:2" ht="15">
-      <c r="A1353" s="49" t="s">
+      <c r="A1353" s="48" t="s">
         <v>1855</v>
       </c>
       <c r="B1353" s="15" t="s">
@@ -31795,7 +31795,7 @@
       </c>
     </row>
     <row r="1354" spans="1:2" ht="20.399999999999999">
-      <c r="A1354" s="48" t="s">
+      <c r="A1354" s="47" t="s">
         <v>1856</v>
       </c>
       <c r="B1354" s="4" t="s">
@@ -31867,7 +31867,7 @@
       </c>
     </row>
     <row r="1363" spans="1:2" ht="40.799999999999997">
-      <c r="A1363" s="48" t="s">
+      <c r="A1363" s="47" t="s">
         <v>1865</v>
       </c>
       <c r="B1363" s="4" t="s">
@@ -31899,7 +31899,7 @@
       </c>
     </row>
     <row r="1367" spans="1:2" ht="40.799999999999997">
-      <c r="A1367" s="48" t="s">
+      <c r="A1367" s="47" t="s">
         <v>1869</v>
       </c>
       <c r="B1367" s="4" t="s">
@@ -31955,7 +31955,7 @@
       </c>
     </row>
     <row r="1374" spans="1:2" ht="40.799999999999997">
-      <c r="A1374" s="48" t="s">
+      <c r="A1374" s="47" t="s">
         <v>1876</v>
       </c>
       <c r="B1374" s="4" t="s">
@@ -31963,7 +31963,7 @@
       </c>
     </row>
     <row r="1375" spans="1:2" ht="15">
-      <c r="A1375" s="49" t="s">
+      <c r="A1375" s="48" t="s">
         <v>1877</v>
       </c>
       <c r="B1375" s="15" t="s">
@@ -31971,7 +31971,7 @@
       </c>
     </row>
     <row r="1376" spans="1:2" ht="15">
-      <c r="A1376" s="49" t="s">
+      <c r="A1376" s="48" t="s">
         <v>1878</v>
       </c>
       <c r="B1376" s="15" t="s">
@@ -31979,7 +31979,7 @@
       </c>
     </row>
     <row r="1377" spans="1:2" ht="15">
-      <c r="A1377" s="49" t="s">
+      <c r="A1377" s="48" t="s">
         <v>1879</v>
       </c>
       <c r="B1377" s="15" t="s">
@@ -31987,7 +31987,7 @@
       </c>
     </row>
     <row r="1378" spans="1:2" ht="15">
-      <c r="A1378" s="49" t="s">
+      <c r="A1378" s="48" t="s">
         <v>1880</v>
       </c>
       <c r="B1378" s="15" t="s">
@@ -31995,7 +31995,7 @@
       </c>
     </row>
     <row r="1379" spans="1:2" ht="15">
-      <c r="A1379" s="49" t="s">
+      <c r="A1379" s="48" t="s">
         <v>1881</v>
       </c>
       <c r="B1379" s="15" t="s">
@@ -32003,7 +32003,7 @@
       </c>
     </row>
     <row r="1380" spans="1:2" ht="15">
-      <c r="A1380" s="49" t="s">
+      <c r="A1380" s="48" t="s">
         <v>1882</v>
       </c>
       <c r="B1380" s="15" t="s">
@@ -32011,7 +32011,7 @@
       </c>
     </row>
     <row r="1381" spans="1:2" ht="40.799999999999997">
-      <c r="A1381" s="48" t="s">
+      <c r="A1381" s="47" t="s">
         <v>1883</v>
       </c>
       <c r="B1381" s="4" t="s">
@@ -32051,7 +32051,7 @@
       </c>
     </row>
     <row r="1386" spans="1:2" s="9" customFormat="1" ht="40.799999999999997">
-      <c r="A1386" s="48" t="s">
+      <c r="A1386" s="47" t="s">
         <v>1893</v>
       </c>
       <c r="B1386" s="15" t="s">
@@ -32099,7 +32099,7 @@
       </c>
     </row>
     <row r="1392" spans="1:2" ht="40.799999999999997">
-      <c r="A1392" s="48" t="s">
+      <c r="A1392" s="47" t="s">
         <v>1894</v>
       </c>
       <c r="B1392" s="4" t="s">
@@ -32139,7 +32139,7 @@
       </c>
     </row>
     <row r="1397" spans="1:2" ht="40.799999999999997">
-      <c r="A1397" s="48" t="s">
+      <c r="A1397" s="47" t="s">
         <v>1899</v>
       </c>
       <c r="B1397" s="4" t="s">
@@ -32219,7 +32219,7 @@
       </c>
     </row>
     <row r="1407" spans="1:2" ht="20.399999999999999">
-      <c r="A1407" s="48" t="s">
+      <c r="A1407" s="47" t="s">
         <v>1909</v>
       </c>
       <c r="B1407" s="15" t="s">
@@ -32251,7 +32251,7 @@
       </c>
     </row>
     <row r="1411" spans="1:2" ht="20.399999999999999">
-      <c r="A1411" s="48" t="s">
+      <c r="A1411" s="47" t="s">
         <v>1913</v>
       </c>
       <c r="B1411" s="4" t="s">
@@ -32292,8 +32292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -32587,8 +32587,8 @@
         <v>30</v>
       </c>
       <c r="N11" s="10"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
     </row>
     <row r="12" spans="1:19" s="9" customFormat="1">
       <c r="A12" s="9" t="s">

</xml_diff>

<commit_message>
added 410 to be translated from Standard
</commit_message>
<xml_diff>
--- a/LUO.xlsx
+++ b/LUO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ogayo\OneDrive\Desktop\Masakhane\Luo-News-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A914A69-DC98-459C-8019-3A951848B717}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDBA03F-AB1B-4578-87E0-694CF34D6EB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined_text" sheetId="9" r:id="rId1"/>
     <sheet name="New 10-3-2021" sheetId="17" r:id="rId2"/>
-    <sheet name="New May 2021" sheetId="18" r:id="rId3"/>
-    <sheet name="Classified" sheetId="2" r:id="rId4"/>
+    <sheet name="Classified" sheetId="2" r:id="rId3"/>
+    <sheet name="New May 2021" sheetId="18" r:id="rId4"/>
     <sheet name="Statistics" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4639" uniqueCount="1917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4644" uniqueCount="1922">
   <si>
     <t>Jii 7 jowito ngimagi e masira mar apaya yoo Kisian e County ma Kisumu</t>
   </si>
@@ -5804,12 +5804,27 @@
   <si>
     <t>Abdulkadir koro okao kar wuongi mosenindo Yussuf Haji mane magoro olalgo kane en e senator ma Garissa kuno</t>
   </si>
+  <si>
+    <t>Starts from 1276 in Classified sheet</t>
+  </si>
+  <si>
+    <t>Regional Commissioner ma Nyanza koro ne owuoyo ewii ikruok moseketi ne Madaraka Day</t>
+  </si>
+  <si>
+    <t>Regional Commissioner ma Nyanza migosi Magu Mutindika kawuono koro ne oyango ni giseketo okenge duto mag biro thiro landruok mar tuo mar corona e kinde nyasi mag Madaraka Day ma higani ma obiro bago e boma ma Kisumu -kowacho ni giketo okengego kaluwore gi wach jimbruok mag landruok mar tuono</t>
+  </si>
+  <si>
+    <t>Kanomedowuoyo ewii wachno migosi Mutindika nowacho ni gibironeno ni alap ma Jomo Kenyatta International Stadium man Mamboleo Kisumu ma ibiro bagoe nyasino obiro oluwo chike duto mag kedo gi tuono kod neno ni welo duto mabiro dhi kanyo chiengno jobiro oluwo chike mag kedo gi tuono bende</t>
+  </si>
+  <si>
+    <t>Kanowuoyo e boma ma Kisumu jatelono bende ne oyango ni yoore mag arita osehiki mogik tik e boma ma Kisumu kuno ka iikruok ne nyasino.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5983,6 +5998,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -6341,7 +6362,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6465,6 +6486,9 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -12053,8 +12077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A1414"/>
   <sheetViews>
-    <sheetView topLeftCell="A1053" workbookViewId="0">
-      <selection activeCell="D1058" sqref="D1058"/>
+    <sheetView topLeftCell="A1401" workbookViewId="0">
+      <selection activeCell="A1414" sqref="A1414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -19143,7 +19167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF2FC49-8576-4274-9513-E8D9E893D3B5}">
   <dimension ref="A1:A358"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A340" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -20949,25 +20973,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5386CA97-9DB9-4D9E-A52E-CC64BCC04B59}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C1418"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B1414"/>
-  <sheetViews>
-    <sheetView topLeftCell="A1157" workbookViewId="0">
-      <selection activeCell="B1157" sqref="B1157"/>
+    <sheetView tabSelected="1" topLeftCell="A1412" workbookViewId="0">
+      <selection activeCell="D1456" sqref="D1456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -31203,9 +31213,7 @@
       </c>
     </row>
     <row r="1280" spans="1:2" ht="19.8">
-      <c r="A1280" s="46">
-        <v>8</v>
-      </c>
+      <c r="A1280" s="46"/>
       <c r="B1280" s="21" t="s">
         <v>8</v>
       </c>
@@ -32234,7 +32242,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1409" spans="1:2" ht="138.6">
+    <row r="1409" spans="1:3" ht="138.6">
       <c r="A1409" s="46" t="s">
         <v>1911</v>
       </c>
@@ -32242,7 +32250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1410" spans="1:2" ht="138.6">
+    <row r="1410" spans="1:3" ht="138.6">
       <c r="A1410" s="46" t="s">
         <v>1912</v>
       </c>
@@ -32250,7 +32258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1411" spans="1:2" ht="20.399999999999999">
+    <row r="1411" spans="1:3" ht="20.399999999999999">
       <c r="A1411" s="47" t="s">
         <v>1913</v>
       </c>
@@ -32258,7 +32266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1412" spans="1:2" ht="39.6">
+    <row r="1412" spans="1:3" ht="39.6">
       <c r="A1412" s="46" t="s">
         <v>1914</v>
       </c>
@@ -32266,7 +32274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1413" spans="1:2" ht="19.8">
+    <row r="1413" spans="1:3" ht="19.8">
       <c r="A1413" s="46" t="s">
         <v>1915</v>
       </c>
@@ -32274,17 +32282,63 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1414" spans="1:2" ht="39.6">
+    <row r="1414" spans="1:3" ht="39.6">
       <c r="A1414" s="46" t="s">
         <v>1916</v>
       </c>
       <c r="B1414" s="15" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:3" ht="40.799999999999997">
+      <c r="A1415" s="50" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C1415">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:3" ht="79.2">
+      <c r="A1416" s="46" t="s">
+        <v>1919</v>
+      </c>
+      <c r="C1416">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:3" ht="79.2">
+      <c r="A1417" s="46" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:3" ht="39.6">
+      <c r="A1418" s="46" t="s">
+        <v>1921</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5386CA97-9DB9-4D9E-A52E-CC64BCC04B59}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -32292,8 +32346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
added 20 more Dholuo sentences, and translation folder
</commit_message>
<xml_diff>
--- a/LUO.xlsx
+++ b/LUO.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ogayo\OneDrive\Desktop\Masakhane\Luo-News-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CE1487-17DA-4274-8A19-C423730F18F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490C53B3-39C9-489A-8603-CE38A41239AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined_text" sheetId="9" r:id="rId1"/>
     <sheet name="New 10-3-2021" sheetId="17" r:id="rId2"/>
     <sheet name="Classified" sheetId="2" r:id="rId3"/>
-    <sheet name="New May 2021" sheetId="18" r:id="rId4"/>
+    <sheet name="May- June 2021" sheetId="18" r:id="rId4"/>
     <sheet name="Statistics" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5257" uniqueCount="2233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5294" uniqueCount="2253">
   <si>
     <t>Jii 7 jowito ngimagi e masira mar apaya yoo Kisian e County ma Kisumu</t>
   </si>
@@ -6461,9 +6461,6 @@
     <t>Chief justice machon migosi David Maraga wachoni Ker Uhuru Kenyatta onego thich oko e tich kaluoreni oserem tayo chenro mar chamo muma mar jong'ad buche 41 manosepuodhi kod duol mar doho.</t>
   </si>
   <si>
-    <t>Lolwe TV</t>
-  </si>
-  <si>
     <t>Period/Source</t>
   </si>
   <si>
@@ -6582,9 +6579,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tend duond Bura mar ODM ogolo chik ne Mca's mag county assembly ma Migori ochak okang' mokwongo mar thicho oko eapis Gov. Okoth Obado kaluore gi pek mar Case Mar Mibadhi momake. </t>
-  </si>
-  <si>
-    <t>Radio Lake Victoria</t>
   </si>
   <si>
     <t>Riwruok mar adhula e Africa CAF, ogoo Gor Mahia fine mar siling tara 3 kaachiel bende gi kumo Kenneth Muguna gi Boniface Oluoch ma iwacho ni nomonjo jakudh firimbi e piny Zambia e tugo e kind Gor gi Napsa Stars.</t>
@@ -6754,6 +6748,72 @@
   </si>
   <si>
     <t>Jakom Ambrose Rachier oyango mano.</t>
+  </si>
+  <si>
+    <t>Laktar Amoth ne oguel kaka jakom board maduong mar WHO</t>
+  </si>
+  <si>
+    <t>Riuruok mochungne weche mag thieth e bwo piny mangima -World Health Organization -WHO- kawuono ne oguelo Director makojolo e migao mochungne yoore mag thieth e pachoka laktar Patrick Amoth kaka jakom board maduong mar riuruok mar WHO no</t>
+  </si>
+  <si>
+    <t>Magi ne oyangi kod jatend migao mochungne yoore mag thieth e riuruogno laktar Harsh Vardhan mane otimo lendono e romo mar 149 mar board mar riuruok mar World Health Organizationno</t>
+  </si>
+  <si>
+    <t>E dwe mar 5 mar higa mokalo , laktar Amoth ne oyier kaka jalup ker mar board maduong mar riuruok mar World Health Organizationno – e lemo mane odhi bede kuom higni ariyo</t>
+  </si>
+  <si>
+    <t>Gikone gavana mar county ma Migori Zachary Okoth Obado ochopo e nyim komiti mar od bura mar senate ma ng’iyo kaka itiyo gi omenda jopiny.</t>
+  </si>
+  <si>
+    <t>Migosi Obado nyocha oluongi gi komitino mondo mii ochopi kawuono ma ok olewo bang’ ka dwee mokalo ne orem ma ok ochopo kata bang’ kane osemiye milome.</t>
+  </si>
+  <si>
+    <t>Komitino nyocha nikod penjo ewii lipod odita jener ka achiel kuom weche nen ni tend county ma migori ne orem ma ok ochiwo oboke moko ma dwarore ne apis odita jener mondo mii ne non kaka itiyo gi omenda e piny owacho mar migori.</t>
+  </si>
+  <si>
+    <t>Gavana Obado kata kamano okoo ni ne oluwore gi okenge mag kedo gi midhusi mar coronavirus nimar hike thoth ne 58 kendo ne ok onyal chopo e apise dhii kawo obokego mondo mii ochiwgi.</t>
+  </si>
+  <si>
+    <t>Ramogi website June 2021</t>
+  </si>
+  <si>
+    <t>Tarik moket mar yalo appeal mar Paro mar chik mar BBI koro ong'uko tarik mane iliekoni itime ombulu mar Paro.</t>
+  </si>
+  <si>
+    <t>Waikore mar kelonu lendo achiel kachiel kowuok e paw tuke mar Jomo Kenyatta International Stadium Kisumu Mamboleo e nyasi mar 58 mar Madaraka day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joohala moko bende osechopo e paw tuke mar Jomo Kenyatta International Stadium Kisumu e nyasi mar MadarakaDay 2021 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaka Weche Chalo e paw tuke mar Jomo Kenyatta International Stadium Kisumu e nyasi mar 58 mar #MadarakaDay2021 </t>
+  </si>
+  <si>
+    <t>Radio Lake Victoria Twitter</t>
+  </si>
+  <si>
+    <t>Lolwe TV Twiter</t>
+  </si>
+  <si>
+    <t>Piny Uingereza chano bago romo odiochieng'  makawuono gi jotend ute thieth mawuok e pinje abirio madongo momewo,mong'ere kaka G7 kumagidhi wuoye ewi pinje maonge nyalo maok nyalo yudo chanjo mar Covid -19 kaachiel gi tuoche manenore e Lee</t>
+  </si>
+  <si>
+    <t>Duol mar African Union(AU ) ochungo kuom thuolo pinyno mar  Mali ebedo jakanyo margi kaluore giloko loch magiloko kendo e tielo mar ariyo ekind dweche ochiko mokalo.</t>
+  </si>
+  <si>
+    <t>Duolno mar AU kokalo e telo mochung'ne kelo kwe kod arita okao ondamono nyakachieng' gilure gi chike.</t>
+  </si>
+  <si>
+    <t>Piny Australia ochoro nyime lockdown mar gweng' ma Melbourne kuom juma achiel kaluore gi medruok mar midhusi mar Corona e boma ma Melbourne juma mokadho.</t>
+  </si>
+  <si>
+    <t>Ker mapiny South Africa Cyril Ramaphosa owachoni pinyno chano keto chike motegno mag Covid -19 kaluoreni third wave mar Corona nyalo nenore machiegni.</t>
+  </si>
+  <si>
+    <t>Lolwe Twitter June</t>
+  </si>
+  <si>
+    <t>Ramogi Twitter June</t>
   </si>
 </sst>
 </file>
@@ -7438,9 +7498,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7461,6 +7518,9 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -20250,7 +20310,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="28.8">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>1222</v>
       </c>
     </row>
@@ -22046,10 +22106,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C1722"/>
+  <dimension ref="A1:C1738"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1712" workbookViewId="0">
-      <selection activeCell="A1718" sqref="A1718"/>
+    <sheetView topLeftCell="A1729" workbookViewId="0">
+      <selection activeCell="A1738" sqref="A1738"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -22242,7 +22302,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="28.8">
+    <row r="24" spans="1:2" ht="43.2">
       <c r="A24" s="21" t="s">
         <v>30</v>
       </c>
@@ -22378,7 +22438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="43.2">
+    <row r="41" spans="1:2" ht="57.6">
       <c r="A41" s="21" t="s">
         <v>48</v>
       </c>
@@ -22442,7 +22502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="57.6">
+    <row r="49" spans="1:2" ht="72">
       <c r="A49" s="21" t="s">
         <v>56</v>
       </c>
@@ -22530,7 +22590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" ht="28.8">
       <c r="A60" s="19" t="s">
         <v>67</v>
       </c>
@@ -22538,7 +22598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" ht="28.8">
       <c r="A61" s="19" t="s">
         <v>68</v>
       </c>
@@ -22610,7 +22670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="28.8">
+    <row r="70" spans="1:2" ht="43.2">
       <c r="A70" s="21" t="s">
         <v>77</v>
       </c>
@@ -22706,7 +22766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="43.2">
+    <row r="82" spans="1:2" ht="57.6">
       <c r="A82" s="21" t="s">
         <v>89</v>
       </c>
@@ -22746,7 +22806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="28.8">
+    <row r="87" spans="1:2" ht="43.2">
       <c r="A87" s="21" t="s">
         <v>94</v>
       </c>
@@ -22866,7 +22926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="28.8">
+    <row r="102" spans="1:2" ht="43.2">
       <c r="A102" s="21" t="s">
         <v>107</v>
       </c>
@@ -23050,7 +23110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="28.8">
+    <row r="125" spans="1:2" ht="43.2">
       <c r="A125" s="21" t="s">
         <v>141</v>
       </c>
@@ -23074,7 +23134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="43.2">
+    <row r="128" spans="1:2" ht="57.6">
       <c r="A128" s="21" t="s">
         <v>144</v>
       </c>
@@ -23090,7 +23150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="28.8">
+    <row r="130" spans="1:2" ht="43.2">
       <c r="A130" s="21" t="s">
         <v>146</v>
       </c>
@@ -23130,7 +23190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="28.8">
+    <row r="135" spans="1:2" ht="43.2">
       <c r="A135" s="21" t="s">
         <v>151</v>
       </c>
@@ -23202,7 +23262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="28.8">
+    <row r="144" spans="1:2" ht="43.2">
       <c r="A144" s="21" t="s">
         <v>160</v>
       </c>
@@ -23258,7 +23318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="28.8">
+    <row r="151" spans="1:2" ht="43.2">
       <c r="A151" s="21" t="s">
         <v>167</v>
       </c>
@@ -23290,7 +23350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="28.8">
+    <row r="155" spans="1:2" ht="43.2">
       <c r="A155" s="21" t="s">
         <v>171</v>
       </c>
@@ -23298,7 +23358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" ht="28.8">
       <c r="A156" s="21" t="s">
         <v>172</v>
       </c>
@@ -23314,7 +23374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" ht="28.8">
       <c r="A158" s="21" t="s">
         <v>174</v>
       </c>
@@ -23410,7 +23470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="28.8">
+    <row r="170" spans="1:2" ht="43.2">
       <c r="A170" s="21" t="s">
         <v>184</v>
       </c>
@@ -23554,7 +23614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="43.2">
+    <row r="188" spans="1:2" ht="57.6">
       <c r="A188" s="21" t="s">
         <v>203</v>
       </c>
@@ -23570,7 +23630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="28.8">
+    <row r="190" spans="1:2" ht="43.2">
       <c r="A190" s="21" t="s">
         <v>205</v>
       </c>
@@ -23602,7 +23662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="43.2">
+    <row r="194" spans="1:2" ht="57.6">
       <c r="A194" s="21" t="s">
         <v>209</v>
       </c>
@@ -23610,7 +23670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="43.2">
+    <row r="195" spans="1:2" ht="57.6">
       <c r="A195" s="21" t="s">
         <v>210</v>
       </c>
@@ -23722,7 +23782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="28.8">
+    <row r="209" spans="1:2" ht="43.2">
       <c r="A209" s="21" t="s">
         <v>224</v>
       </c>
@@ -23730,7 +23790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="28.8">
+    <row r="210" spans="1:2" ht="43.2">
       <c r="A210" s="21" t="s">
         <v>225</v>
       </c>
@@ -23762,7 +23822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="43.2">
+    <row r="214" spans="1:2" ht="57.6">
       <c r="A214" s="21" t="s">
         <v>229</v>
       </c>
@@ -23842,7 +23902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="28.8">
+    <row r="224" spans="1:2" ht="43.2">
       <c r="A224" s="21" t="s">
         <v>237</v>
       </c>
@@ -23882,7 +23942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="28.8">
+    <row r="229" spans="1:2" ht="43.2">
       <c r="A229" s="21" t="s">
         <v>241</v>
       </c>
@@ -23922,7 +23982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" ht="28.8">
       <c r="A234" s="21" t="s">
         <v>245</v>
       </c>
@@ -24034,7 +24094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="28.8">
+    <row r="248" spans="1:2" ht="43.2">
       <c r="A248" s="21" t="s">
         <v>117</v>
       </c>
@@ -24066,7 +24126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" ht="28.8">
       <c r="A252" s="21" t="s">
         <v>121</v>
       </c>
@@ -24138,7 +24198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="28.8">
+    <row r="261" spans="1:2" ht="43.2">
       <c r="A261" s="21" t="s">
         <v>263</v>
       </c>
@@ -24146,7 +24206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="28.8">
+    <row r="262" spans="1:2" ht="43.2">
       <c r="A262" s="21" t="s">
         <v>264</v>
       </c>
@@ -24274,7 +24334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" ht="28.8">
       <c r="A278" s="21" t="s">
         <v>281</v>
       </c>
@@ -24386,7 +24446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="292" spans="1:2" ht="28.8">
+    <row r="292" spans="1:2" ht="43.2">
       <c r="A292" s="21" t="s">
         <v>295</v>
       </c>
@@ -24434,7 +24494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="28.8">
+    <row r="298" spans="1:2" ht="43.2">
       <c r="A298" s="21" t="s">
         <v>301</v>
       </c>
@@ -24466,7 +24526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="28.8">
+    <row r="302" spans="1:2" ht="43.2">
       <c r="A302" s="21" t="s">
         <v>305</v>
       </c>
@@ -24618,7 +24678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="321" spans="1:2" ht="28.8">
+    <row r="321" spans="1:2" ht="43.2">
       <c r="A321" s="21" t="s">
         <v>320</v>
       </c>
@@ -24634,7 +24694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="323" spans="1:2" ht="28.8">
+    <row r="323" spans="1:2" ht="43.2">
       <c r="A323" s="21" t="s">
         <v>324</v>
       </c>
@@ -24642,7 +24702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="28.8">
+    <row r="324" spans="1:2" ht="43.2">
       <c r="A324" s="21" t="s">
         <v>325</v>
       </c>
@@ -32455,7 +32515,7 @@
       </c>
     </row>
     <row r="1301" spans="1:2" ht="30">
-      <c r="A1301" s="51" t="s">
+      <c r="A1301" s="50" t="s">
         <v>1806</v>
       </c>
       <c r="B1301" t="s">
@@ -32463,7 +32523,7 @@
       </c>
     </row>
     <row r="1302" spans="1:2" ht="45">
-      <c r="A1302" s="51" t="s">
+      <c r="A1302" s="50" t="s">
         <v>1807</v>
       </c>
       <c r="B1302" s="8" t="s">
@@ -32471,7 +32531,7 @@
       </c>
     </row>
     <row r="1303" spans="1:2" ht="30">
-      <c r="A1303" s="51" t="s">
+      <c r="A1303" s="50" t="s">
         <v>1808</v>
       </c>
       <c r="B1303" s="8" t="s">
@@ -32479,7 +32539,7 @@
       </c>
     </row>
     <row r="1304" spans="1:2" ht="15">
-      <c r="A1304" s="51" t="s">
+      <c r="A1304" s="50" t="s">
         <v>1809</v>
       </c>
       <c r="B1304" s="8" t="s">
@@ -32487,7 +32547,7 @@
       </c>
     </row>
     <row r="1305" spans="1:2" ht="15">
-      <c r="A1305" s="51" t="s">
+      <c r="A1305" s="50" t="s">
         <v>1810</v>
       </c>
       <c r="B1305" s="8" t="s">
@@ -32503,7 +32563,7 @@
       </c>
     </row>
     <row r="1307" spans="1:2" ht="30">
-      <c r="A1307" s="51" t="s">
+      <c r="A1307" s="50" t="s">
         <v>1812</v>
       </c>
       <c r="B1307" s="3" t="s">
@@ -32511,7 +32571,7 @@
       </c>
     </row>
     <row r="1308" spans="1:2" ht="60">
-      <c r="A1308" s="51" t="s">
+      <c r="A1308" s="50" t="s">
         <v>1813</v>
       </c>
       <c r="B1308" s="14" t="s">
@@ -32519,7 +32579,7 @@
       </c>
     </row>
     <row r="1309" spans="1:2" ht="45">
-      <c r="A1309" s="51" t="s">
+      <c r="A1309" s="50" t="s">
         <v>1814</v>
       </c>
       <c r="B1309" s="14" t="s">
@@ -32535,7 +32595,7 @@
       </c>
     </row>
     <row r="1311" spans="1:2" ht="45">
-      <c r="A1311" s="51" t="s">
+      <c r="A1311" s="50" t="s">
         <v>1816</v>
       </c>
       <c r="B1311" s="3" t="s">
@@ -32543,7 +32603,7 @@
       </c>
     </row>
     <row r="1312" spans="1:2" ht="30">
-      <c r="A1312" s="51" t="s">
+      <c r="A1312" s="50" t="s">
         <v>1817</v>
       </c>
       <c r="B1312" s="14" t="s">
@@ -32551,7 +32611,7 @@
       </c>
     </row>
     <row r="1313" spans="1:2" ht="15">
-      <c r="A1313" s="51" t="s">
+      <c r="A1313" s="50" t="s">
         <v>1818</v>
       </c>
       <c r="B1313" s="14" t="s">
@@ -32567,7 +32627,7 @@
       </c>
     </row>
     <row r="1315" spans="1:2" ht="30">
-      <c r="A1315" s="51" t="s">
+      <c r="A1315" s="50" t="s">
         <v>1820</v>
       </c>
       <c r="B1315" s="14" t="s">
@@ -32575,7 +32635,7 @@
       </c>
     </row>
     <row r="1316" spans="1:2" ht="15">
-      <c r="A1316" s="51" t="s">
+      <c r="A1316" s="50" t="s">
         <v>1821</v>
       </c>
       <c r="B1316" s="14" t="s">
@@ -32583,7 +32643,7 @@
       </c>
     </row>
     <row r="1317" spans="1:2" ht="30">
-      <c r="A1317" s="51" t="s">
+      <c r="A1317" s="50" t="s">
         <v>1822</v>
       </c>
       <c r="B1317" s="14" t="s">
@@ -32591,7 +32651,7 @@
       </c>
     </row>
     <row r="1318" spans="1:2" ht="15">
-      <c r="A1318" s="51" t="s">
+      <c r="A1318" s="50" t="s">
         <v>1823</v>
       </c>
       <c r="B1318" s="14" t="s">
@@ -32791,7 +32851,7 @@
       </c>
     </row>
     <row r="1343" spans="1:2" ht="45">
-      <c r="A1343" s="51" t="s">
+      <c r="A1343" s="50" t="s">
         <v>1848</v>
       </c>
       <c r="B1343" s="14" t="s">
@@ -32799,7 +32859,7 @@
       </c>
     </row>
     <row r="1344" spans="1:2" ht="30">
-      <c r="A1344" s="51" t="s">
+      <c r="A1344" s="50" t="s">
         <v>1850</v>
       </c>
       <c r="B1344" s="3" t="s">
@@ -32807,7 +32867,7 @@
       </c>
     </row>
     <row r="1345" spans="1:2" ht="15">
-      <c r="A1345" s="51" t="s">
+      <c r="A1345" s="50" t="s">
         <v>1851</v>
       </c>
       <c r="B1345" s="14" t="s">
@@ -32815,7 +32875,7 @@
       </c>
     </row>
     <row r="1346" spans="1:2" ht="15">
-      <c r="A1346" s="51" t="s">
+      <c r="A1346" s="50" t="s">
         <v>1849</v>
       </c>
       <c r="B1346" s="14" t="s">
@@ -32831,7 +32891,7 @@
       </c>
     </row>
     <row r="1348" spans="1:2" ht="45">
-      <c r="A1348" s="51" t="s">
+      <c r="A1348" s="50" t="s">
         <v>1853</v>
       </c>
       <c r="B1348" s="14" t="s">
@@ -32839,7 +32899,7 @@
       </c>
     </row>
     <row r="1349" spans="1:2" ht="30">
-      <c r="A1349" s="51" t="s">
+      <c r="A1349" s="50" t="s">
         <v>1854</v>
       </c>
       <c r="B1349" s="3" t="s">
@@ -32847,7 +32907,7 @@
       </c>
     </row>
     <row r="1350" spans="1:2" ht="60">
-      <c r="A1350" s="51" t="s">
+      <c r="A1350" s="50" t="s">
         <v>1855</v>
       </c>
       <c r="B1350" s="14" t="s">
@@ -33023,7 +33083,7 @@
       </c>
     </row>
     <row r="1372" spans="1:2" ht="30">
-      <c r="A1372" s="51" t="s">
+      <c r="A1372" s="50" t="s">
         <v>1877</v>
       </c>
       <c r="B1372" s="14" t="s">
@@ -33031,7 +33091,7 @@
       </c>
     </row>
     <row r="1373" spans="1:2" ht="30">
-      <c r="A1373" s="51" t="s">
+      <c r="A1373" s="50" t="s">
         <v>1878</v>
       </c>
       <c r="B1373" s="3" t="s">
@@ -33039,7 +33099,7 @@
       </c>
     </row>
     <row r="1374" spans="1:2" ht="30">
-      <c r="A1374" s="51" t="s">
+      <c r="A1374" s="50" t="s">
         <v>1879</v>
       </c>
       <c r="B1374" s="14" t="s">
@@ -33047,7 +33107,7 @@
       </c>
     </row>
     <row r="1375" spans="1:2" ht="45">
-      <c r="A1375" s="51" t="s">
+      <c r="A1375" s="50" t="s">
         <v>1880</v>
       </c>
       <c r="B1375" s="14" t="s">
@@ -33055,7 +33115,7 @@
       </c>
     </row>
     <row r="1376" spans="1:2" ht="60">
-      <c r="A1376" s="51" t="s">
+      <c r="A1376" s="50" t="s">
         <v>1881</v>
       </c>
       <c r="B1376" s="14" t="s">
@@ -33063,7 +33123,7 @@
       </c>
     </row>
     <row r="1377" spans="1:2" ht="30">
-      <c r="A1377" s="51" t="s">
+      <c r="A1377" s="50" t="s">
         <v>1882</v>
       </c>
       <c r="B1377" s="14" t="s">
@@ -33375,7 +33435,7 @@
       </c>
     </row>
     <row r="1416" spans="1:3" ht="26.4">
-      <c r="A1416" s="48" t="s">
+      <c r="A1416" s="47" t="s">
         <v>1921</v>
       </c>
       <c r="B1416" s="3" t="s">
@@ -33391,7 +33451,7 @@
       </c>
     </row>
     <row r="1418" spans="1:3" ht="26.4">
-      <c r="A1418" s="48" t="s">
+      <c r="A1418" s="47" t="s">
         <v>1923</v>
       </c>
       <c r="B1418" s="3" t="s">
@@ -33431,7 +33491,7 @@
       </c>
     </row>
     <row r="1423" spans="1:3" ht="81.599999999999994">
-      <c r="A1423" s="52" t="s">
+      <c r="A1423" s="51" t="s">
         <v>1928</v>
       </c>
       <c r="B1423" s="14" t="s">
@@ -33471,7 +33531,7 @@
       </c>
     </row>
     <row r="1428" spans="1:2" ht="26.4">
-      <c r="A1428" s="48" t="s">
+      <c r="A1428" s="47" t="s">
         <v>1933</v>
       </c>
       <c r="B1428" s="3" t="s">
@@ -33487,7 +33547,7 @@
       </c>
     </row>
     <row r="1430" spans="1:2" ht="26.4">
-      <c r="A1430" s="48" t="s">
+      <c r="A1430" s="47" t="s">
         <v>1935</v>
       </c>
       <c r="B1430" s="3" t="s">
@@ -33511,7 +33571,7 @@
       </c>
     </row>
     <row r="1433" spans="1:2" ht="26.4">
-      <c r="A1433" s="48" t="s">
+      <c r="A1433" s="47" t="s">
         <v>1938</v>
       </c>
       <c r="B1433" s="14" t="s">
@@ -33519,7 +33579,7 @@
       </c>
     </row>
     <row r="1434" spans="1:2" ht="26.4">
-      <c r="A1434" s="48" t="s">
+      <c r="A1434" s="47" t="s">
         <v>1939</v>
       </c>
       <c r="B1434" s="14" t="s">
@@ -33527,7 +33587,7 @@
       </c>
     </row>
     <row r="1435" spans="1:2" ht="26.4">
-      <c r="A1435" s="48" t="s">
+      <c r="A1435" s="47" t="s">
         <v>1940</v>
       </c>
       <c r="B1435" s="3" t="s">
@@ -33535,7 +33595,7 @@
       </c>
     </row>
     <row r="1436" spans="1:2" ht="39.6">
-      <c r="A1436" s="48" t="s">
+      <c r="A1436" s="47" t="s">
         <v>1941</v>
       </c>
       <c r="B1436" s="14" t="s">
@@ -33543,7 +33603,7 @@
       </c>
     </row>
     <row r="1437" spans="1:2">
-      <c r="A1437" s="48" t="s">
+      <c r="A1437" s="47" t="s">
         <v>1942</v>
       </c>
       <c r="B1437" s="3" t="s">
@@ -33559,7 +33619,7 @@
       </c>
     </row>
     <row r="1439" spans="1:2" ht="39.6">
-      <c r="A1439" s="48" t="s">
+      <c r="A1439" s="47" t="s">
         <v>1944</v>
       </c>
       <c r="B1439" s="3" t="s">
@@ -33567,7 +33627,7 @@
       </c>
     </row>
     <row r="1440" spans="1:2" ht="81.599999999999994">
-      <c r="A1440" s="52" t="s">
+      <c r="A1440" s="51" t="s">
         <v>1945</v>
       </c>
       <c r="B1440" s="14" t="s">
@@ -33599,7 +33659,7 @@
       </c>
     </row>
     <row r="1444" spans="1:2" ht="26.4">
-      <c r="A1444" s="48" t="s">
+      <c r="A1444" s="47" t="s">
         <v>1949</v>
       </c>
       <c r="B1444" s="3" t="s">
@@ -33607,7 +33667,7 @@
       </c>
     </row>
     <row r="1445" spans="1:2" ht="26.4">
-      <c r="A1445" s="50" t="s">
+      <c r="A1445" s="49" t="s">
         <v>1950</v>
       </c>
       <c r="B1445" s="3" t="s">
@@ -33623,7 +33683,7 @@
       </c>
     </row>
     <row r="1447" spans="1:2" ht="26.4">
-      <c r="A1447" s="48" t="s">
+      <c r="A1447" s="47" t="s">
         <v>1952</v>
       </c>
       <c r="B1447" s="3" t="s">
@@ -33639,7 +33699,7 @@
       </c>
     </row>
     <row r="1449" spans="1:2" ht="26.4">
-      <c r="A1449" s="48" t="s">
+      <c r="A1449" s="47" t="s">
         <v>1954</v>
       </c>
       <c r="B1449" s="14" t="s">
@@ -33655,7 +33715,7 @@
       </c>
     </row>
     <row r="1451" spans="1:2" ht="26.4">
-      <c r="A1451" s="50" t="s">
+      <c r="A1451" s="49" t="s">
         <v>1956</v>
       </c>
       <c r="B1451" s="14" t="s">
@@ -33671,7 +33731,7 @@
       </c>
     </row>
     <row r="1453" spans="1:2" ht="26.4">
-      <c r="A1453" s="48" t="s">
+      <c r="A1453" s="47" t="s">
         <v>1958</v>
       </c>
       <c r="B1453" s="14" t="s">
@@ -33695,7 +33755,7 @@
       </c>
     </row>
     <row r="1456" spans="1:2" ht="26.4">
-      <c r="A1456" s="48" t="s">
+      <c r="A1456" s="47" t="s">
         <v>1961</v>
       </c>
       <c r="B1456" s="14" t="s">
@@ -33703,7 +33763,7 @@
       </c>
     </row>
     <row r="1457" spans="1:2" ht="39.6">
-      <c r="A1457" s="48" t="s">
+      <c r="A1457" s="47" t="s">
         <v>1962</v>
       </c>
       <c r="B1457" s="14" t="s">
@@ -33727,7 +33787,7 @@
       </c>
     </row>
     <row r="1460" spans="1:2">
-      <c r="A1460" s="47" t="s">
+      <c r="A1460" s="46" t="s">
         <v>1965</v>
       </c>
       <c r="B1460" s="14" t="s">
@@ -33743,7 +33803,7 @@
       </c>
     </row>
     <row r="1462" spans="1:2">
-      <c r="A1462" s="47" t="s">
+      <c r="A1462" s="46" t="s">
         <v>1967</v>
       </c>
       <c r="B1462" s="14" t="s">
@@ -33759,7 +33819,7 @@
       </c>
     </row>
     <row r="1464" spans="1:2">
-      <c r="A1464" s="47" t="s">
+      <c r="A1464" s="46" t="s">
         <v>1969</v>
       </c>
       <c r="B1464" s="14" t="s">
@@ -33767,7 +33827,7 @@
       </c>
     </row>
     <row r="1465" spans="1:2">
-      <c r="A1465" s="47" t="s">
+      <c r="A1465" s="46" t="s">
         <v>1970</v>
       </c>
       <c r="B1465" s="14" t="s">
@@ -33775,7 +33835,7 @@
       </c>
     </row>
     <row r="1466" spans="1:2">
-      <c r="A1466" s="47" t="s">
+      <c r="A1466" s="46" t="s">
         <v>1971</v>
       </c>
       <c r="B1466" s="3" t="s">
@@ -33783,7 +33843,7 @@
       </c>
     </row>
     <row r="1467" spans="1:2" ht="20.399999999999999">
-      <c r="A1467" s="49" t="s">
+      <c r="A1467" s="48" t="s">
         <v>1972</v>
       </c>
       <c r="B1467" s="3" t="s">
@@ -33791,7 +33851,7 @@
       </c>
     </row>
     <row r="1468" spans="1:2">
-      <c r="A1468" s="47" t="s">
+      <c r="A1468" s="46" t="s">
         <v>1973</v>
       </c>
       <c r="B1468" s="14" t="s">
@@ -33799,7 +33859,7 @@
       </c>
     </row>
     <row r="1469" spans="1:2">
-      <c r="A1469" s="47" t="s">
+      <c r="A1469" s="46" t="s">
         <v>1974</v>
       </c>
       <c r="B1469" s="14" t="s">
@@ -33807,7 +33867,7 @@
       </c>
     </row>
     <row r="1470" spans="1:2">
-      <c r="A1470" s="47" t="s">
+      <c r="A1470" s="46" t="s">
         <v>1975</v>
       </c>
       <c r="B1470" s="14" t="s">
@@ -33815,7 +33875,7 @@
       </c>
     </row>
     <row r="1471" spans="1:2">
-      <c r="A1471" s="47" t="s">
+      <c r="A1471" s="46" t="s">
         <v>1976</v>
       </c>
       <c r="B1471" s="14" t="s">
@@ -33831,7 +33891,7 @@
       </c>
     </row>
     <row r="1473" spans="1:2">
-      <c r="A1473" s="47" t="s">
+      <c r="A1473" s="46" t="s">
         <v>1978</v>
       </c>
       <c r="B1473" s="14" t="s">
@@ -33839,7 +33899,7 @@
       </c>
     </row>
     <row r="1474" spans="1:2">
-      <c r="A1474" s="47" t="s">
+      <c r="A1474" s="46" t="s">
         <v>1979</v>
       </c>
       <c r="B1474" s="14" t="s">
@@ -33847,7 +33907,7 @@
       </c>
     </row>
     <row r="1475" spans="1:2">
-      <c r="A1475" s="47" t="s">
+      <c r="A1475" s="46" t="s">
         <v>1980</v>
       </c>
       <c r="B1475" s="14" t="s">
@@ -33871,7 +33931,7 @@
       </c>
     </row>
     <row r="1478" spans="1:2">
-      <c r="A1478" s="47" t="s">
+      <c r="A1478" s="46" t="s">
         <v>1982</v>
       </c>
       <c r="B1478" s="14" t="s">
@@ -33879,7 +33939,7 @@
       </c>
     </row>
     <row r="1479" spans="1:2">
-      <c r="A1479" s="47" t="s">
+      <c r="A1479" s="46" t="s">
         <v>1984</v>
       </c>
       <c r="B1479" s="3" t="s">
@@ -33895,7 +33955,7 @@
       </c>
     </row>
     <row r="1481" spans="1:2">
-      <c r="A1481" s="47" t="s">
+      <c r="A1481" s="46" t="s">
         <v>1986</v>
       </c>
       <c r="B1481" s="14" t="s">
@@ -33903,7 +33963,7 @@
       </c>
     </row>
     <row r="1482" spans="1:2">
-      <c r="A1482" s="47" t="s">
+      <c r="A1482" s="46" t="s">
         <v>1987</v>
       </c>
       <c r="B1482" s="14" t="s">
@@ -33911,7 +33971,7 @@
       </c>
     </row>
     <row r="1483" spans="1:2">
-      <c r="A1483" s="47" t="s">
+      <c r="A1483" s="46" t="s">
         <v>1988</v>
       </c>
       <c r="B1483" s="14" t="s">
@@ -33919,12 +33979,12 @@
       </c>
     </row>
     <row r="1484" spans="1:2">
-      <c r="A1484" s="47" t="s">
+      <c r="A1484" s="46" t="s">
         <v>1989</v>
       </c>
     </row>
     <row r="1485" spans="1:2">
-      <c r="A1485" s="47" t="s">
+      <c r="A1485" s="46" t="s">
         <v>1990</v>
       </c>
       <c r="B1485" s="3" t="s">
@@ -33932,7 +33992,7 @@
       </c>
     </row>
     <row r="1486" spans="1:2">
-      <c r="A1486" s="47" t="s">
+      <c r="A1486" s="46" t="s">
         <v>1991</v>
       </c>
       <c r="B1486" s="3" t="s">
@@ -33940,7 +34000,7 @@
       </c>
     </row>
     <row r="1487" spans="1:2">
-      <c r="A1487" s="47" t="s">
+      <c r="A1487" s="46" t="s">
         <v>1992</v>
       </c>
       <c r="B1487" s="3" t="s">
@@ -33956,7 +34016,7 @@
       </c>
     </row>
     <row r="1489" spans="1:2">
-      <c r="A1489" s="47" t="s">
+      <c r="A1489" s="46" t="s">
         <v>1994</v>
       </c>
       <c r="B1489" s="14" t="s">
@@ -33972,7 +34032,7 @@
       </c>
     </row>
     <row r="1491" spans="1:2">
-      <c r="A1491" s="47" t="s">
+      <c r="A1491" s="46" t="s">
         <v>1996</v>
       </c>
       <c r="B1491" s="14" t="s">
@@ -33980,7 +34040,7 @@
       </c>
     </row>
     <row r="1492" spans="1:2">
-      <c r="A1492" s="47" t="s">
+      <c r="A1492" s="46" t="s">
         <v>1997</v>
       </c>
       <c r="B1492" s="14" t="s">
@@ -33996,7 +34056,7 @@
       </c>
     </row>
     <row r="1494" spans="1:2">
-      <c r="A1494" s="47" t="s">
+      <c r="A1494" s="46" t="s">
         <v>1999</v>
       </c>
       <c r="B1494" s="3" t="s">
@@ -34004,7 +34064,7 @@
       </c>
     </row>
     <row r="1495" spans="1:2">
-      <c r="A1495" s="47" t="s">
+      <c r="A1495" s="46" t="s">
         <v>2000</v>
       </c>
       <c r="B1495" s="3" t="s">
@@ -34012,7 +34072,7 @@
       </c>
     </row>
     <row r="1496" spans="1:2">
-      <c r="A1496" s="47" t="s">
+      <c r="A1496" s="46" t="s">
         <v>2001</v>
       </c>
       <c r="B1496" s="14" t="s">
@@ -34020,7 +34080,7 @@
       </c>
     </row>
     <row r="1497" spans="1:2">
-      <c r="A1497" s="47" t="s">
+      <c r="A1497" s="46" t="s">
         <v>2002</v>
       </c>
       <c r="B1497" s="14" t="s">
@@ -34028,7 +34088,7 @@
       </c>
     </row>
     <row r="1498" spans="1:2">
-      <c r="A1498" s="47" t="s">
+      <c r="A1498" s="46" t="s">
         <v>2003</v>
       </c>
       <c r="B1498" s="14" t="s">
@@ -34044,7 +34104,7 @@
       </c>
     </row>
     <row r="1500" spans="1:2">
-      <c r="A1500" s="47" t="s">
+      <c r="A1500" s="46" t="s">
         <v>2005</v>
       </c>
       <c r="B1500" s="14" t="s">
@@ -34052,7 +34112,7 @@
       </c>
     </row>
     <row r="1501" spans="1:2">
-      <c r="A1501" s="47" t="s">
+      <c r="A1501" s="46" t="s">
         <v>2006</v>
       </c>
       <c r="B1501" s="3" t="s">
@@ -34060,7 +34120,7 @@
       </c>
     </row>
     <row r="1502" spans="1:2">
-      <c r="A1502" s="47" t="s">
+      <c r="A1502" s="46" t="s">
         <v>2007</v>
       </c>
       <c r="B1502" s="14" t="s">
@@ -34068,7 +34128,7 @@
       </c>
     </row>
     <row r="1503" spans="1:2">
-      <c r="A1503" s="47" t="s">
+      <c r="A1503" s="46" t="s">
         <v>2008</v>
       </c>
       <c r="B1503" s="3" t="s">
@@ -34084,7 +34144,7 @@
       </c>
     </row>
     <row r="1505" spans="1:2">
-      <c r="A1505" s="47" t="s">
+      <c r="A1505" s="46" t="s">
         <v>2010</v>
       </c>
       <c r="B1505" s="3" t="s">
@@ -34092,7 +34152,7 @@
       </c>
     </row>
     <row r="1506" spans="1:2">
-      <c r="A1506" s="47" t="s">
+      <c r="A1506" s="46" t="s">
         <v>2011</v>
       </c>
       <c r="B1506" s="3" t="s">
@@ -34108,7 +34168,7 @@
       </c>
     </row>
     <row r="1508" spans="1:2">
-      <c r="A1508" s="47" t="s">
+      <c r="A1508" s="46" t="s">
         <v>2013</v>
       </c>
       <c r="B1508" s="3" t="s">
@@ -34116,7 +34176,7 @@
       </c>
     </row>
     <row r="1509" spans="1:2">
-      <c r="A1509" s="47" t="s">
+      <c r="A1509" s="46" t="s">
         <v>2014</v>
       </c>
       <c r="B1509" s="3" t="s">
@@ -34124,7 +34184,7 @@
       </c>
     </row>
     <row r="1510" spans="1:2">
-      <c r="A1510" s="47" t="s">
+      <c r="A1510" s="46" t="s">
         <v>2015</v>
       </c>
       <c r="B1510" s="3" t="s">
@@ -34132,7 +34192,7 @@
       </c>
     </row>
     <row r="1511" spans="1:2">
-      <c r="A1511" s="47" t="s">
+      <c r="A1511" s="46" t="s">
         <v>2016</v>
       </c>
       <c r="B1511" s="3" t="s">
@@ -34140,7 +34200,7 @@
       </c>
     </row>
     <row r="1512" spans="1:2">
-      <c r="A1512" s="47" t="s">
+      <c r="A1512" s="46" t="s">
         <v>2017</v>
       </c>
       <c r="B1512" s="3" t="s">
@@ -34156,7 +34216,7 @@
       </c>
     </row>
     <row r="1514" spans="1:2" ht="20.399999999999999">
-      <c r="A1514" s="49" t="s">
+      <c r="A1514" s="48" t="s">
         <v>2019</v>
       </c>
       <c r="B1514" s="3" t="s">
@@ -34164,7 +34224,7 @@
       </c>
     </row>
     <row r="1515" spans="1:2">
-      <c r="A1515" s="47" t="s">
+      <c r="A1515" s="46" t="s">
         <v>2020</v>
       </c>
       <c r="B1515" s="3" t="s">
@@ -34172,7 +34232,7 @@
       </c>
     </row>
     <row r="1516" spans="1:2">
-      <c r="A1516" s="47" t="s">
+      <c r="A1516" s="46" t="s">
         <v>2022</v>
       </c>
       <c r="B1516" s="3" t="s">
@@ -34180,7 +34240,7 @@
       </c>
     </row>
     <row r="1517" spans="1:2">
-      <c r="A1517" s="47" t="s">
+      <c r="A1517" s="46" t="s">
         <v>2023</v>
       </c>
       <c r="B1517" s="3" t="s">
@@ -34188,7 +34248,7 @@
       </c>
     </row>
     <row r="1518" spans="1:2">
-      <c r="A1518" s="47" t="s">
+      <c r="A1518" s="46" t="s">
         <v>2024</v>
       </c>
       <c r="B1518" s="3" t="s">
@@ -34204,7 +34264,7 @@
       </c>
     </row>
     <row r="1520" spans="1:2" s="8" customFormat="1">
-      <c r="A1520" s="47" t="s">
+      <c r="A1520" s="46" t="s">
         <v>2026</v>
       </c>
       <c r="B1520" s="14" t="s">
@@ -34212,7 +34272,7 @@
       </c>
     </row>
     <row r="1521" spans="1:2">
-      <c r="A1521" s="47" t="s">
+      <c r="A1521" s="46" t="s">
         <v>2027</v>
       </c>
       <c r="B1521" s="3" t="s">
@@ -34220,7 +34280,7 @@
       </c>
     </row>
     <row r="1522" spans="1:2">
-      <c r="A1522" s="47" t="s">
+      <c r="A1522" s="46" t="s">
         <v>2028</v>
       </c>
       <c r="B1522" s="3" t="s">
@@ -34228,7 +34288,7 @@
       </c>
     </row>
     <row r="1523" spans="1:2">
-      <c r="A1523" s="47" t="s">
+      <c r="A1523" s="46" t="s">
         <v>2029</v>
       </c>
       <c r="B1523" s="3" t="s">
@@ -34244,7 +34304,7 @@
       </c>
     </row>
     <row r="1525" spans="1:2">
-      <c r="A1525" s="47" t="s">
+      <c r="A1525" s="46" t="s">
         <v>2031</v>
       </c>
       <c r="B1525" s="3" t="s">
@@ -34252,7 +34312,7 @@
       </c>
     </row>
     <row r="1526" spans="1:2">
-      <c r="A1526" s="47" t="s">
+      <c r="A1526" s="46" t="s">
         <v>2032</v>
       </c>
       <c r="B1526" s="3" t="s">
@@ -34260,7 +34320,7 @@
       </c>
     </row>
     <row r="1527" spans="1:2">
-      <c r="A1527" s="47" t="s">
+      <c r="A1527" s="46" t="s">
         <v>2033</v>
       </c>
       <c r="B1527" s="3" t="s">
@@ -34268,7 +34328,7 @@
       </c>
     </row>
     <row r="1528" spans="1:2">
-      <c r="A1528" s="47" t="s">
+      <c r="A1528" s="46" t="s">
         <v>2034</v>
       </c>
       <c r="B1528" s="3" t="s">
@@ -34276,7 +34336,7 @@
       </c>
     </row>
     <row r="1529" spans="1:2">
-      <c r="A1529" s="47" t="s">
+      <c r="A1529" s="46" t="s">
         <v>2035</v>
       </c>
       <c r="B1529" s="3" t="s">
@@ -34292,7 +34352,7 @@
       </c>
     </row>
     <row r="1531" spans="1:2" ht="20.399999999999999">
-      <c r="A1531" s="49" t="s">
+      <c r="A1531" s="48" t="s">
         <v>2037</v>
       </c>
       <c r="B1531" s="3" t="s">
@@ -34308,7 +34368,7 @@
       </c>
     </row>
     <row r="1533" spans="1:2">
-      <c r="A1533" s="47" t="s">
+      <c r="A1533" s="46" t="s">
         <v>2039</v>
       </c>
       <c r="B1533" s="3" t="s">
@@ -34316,7 +34376,7 @@
       </c>
     </row>
     <row r="1534" spans="1:2" ht="20.399999999999999">
-      <c r="A1534" s="49" t="s">
+      <c r="A1534" s="48" t="s">
         <v>2040</v>
       </c>
       <c r="B1534" s="3" t="s">
@@ -34332,7 +34392,7 @@
       </c>
     </row>
     <row r="1536" spans="1:2">
-      <c r="A1536" s="47" t="s">
+      <c r="A1536" s="46" t="s">
         <v>2042</v>
       </c>
       <c r="B1536" s="3" t="s">
@@ -34340,7 +34400,7 @@
       </c>
     </row>
     <row r="1537" spans="1:2">
-      <c r="A1537" s="47" t="s">
+      <c r="A1537" s="46" t="s">
         <v>2043</v>
       </c>
       <c r="B1537" s="3" t="s">
@@ -34348,7 +34408,7 @@
       </c>
     </row>
     <row r="1538" spans="1:2">
-      <c r="A1538" s="47" t="s">
+      <c r="A1538" s="46" t="s">
         <v>2044</v>
       </c>
       <c r="B1538" s="3" t="s">
@@ -34356,7 +34416,7 @@
       </c>
     </row>
     <row r="1539" spans="1:2">
-      <c r="A1539" s="47" t="s">
+      <c r="A1539" s="46" t="s">
         <v>2045</v>
       </c>
       <c r="B1539" s="3" t="s">
@@ -34372,7 +34432,7 @@
       </c>
     </row>
     <row r="1541" spans="1:2">
-      <c r="A1541" s="47" t="s">
+      <c r="A1541" s="46" t="s">
         <v>2047</v>
       </c>
       <c r="B1541" s="14" t="s">
@@ -34388,7 +34448,7 @@
       </c>
     </row>
     <row r="1543" spans="1:2">
-      <c r="A1543" s="47" t="s">
+      <c r="A1543" s="46" t="s">
         <v>2049</v>
       </c>
       <c r="B1543" s="3" t="s">
@@ -34404,7 +34464,7 @@
       </c>
     </row>
     <row r="1545" spans="1:2">
-      <c r="A1545" s="47" t="s">
+      <c r="A1545" s="46" t="s">
         <v>2051</v>
       </c>
       <c r="B1545" s="14" t="s">
@@ -34420,7 +34480,7 @@
       </c>
     </row>
     <row r="1547" spans="1:2">
-      <c r="A1547" s="47" t="s">
+      <c r="A1547" s="46" t="s">
         <v>2053</v>
       </c>
       <c r="B1547" s="3" t="s">
@@ -34428,7 +34488,7 @@
       </c>
     </row>
     <row r="1548" spans="1:2">
-      <c r="A1548" s="47" t="s">
+      <c r="A1548" s="46" t="s">
         <v>2054</v>
       </c>
       <c r="B1548" s="3" t="s">
@@ -34444,7 +34504,7 @@
       </c>
     </row>
     <row r="1550" spans="1:2">
-      <c r="A1550" s="47" t="s">
+      <c r="A1550" s="46" t="s">
         <v>2056</v>
       </c>
       <c r="B1550" s="3" t="s">
@@ -34460,7 +34520,7 @@
       </c>
     </row>
     <row r="1552" spans="1:2">
-      <c r="A1552" s="47" t="s">
+      <c r="A1552" s="46" t="s">
         <v>2058</v>
       </c>
       <c r="B1552" s="3" t="s">
@@ -34476,7 +34536,7 @@
       </c>
     </row>
     <row r="1554" spans="1:2">
-      <c r="A1554" s="47" t="s">
+      <c r="A1554" s="46" t="s">
         <v>2060</v>
       </c>
       <c r="B1554" s="3" t="s">
@@ -34492,7 +34552,7 @@
       </c>
     </row>
     <row r="1556" spans="1:2">
-      <c r="A1556" s="47" t="s">
+      <c r="A1556" s="46" t="s">
         <v>2062</v>
       </c>
       <c r="B1556" s="3" t="s">
@@ -34500,7 +34560,7 @@
       </c>
     </row>
     <row r="1557" spans="1:2">
-      <c r="A1557" s="47" t="s">
+      <c r="A1557" s="46" t="s">
         <v>2063</v>
       </c>
       <c r="B1557" s="3" t="s">
@@ -34508,7 +34568,7 @@
       </c>
     </row>
     <row r="1558" spans="1:2">
-      <c r="A1558" s="47" t="s">
+      <c r="A1558" s="46" t="s">
         <v>2064</v>
       </c>
       <c r="B1558" s="3" t="s">
@@ -34524,7 +34584,7 @@
       </c>
     </row>
     <row r="1560" spans="1:2">
-      <c r="A1560" s="47" t="s">
+      <c r="A1560" s="46" t="s">
         <v>2066</v>
       </c>
       <c r="B1560" s="3" t="s">
@@ -34540,7 +34600,7 @@
       </c>
     </row>
     <row r="1562" spans="1:2">
-      <c r="A1562" s="47" t="s">
+      <c r="A1562" s="46" t="s">
         <v>2068</v>
       </c>
       <c r="B1562" s="3" t="s">
@@ -34548,7 +34608,7 @@
       </c>
     </row>
     <row r="1563" spans="1:2">
-      <c r="A1563" s="47" t="s">
+      <c r="A1563" s="46" t="s">
         <v>2069</v>
       </c>
       <c r="B1563" s="3" t="s">
@@ -34556,7 +34616,7 @@
       </c>
     </row>
     <row r="1564" spans="1:2">
-      <c r="A1564" s="47" t="s">
+      <c r="A1564" s="46" t="s">
         <v>2070</v>
       </c>
       <c r="B1564" s="3" t="s">
@@ -34564,7 +34624,7 @@
       </c>
     </row>
     <row r="1565" spans="1:2">
-      <c r="A1565" s="47" t="s">
+      <c r="A1565" s="46" t="s">
         <v>2071</v>
       </c>
       <c r="B1565" s="3" t="s">
@@ -34572,7 +34632,7 @@
       </c>
     </row>
     <row r="1566" spans="1:2">
-      <c r="A1566" s="47" t="s">
+      <c r="A1566" s="46" t="s">
         <v>2072</v>
       </c>
       <c r="B1566" s="3" t="s">
@@ -34588,7 +34648,7 @@
       </c>
     </row>
     <row r="1568" spans="1:2">
-      <c r="A1568" s="47" t="s">
+      <c r="A1568" s="46" t="s">
         <v>2074</v>
       </c>
       <c r="B1568" s="3" t="s">
@@ -34604,7 +34664,7 @@
       </c>
     </row>
     <row r="1570" spans="1:2">
-      <c r="A1570" s="47" t="s">
+      <c r="A1570" s="46" t="s">
         <v>2076</v>
       </c>
       <c r="B1570" s="3" t="s">
@@ -34620,7 +34680,7 @@
       </c>
     </row>
     <row r="1572" spans="1:2">
-      <c r="A1572" s="47" t="s">
+      <c r="A1572" s="46" t="s">
         <v>2077</v>
       </c>
       <c r="B1572" s="3" t="s">
@@ -34636,7 +34696,7 @@
       </c>
     </row>
     <row r="1574" spans="1:2">
-      <c r="A1574" s="47" t="s">
+      <c r="A1574" s="46" t="s">
         <v>2079</v>
       </c>
       <c r="B1574" s="3" t="s">
@@ -34652,7 +34712,7 @@
       </c>
     </row>
     <row r="1576" spans="1:2">
-      <c r="A1576" s="47" t="s">
+      <c r="A1576" s="46" t="s">
         <v>2081</v>
       </c>
       <c r="B1576" s="3" t="s">
@@ -34660,7 +34720,7 @@
       </c>
     </row>
     <row r="1577" spans="1:2">
-      <c r="A1577" s="47" t="s">
+      <c r="A1577" s="46" t="s">
         <v>2082</v>
       </c>
       <c r="B1577" s="3" t="s">
@@ -34676,7 +34736,7 @@
       </c>
     </row>
     <row r="1579" spans="1:2">
-      <c r="A1579" s="47" t="s">
+      <c r="A1579" s="46" t="s">
         <v>2084</v>
       </c>
       <c r="B1579" s="3" t="s">
@@ -34684,7 +34744,7 @@
       </c>
     </row>
     <row r="1580" spans="1:2">
-      <c r="A1580" s="47" t="s">
+      <c r="A1580" s="46" t="s">
         <v>2085</v>
       </c>
       <c r="B1580" s="3" t="s">
@@ -34692,7 +34752,7 @@
       </c>
     </row>
     <row r="1581" spans="1:2">
-      <c r="A1581" s="47" t="s">
+      <c r="A1581" s="46" t="s">
         <v>2086</v>
       </c>
       <c r="B1581" s="3" t="s">
@@ -34708,7 +34768,7 @@
       </c>
     </row>
     <row r="1583" spans="1:2">
-      <c r="A1583" s="47" t="s">
+      <c r="A1583" s="46" t="s">
         <v>2088</v>
       </c>
       <c r="B1583" s="3" t="s">
@@ -34716,7 +34776,7 @@
       </c>
     </row>
     <row r="1584" spans="1:2">
-      <c r="A1584" s="47" t="s">
+      <c r="A1584" s="46" t="s">
         <v>2089</v>
       </c>
       <c r="B1584" s="3" t="s">
@@ -34724,7 +34784,7 @@
       </c>
     </row>
     <row r="1585" spans="1:2">
-      <c r="A1585" s="47" t="s">
+      <c r="A1585" s="46" t="s">
         <v>2090</v>
       </c>
       <c r="B1585" s="3" t="s">
@@ -34732,7 +34792,7 @@
       </c>
     </row>
     <row r="1586" spans="1:2">
-      <c r="A1586" s="47" t="s">
+      <c r="A1586" s="46" t="s">
         <v>2091</v>
       </c>
       <c r="B1586" s="3" t="s">
@@ -34740,7 +34800,7 @@
       </c>
     </row>
     <row r="1587" spans="1:2">
-      <c r="A1587" s="47" t="s">
+      <c r="A1587" s="46" t="s">
         <v>2092</v>
       </c>
       <c r="B1587" s="3" t="s">
@@ -34756,7 +34816,7 @@
       </c>
     </row>
     <row r="1589" spans="1:2">
-      <c r="A1589" s="47" t="s">
+      <c r="A1589" s="46" t="s">
         <v>2094</v>
       </c>
       <c r="B1589" s="3" t="s">
@@ -34764,7 +34824,7 @@
       </c>
     </row>
     <row r="1590" spans="1:2" ht="20.399999999999999">
-      <c r="A1590" s="49" t="s">
+      <c r="A1590" s="48" t="s">
         <v>2095</v>
       </c>
       <c r="B1590" s="3" t="s">
@@ -34772,7 +34832,7 @@
       </c>
     </row>
     <row r="1591" spans="1:2">
-      <c r="A1591" s="47" t="s">
+      <c r="A1591" s="46" t="s">
         <v>2096</v>
       </c>
       <c r="B1591" s="3" t="s">
@@ -34780,7 +34840,7 @@
       </c>
     </row>
     <row r="1592" spans="1:2">
-      <c r="A1592" s="47" t="s">
+      <c r="A1592" s="46" t="s">
         <v>2097</v>
       </c>
       <c r="B1592" s="3" t="s">
@@ -34788,7 +34848,7 @@
       </c>
     </row>
     <row r="1593" spans="1:2">
-      <c r="A1593" s="47" t="s">
+      <c r="A1593" s="46" t="s">
         <v>2098</v>
       </c>
       <c r="B1593" s="3" t="s">
@@ -34796,7 +34856,7 @@
       </c>
     </row>
     <row r="1594" spans="1:2">
-      <c r="A1594" s="47" t="s">
+      <c r="A1594" s="46" t="s">
         <v>2099</v>
       </c>
       <c r="B1594" s="3" t="s">
@@ -34812,7 +34872,7 @@
       </c>
     </row>
     <row r="1596" spans="1:2">
-      <c r="A1596" s="47" t="s">
+      <c r="A1596" s="46" t="s">
         <v>2101</v>
       </c>
       <c r="B1596" s="3" t="s">
@@ -34820,7 +34880,7 @@
       </c>
     </row>
     <row r="1597" spans="1:2">
-      <c r="A1597" s="47" t="s">
+      <c r="A1597" s="46" t="s">
         <v>2102</v>
       </c>
       <c r="B1597" s="3" t="s">
@@ -34836,7 +34896,7 @@
       </c>
     </row>
     <row r="1599" spans="1:2">
-      <c r="A1599" s="47" t="s">
+      <c r="A1599" s="46" t="s">
         <v>2104</v>
       </c>
       <c r="B1599" s="3" t="s">
@@ -34844,7 +34904,7 @@
       </c>
     </row>
     <row r="1600" spans="1:2">
-      <c r="A1600" s="47" t="s">
+      <c r="A1600" s="46" t="s">
         <v>2105</v>
       </c>
       <c r="B1600" s="3" t="s">
@@ -34852,7 +34912,7 @@
       </c>
     </row>
     <row r="1601" spans="1:2">
-      <c r="A1601" s="47" t="s">
+      <c r="A1601" s="46" t="s">
         <v>2106</v>
       </c>
       <c r="B1601" s="3" t="s">
@@ -34860,7 +34920,7 @@
       </c>
     </row>
     <row r="1602" spans="1:2">
-      <c r="A1602" s="47" t="s">
+      <c r="A1602" s="46" t="s">
         <v>2107</v>
       </c>
       <c r="B1602" s="3" t="s">
@@ -34868,7 +34928,7 @@
       </c>
     </row>
     <row r="1603" spans="1:2">
-      <c r="A1603" s="47" t="s">
+      <c r="A1603" s="46" t="s">
         <v>2108</v>
       </c>
       <c r="B1603" s="3" t="s">
@@ -34876,7 +34936,7 @@
       </c>
     </row>
     <row r="1604" spans="1:2">
-      <c r="A1604" s="47" t="s">
+      <c r="A1604" s="46" t="s">
         <v>2109</v>
       </c>
       <c r="B1604" s="3" t="s">
@@ -34884,7 +34944,7 @@
       </c>
     </row>
     <row r="1605" spans="1:2">
-      <c r="A1605" s="47" t="s">
+      <c r="A1605" s="46" t="s">
         <v>2110</v>
       </c>
       <c r="B1605" s="3" t="s">
@@ -34892,7 +34952,7 @@
       </c>
     </row>
     <row r="1606" spans="1:2">
-      <c r="A1606" s="47" t="s">
+      <c r="A1606" s="46" t="s">
         <v>2111</v>
       </c>
       <c r="B1606" s="3" t="s">
@@ -34900,7 +34960,7 @@
       </c>
     </row>
     <row r="1607" spans="1:2">
-      <c r="A1607" s="47" t="s">
+      <c r="A1607" s="46" t="s">
         <v>2112</v>
       </c>
       <c r="B1607" s="3" t="s">
@@ -34908,7 +34968,7 @@
       </c>
     </row>
     <row r="1608" spans="1:2">
-      <c r="A1608" s="47" t="s">
+      <c r="A1608" s="46" t="s">
         <v>2113</v>
       </c>
       <c r="B1608" s="3" t="s">
@@ -34916,7 +34976,7 @@
       </c>
     </row>
     <row r="1609" spans="1:2">
-      <c r="A1609" s="47" t="s">
+      <c r="A1609" s="46" t="s">
         <v>2114</v>
       </c>
       <c r="B1609" s="3" t="s">
@@ -34924,7 +34984,7 @@
       </c>
     </row>
     <row r="1610" spans="1:2">
-      <c r="A1610" s="47" t="s">
+      <c r="A1610" s="46" t="s">
         <v>2115</v>
       </c>
       <c r="B1610" s="3" t="s">
@@ -34932,7 +34992,7 @@
       </c>
     </row>
     <row r="1611" spans="1:2">
-      <c r="A1611" s="47" t="s">
+      <c r="A1611" s="46" t="s">
         <v>2116</v>
       </c>
       <c r="B1611" s="3" t="s">
@@ -34940,7 +35000,7 @@
       </c>
     </row>
     <row r="1612" spans="1:2">
-      <c r="A1612" s="47" t="s">
+      <c r="A1612" s="46" t="s">
         <v>2117</v>
       </c>
       <c r="B1612" s="3" t="s">
@@ -34948,7 +35008,7 @@
       </c>
     </row>
     <row r="1613" spans="1:2" ht="20.399999999999999">
-      <c r="A1613" s="49" t="s">
+      <c r="A1613" s="48" t="s">
         <v>2118</v>
       </c>
       <c r="B1613" s="14" t="s">
@@ -34956,7 +35016,7 @@
       </c>
     </row>
     <row r="1614" spans="1:2">
-      <c r="A1614" s="47" t="s">
+      <c r="A1614" s="46" t="s">
         <v>2119</v>
       </c>
       <c r="B1614" s="14" t="s">
@@ -34964,7 +35024,7 @@
       </c>
     </row>
     <row r="1615" spans="1:2">
-      <c r="A1615" s="47" t="s">
+      <c r="A1615" s="46" t="s">
         <v>2120</v>
       </c>
       <c r="B1615" s="3" t="s">
@@ -34980,7 +35040,7 @@
       </c>
     </row>
     <row r="1617" spans="1:2">
-      <c r="A1617" s="47" t="s">
+      <c r="A1617" s="46" t="s">
         <v>2122</v>
       </c>
       <c r="B1617" s="3" t="s">
@@ -34988,7 +35048,7 @@
       </c>
     </row>
     <row r="1618" spans="1:2">
-      <c r="A1618" s="47" t="s">
+      <c r="A1618" s="46" t="s">
         <v>2123</v>
       </c>
       <c r="B1618" s="3" t="s">
@@ -35004,7 +35064,7 @@
       </c>
     </row>
     <row r="1620" spans="1:2">
-      <c r="A1620" s="47" t="s">
+      <c r="A1620" s="46" t="s">
         <v>2125</v>
       </c>
       <c r="B1620" s="3" t="s">
@@ -35012,7 +35072,7 @@
       </c>
     </row>
     <row r="1621" spans="1:2">
-      <c r="A1621" s="47" t="s">
+      <c r="A1621" s="46" t="s">
         <v>2126</v>
       </c>
       <c r="B1621" s="3" t="s">
@@ -35020,7 +35080,7 @@
       </c>
     </row>
     <row r="1622" spans="1:2">
-      <c r="A1622" s="47" t="s">
+      <c r="A1622" s="46" t="s">
         <v>2128</v>
       </c>
       <c r="B1622" s="3" t="s">
@@ -35044,7 +35104,7 @@
       </c>
     </row>
     <row r="1625" spans="1:2">
-      <c r="A1625" s="47" t="s">
+      <c r="A1625" s="46" t="s">
         <v>2130</v>
       </c>
       <c r="B1625" s="3" t="s">
@@ -35052,7 +35112,7 @@
       </c>
     </row>
     <row r="1626" spans="1:2">
-      <c r="A1626" s="47" t="s">
+      <c r="A1626" s="46" t="s">
         <v>2131</v>
       </c>
       <c r="B1626" s="14" t="s">
@@ -35060,7 +35120,7 @@
       </c>
     </row>
     <row r="1627" spans="1:2">
-      <c r="A1627" s="47" t="s">
+      <c r="A1627" s="46" t="s">
         <v>2132</v>
       </c>
       <c r="B1627" s="14" t="s">
@@ -35068,7 +35128,7 @@
       </c>
     </row>
     <row r="1628" spans="1:2">
-      <c r="A1628" s="47" t="s">
+      <c r="A1628" s="46" t="s">
         <v>2134</v>
       </c>
       <c r="B1628" s="3" t="s">
@@ -35076,7 +35136,7 @@
       </c>
     </row>
     <row r="1629" spans="1:2">
-      <c r="A1629" s="47" t="s">
+      <c r="A1629" s="46" t="s">
         <v>2133</v>
       </c>
       <c r="B1629" s="3" t="s">
@@ -35084,56 +35144,56 @@
       </c>
     </row>
     <row r="1630" spans="1:2">
-      <c r="A1630" s="47" t="s">
-        <v>2139</v>
+      <c r="A1630" s="46" t="s">
+        <v>2138</v>
       </c>
       <c r="B1630" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="1631" spans="1:2" ht="26.4">
-      <c r="A1631" s="50" t="s">
-        <v>2140</v>
+      <c r="A1631" s="49" t="s">
+        <v>2139</v>
       </c>
       <c r="B1631" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="1632" spans="1:2">
-      <c r="A1632" s="47" t="s">
+      <c r="A1632" s="46" t="s">
+        <v>2140</v>
+      </c>
+      <c r="B1632" s="46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:2">
+      <c r="A1633" s="46" t="s">
         <v>2141</v>
       </c>
-      <c r="B1632" s="47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1633" spans="1:2">
-      <c r="A1633" s="47" t="s">
+      <c r="B1633" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:2">
+      <c r="A1634" s="46" t="s">
         <v>2142</v>
       </c>
-      <c r="B1633" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1634" spans="1:2">
-      <c r="A1634" s="47" t="s">
+      <c r="B1634" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:2">
+      <c r="A1635" s="46" t="s">
         <v>2143</v>
-      </c>
-      <c r="B1634" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1635" spans="1:2">
-      <c r="A1635" s="47" t="s">
-        <v>2144</v>
       </c>
       <c r="B1635" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="1636" spans="1:2">
-      <c r="A1636" s="47" t="s">
-        <v>2145</v>
+      <c r="A1636" s="46" t="s">
+        <v>2144</v>
       </c>
       <c r="B1636" s="3" t="s">
         <v>34</v>
@@ -35141,151 +35201,151 @@
     </row>
     <row r="1637" spans="1:2" ht="28.8">
       <c r="A1637" s="13" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="B1637" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="1638" spans="1:2">
-      <c r="A1638" s="47" t="s">
+      <c r="A1638" s="46" t="s">
+        <v>2145</v>
+      </c>
+      <c r="B1638" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:2">
+      <c r="A1639" s="46" t="s">
         <v>2146</v>
-      </c>
-      <c r="B1638" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1639" spans="1:2">
-      <c r="A1639" s="47" t="s">
-        <v>2147</v>
       </c>
       <c r="B1639" s="3" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="1640" spans="1:2">
-      <c r="A1640" s="47" t="s">
-        <v>2148</v>
+      <c r="A1640" s="46" t="s">
+        <v>2147</v>
       </c>
       <c r="B1640" s="3" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="1641" spans="1:2">
-      <c r="A1641" s="47" t="s">
+      <c r="A1641" s="46" t="s">
+        <v>2149</v>
+      </c>
+      <c r="B1641" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:2">
+      <c r="A1642" s="46" t="s">
         <v>2150</v>
-      </c>
-      <c r="B1641" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1642" spans="1:2">
-      <c r="A1642" s="47" t="s">
-        <v>2151</v>
       </c>
       <c r="B1642" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1643" spans="1:2">
-      <c r="A1643" s="47" t="s">
+      <c r="A1643" s="46" t="s">
+        <v>2151</v>
+      </c>
+      <c r="B1643" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:2">
+      <c r="A1644" s="46" t="s">
         <v>2152</v>
       </c>
-      <c r="B1643" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1644" spans="1:2">
-      <c r="A1644" s="47" t="s">
+      <c r="B1644" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:2">
+      <c r="A1645" s="46" t="s">
         <v>2153</v>
       </c>
-      <c r="B1644" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1645" spans="1:2">
-      <c r="A1645" s="47" t="s">
+      <c r="B1645" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:2">
+      <c r="A1646" s="46" t="s">
         <v>2154</v>
-      </c>
-      <c r="B1645" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1646" spans="1:2">
-      <c r="A1646" s="47" t="s">
-        <v>2155</v>
       </c>
       <c r="B1646" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1647" spans="1:2">
-      <c r="A1647" s="47" t="s">
-        <v>2156</v>
+      <c r="A1647" s="46" t="s">
+        <v>2155</v>
       </c>
       <c r="B1647" s="3" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="1648" spans="1:2">
-      <c r="A1648" s="47" t="s">
-        <v>2157</v>
+      <c r="A1648" s="46" t="s">
+        <v>2156</v>
       </c>
       <c r="B1648" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1649" spans="1:2">
-      <c r="A1649" s="47" t="s">
+      <c r="A1649" s="46" t="s">
+        <v>2157</v>
+      </c>
+      <c r="B1649" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:2">
+      <c r="A1650" s="46" t="s">
         <v>2158</v>
-      </c>
-      <c r="B1649" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1650" spans="1:2">
-      <c r="A1650" s="47" t="s">
-        <v>2159</v>
       </c>
       <c r="B1650" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1651" spans="1:2">
-      <c r="A1651" s="47" t="s">
-        <v>2160</v>
+      <c r="A1651" s="46" t="s">
+        <v>2159</v>
       </c>
       <c r="B1651" s="3" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="1652" spans="1:2">
-      <c r="A1652" s="47" t="s">
-        <v>2161</v>
+      <c r="A1652" s="46" t="s">
+        <v>2160</v>
       </c>
       <c r="B1652" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1653" spans="1:2">
-      <c r="A1653" s="47" t="s">
-        <v>2162</v>
+      <c r="A1653" s="46" t="s">
+        <v>2161</v>
       </c>
       <c r="B1653" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1654" spans="1:2">
-      <c r="A1654" s="47" t="s">
-        <v>2163</v>
+      <c r="A1654" s="46" t="s">
+        <v>2162</v>
       </c>
       <c r="B1654" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1655" spans="1:2">
-      <c r="A1655" s="47" t="s">
-        <v>2164</v>
+      <c r="A1655" s="46" t="s">
+        <v>2163</v>
       </c>
       <c r="B1655" s="3" t="s">
         <v>8</v>
@@ -35293,87 +35353,87 @@
     </row>
     <row r="1656" spans="1:2">
       <c r="A1656" s="13" t="s">
+        <v>2164</v>
+      </c>
+      <c r="B1656" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:2">
+      <c r="A1657" s="46" t="s">
         <v>2165</v>
-      </c>
-      <c r="B1656" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1657" spans="1:2">
-      <c r="A1657" s="47" t="s">
-        <v>2166</v>
       </c>
       <c r="B1657" s="3" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="1658" spans="1:2" ht="39.6">
-      <c r="A1658" s="50" t="s">
-        <v>2167</v>
+      <c r="A1658" s="49" t="s">
+        <v>2166</v>
       </c>
       <c r="B1658" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1659" spans="1:2">
-      <c r="A1659" s="47" t="s">
+      <c r="A1659" s="46" t="s">
+        <v>2167</v>
+      </c>
+      <c r="B1659" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:2">
+      <c r="A1660" s="46" t="s">
         <v>2168</v>
       </c>
-      <c r="B1659" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1660" spans="1:2">
-      <c r="A1660" s="47" t="s">
+      <c r="B1660" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:2">
+      <c r="A1661" s="46" t="s">
         <v>2169</v>
-      </c>
-      <c r="B1660" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1661" spans="1:2">
-      <c r="A1661" s="47" t="s">
-        <v>2170</v>
       </c>
       <c r="B1661" s="3" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="1662" spans="1:2">
-      <c r="A1662" s="47" t="s">
-        <v>2171</v>
+      <c r="A1662" s="46" t="s">
+        <v>2170</v>
       </c>
       <c r="B1662" s="3" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="1663" spans="1:2">
-      <c r="A1663" s="47" t="s">
-        <v>2172</v>
+      <c r="A1663" s="46" t="s">
+        <v>2171</v>
       </c>
       <c r="B1663" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="1664" spans="1:2">
-      <c r="A1664" s="47" t="s">
-        <v>2174</v>
+      <c r="A1664" s="46" t="s">
+        <v>2173</v>
       </c>
       <c r="B1664" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1665" spans="1:2">
-      <c r="A1665" s="47" t="s">
-        <v>2173</v>
+      <c r="A1665" s="46" t="s">
+        <v>2172</v>
       </c>
       <c r="B1665" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="1666" spans="1:2">
-      <c r="A1666" s="47" t="s">
-        <v>2175</v>
+      <c r="A1666" s="46" t="s">
+        <v>2174</v>
       </c>
       <c r="B1666" s="3" t="s">
         <v>8</v>
@@ -35381,7 +35441,7 @@
     </row>
     <row r="1667" spans="1:2" ht="43.2">
       <c r="A1667" s="13" t="s">
-        <v>2177</v>
+        <v>2175</v>
       </c>
       <c r="B1667" s="3" t="s">
         <v>34</v>
@@ -35389,111 +35449,111 @@
     </row>
     <row r="1668" spans="1:2">
       <c r="A1668" s="13" t="s">
-        <v>2178</v>
+        <v>2176</v>
       </c>
       <c r="B1668" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="1669" spans="1:2">
-      <c r="A1669" s="47" t="s">
+      <c r="A1669" s="46" t="s">
+        <v>2177</v>
+      </c>
+      <c r="B1669" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:2">
+      <c r="A1670" s="46" t="s">
+        <v>2178</v>
+      </c>
+      <c r="B1670" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:2">
+      <c r="A1671" s="46" t="s">
         <v>2179</v>
       </c>
-      <c r="B1669" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1670" spans="1:2">
-      <c r="A1670" s="47" t="s">
+      <c r="B1671" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:2">
+      <c r="A1672" s="46" t="s">
         <v>2180</v>
-      </c>
-      <c r="B1670" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1671" spans="1:2">
-      <c r="A1671" s="47" t="s">
-        <v>2181</v>
-      </c>
-      <c r="B1671" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1672" spans="1:2">
-      <c r="A1672" s="47" t="s">
-        <v>2182</v>
       </c>
       <c r="B1672" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="1673" spans="1:2">
-      <c r="A1673" s="47" t="s">
-        <v>2183</v>
+      <c r="A1673" s="46" t="s">
+        <v>2181</v>
       </c>
       <c r="B1673" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="1674" spans="1:2">
-      <c r="A1674" s="47" t="s">
-        <v>2184</v>
+      <c r="A1674" s="46" t="s">
+        <v>2182</v>
       </c>
       <c r="B1674" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="1675" spans="1:2">
-      <c r="A1675" s="47" t="s">
-        <v>2185</v>
+      <c r="A1675" s="46" t="s">
+        <v>2183</v>
       </c>
       <c r="B1675" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="1676" spans="1:2">
-      <c r="A1676" s="47" t="s">
+      <c r="A1676" s="46" t="s">
+        <v>2184</v>
+      </c>
+      <c r="B1676" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:2">
+      <c r="A1677" s="46" t="s">
+        <v>2185</v>
+      </c>
+      <c r="B1677" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:2">
+      <c r="A1678" s="46" t="s">
         <v>2186</v>
       </c>
-      <c r="B1676" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1677" spans="1:2">
-      <c r="A1677" s="47" t="s">
+      <c r="B1678" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:2">
+      <c r="A1679" s="46" t="s">
+        <v>2188</v>
+      </c>
+      <c r="B1679" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:2">
+      <c r="A1680" s="46" t="s">
         <v>2187</v>
       </c>
-      <c r="B1677" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1678" spans="1:2">
-      <c r="A1678" s="47" t="s">
-        <v>2188</v>
-      </c>
-      <c r="B1678" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1679" spans="1:2">
-      <c r="A1679" s="47" t="s">
-        <v>2190</v>
-      </c>
-      <c r="B1679" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1680" spans="1:2">
-      <c r="A1680" s="47" t="s">
+      <c r="B1680" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:2" ht="28.8">
+      <c r="A1681" s="13" t="s">
         <v>2189</v>
-      </c>
-      <c r="B1680" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1681" spans="1:2">
-      <c r="A1681" s="13" t="s">
-        <v>2191</v>
       </c>
       <c r="B1681" s="3" t="s">
         <v>5</v>
@@ -35501,15 +35561,15 @@
     </row>
     <row r="1682" spans="1:2" ht="28.8">
       <c r="A1682" s="13" t="s">
-        <v>2192</v>
+        <v>2190</v>
       </c>
       <c r="B1682" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="1683" spans="1:2" ht="28.8">
+    <row r="1683" spans="1:2">
       <c r="A1683" s="13" t="s">
-        <v>2193</v>
+        <v>2191</v>
       </c>
       <c r="B1683" s="3" t="s">
         <v>8</v>
@@ -35517,23 +35577,23 @@
     </row>
     <row r="1684" spans="1:2">
       <c r="A1684" s="13" t="s">
-        <v>2194</v>
+        <v>2192</v>
       </c>
       <c r="B1684" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="1685" spans="1:2">
-      <c r="A1685" s="47" t="s">
-        <v>2195</v>
+      <c r="A1685" s="46" t="s">
+        <v>2193</v>
       </c>
       <c r="B1685" s="3" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="1686" spans="1:2">
+    <row r="1686" spans="1:2" ht="28.8">
       <c r="A1686" s="13" t="s">
-        <v>2196</v>
+        <v>2194</v>
       </c>
       <c r="B1686" s="3" t="s">
         <v>664</v>
@@ -35541,31 +35601,31 @@
     </row>
     <row r="1687" spans="1:2" ht="28.8">
       <c r="A1687" s="13" t="s">
+        <v>2195</v>
+      </c>
+      <c r="B1687" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:2">
+      <c r="A1688" s="46" t="s">
+        <v>2196</v>
+      </c>
+      <c r="B1688" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:2">
+      <c r="A1689" s="46" t="s">
         <v>2197</v>
-      </c>
-      <c r="B1687" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1688" spans="1:2" ht="28.8">
-      <c r="A1688" s="47" t="s">
-        <v>2198</v>
-      </c>
-      <c r="B1688" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1689" spans="1:2">
-      <c r="A1689" s="47" t="s">
-        <v>2199</v>
       </c>
       <c r="B1689" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="1690" spans="1:2">
-      <c r="A1690" s="47" t="s">
-        <v>2200</v>
+      <c r="A1690" s="46" t="s">
+        <v>2198</v>
       </c>
       <c r="B1690" s="3" t="s">
         <v>8</v>
@@ -35573,127 +35633,127 @@
     </row>
     <row r="1691" spans="1:2">
       <c r="A1691" s="13" t="s">
+        <v>2199</v>
+      </c>
+      <c r="B1691" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:2">
+      <c r="A1692" s="46" t="s">
+        <v>2200</v>
+      </c>
+      <c r="B1692" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:2">
+      <c r="A1693" s="46" t="s">
         <v>2201</v>
       </c>
-      <c r="B1691" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1692" spans="1:2">
-      <c r="A1692" s="47" t="s">
+      <c r="B1693" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:2">
+      <c r="A1694" s="46" t="s">
         <v>2202</v>
       </c>
-      <c r="B1692" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1693" spans="1:2">
-      <c r="A1693" s="47" t="s">
+      <c r="B1694" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:2" ht="43.2">
+      <c r="A1695" s="13" t="s">
         <v>2203</v>
       </c>
-      <c r="B1693" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1694" spans="1:2">
-      <c r="A1694" s="47" t="s">
+      <c r="B1695" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:2">
+      <c r="A1696" s="46" t="s">
         <v>2204</v>
       </c>
-      <c r="B1694" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1695" spans="1:2">
-      <c r="A1695" s="13" t="s">
+      <c r="B1696" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:2">
+      <c r="A1697" s="46" t="s">
         <v>2205</v>
-      </c>
-      <c r="B1695" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1696" spans="1:2" ht="43.2">
-      <c r="A1696" s="47" t="s">
-        <v>2206</v>
-      </c>
-      <c r="B1696" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1697" spans="1:2">
-      <c r="A1697" s="47" t="s">
-        <v>2207</v>
       </c>
       <c r="B1697" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="1698" spans="1:2">
-      <c r="A1698" s="47" t="s">
-        <v>2208</v>
+      <c r="A1698" s="46" t="s">
+        <v>2206</v>
       </c>
       <c r="B1698" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="1699" spans="1:2">
-      <c r="A1699" s="47" t="s">
-        <v>2209</v>
+      <c r="A1699" s="46" t="s">
+        <v>2207</v>
       </c>
       <c r="B1699" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="1700" spans="1:2">
+    <row r="1700" spans="1:2" ht="43.2">
       <c r="A1700" s="13" t="s">
+        <v>2209</v>
+      </c>
+      <c r="B1700" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:2">
+      <c r="A1701" s="46" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B1701" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:2">
+      <c r="A1702" s="54" t="s">
         <v>2211</v>
-      </c>
-      <c r="B1700" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1701" spans="1:2" ht="43.2">
-      <c r="A1701" s="47" t="s">
-        <v>2212</v>
-      </c>
-      <c r="B1701" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1702" spans="1:2">
-      <c r="A1702" s="55" t="s">
-        <v>2213</v>
       </c>
       <c r="B1702" s="3" t="s">
         <v>2021</v>
       </c>
     </row>
     <row r="1703" spans="1:2">
-      <c r="A1703" s="47" t="s">
-        <v>2214</v>
+      <c r="A1703" s="46" t="s">
+        <v>2212</v>
       </c>
       <c r="B1703" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1704" spans="1:2">
-      <c r="A1704" s="47" t="s">
+      <c r="A1704" s="46" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B1704" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:2">
+      <c r="A1705" s="46" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B1705" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:2" ht="28.8">
+      <c r="A1706" s="13" t="s">
         <v>2215</v>
-      </c>
-      <c r="B1704" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1705" spans="1:2">
-      <c r="A1705" s="47" t="s">
-        <v>2216</v>
-      </c>
-      <c r="B1705" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1706" spans="1:2">
-      <c r="A1706" s="13" t="s">
-        <v>2217</v>
       </c>
       <c r="B1706" s="3" t="s">
         <v>8</v>
@@ -35701,47 +35761,47 @@
     </row>
     <row r="1707" spans="1:2" ht="28.8">
       <c r="A1707" s="13" t="s">
-        <v>2218</v>
+        <v>2216</v>
       </c>
       <c r="B1707" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="1708" spans="1:2" ht="28.8">
-      <c r="A1708" s="47" t="s">
-        <v>2219</v>
+    <row r="1708" spans="1:2">
+      <c r="A1708" s="46" t="s">
+        <v>2217</v>
       </c>
       <c r="B1708" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="1709" spans="1:2">
-      <c r="A1709" s="55" t="s">
-        <v>2220</v>
+      <c r="A1709" s="54" t="s">
+        <v>2218</v>
       </c>
       <c r="B1709" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="1710" spans="1:2">
-      <c r="A1710" s="48" t="s">
-        <v>2221</v>
+    <row r="1710" spans="1:2" ht="26.4">
+      <c r="A1710" s="47" t="s">
+        <v>2219</v>
       </c>
       <c r="B1710" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="1711" spans="1:2" ht="26.4">
-      <c r="A1711" s="47" t="s">
-        <v>2222</v>
+    <row r="1711" spans="1:2">
+      <c r="A1711" s="46" t="s">
+        <v>2220</v>
       </c>
       <c r="B1711" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="1712" spans="1:2">
-      <c r="A1712" s="47" t="s">
-        <v>2223</v>
+      <c r="A1712" s="46" t="s">
+        <v>2221</v>
       </c>
       <c r="B1712" s="3" t="s">
         <v>7</v>
@@ -35749,23 +35809,23 @@
     </row>
     <row r="1713" spans="1:2">
       <c r="A1713" s="13" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="B1713" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="1714" spans="1:2" ht="35.4" customHeight="1">
-      <c r="A1714" s="50" t="s">
-        <v>2225</v>
+      <c r="A1714" s="49" t="s">
+        <v>2223</v>
       </c>
       <c r="B1714" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="1715" spans="1:2" ht="26.4">
+    <row r="1715" spans="1:2">
       <c r="A1715" s="13" t="s">
-        <v>2226</v>
+        <v>2224</v>
       </c>
       <c r="B1715" s="3" t="s">
         <v>34</v>
@@ -35773,39 +35833,39 @@
     </row>
     <row r="1716" spans="1:2">
       <c r="A1716" s="13" t="s">
-        <v>2227</v>
+        <v>2225</v>
       </c>
       <c r="B1716" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="1717" spans="1:2">
-      <c r="A1717" s="47" t="s">
-        <v>2228</v>
+      <c r="A1717" s="46" t="s">
+        <v>2226</v>
       </c>
       <c r="B1717" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="1718" spans="1:2">
+    <row r="1718" spans="1:2" ht="28.8">
       <c r="A1718" s="13" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
       <c r="B1718" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="1719" spans="1:2" ht="28.8">
-      <c r="A1719" s="47" t="s">
-        <v>2230</v>
+    <row r="1719" spans="1:2">
+      <c r="A1719" s="46" t="s">
+        <v>2228</v>
       </c>
       <c r="B1719" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="1720" spans="1:2">
-      <c r="A1720" s="47" t="s">
-        <v>2231</v>
+      <c r="A1720" s="46" t="s">
+        <v>2229</v>
       </c>
       <c r="B1720" s="3" t="s">
         <v>34</v>
@@ -35813,15 +35873,147 @@
     </row>
     <row r="1721" spans="1:2">
       <c r="A1721" s="13" t="s">
-        <v>2232</v>
+        <v>2230</v>
       </c>
       <c r="B1721" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="1722" spans="1:2">
-      <c r="A1722"/>
-      <c r="B1722"/>
+      <c r="A1722" s="46" t="s">
+        <v>2231</v>
+      </c>
+      <c r="B1722" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:2" ht="79.2">
+      <c r="A1723" s="43" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B1723" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:2" ht="59.4">
+      <c r="A1724" s="43" t="s">
+        <v>2233</v>
+      </c>
+      <c r="B1724" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:2" ht="59.4">
+      <c r="A1725" s="43" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B1725" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:2" ht="39.6">
+      <c r="A1726" s="43" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B1726" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:2" ht="59.4">
+      <c r="A1727" s="43" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B1727" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:2" ht="79.2">
+      <c r="A1728" s="43" t="s">
+        <v>2237</v>
+      </c>
+      <c r="B1728" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:2" ht="59.4">
+      <c r="A1729" s="43" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B1729" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:2" ht="28.8">
+      <c r="A1730" s="13" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B1730" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:2" ht="28.8">
+      <c r="A1731" s="13" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B1731" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:2" ht="28.8">
+      <c r="A1732" s="13" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B1732" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:2" ht="28.8">
+      <c r="A1733" s="13" t="s">
+        <v>2243</v>
+      </c>
+      <c r="B1733" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:2" ht="43.2">
+      <c r="A1734" s="13" t="s">
+        <v>2246</v>
+      </c>
+      <c r="B1734" s="3" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:2" ht="28.8">
+      <c r="A1735" s="13" t="s">
+        <v>2247</v>
+      </c>
+      <c r="B1735" s="14" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:2" ht="28.8">
+      <c r="A1736" s="13" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B1736" s="14" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:2">
+      <c r="A1737" s="46" t="s">
+        <v>2249</v>
+      </c>
+      <c r="B1737" s="14" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:2">
+      <c r="A1738" s="46" t="s">
+        <v>2250</v>
+      </c>
+      <c r="B1738" s="14" t="s">
+        <v>664</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35832,27 +36024,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5386CA97-9DB9-4D9E-A52E-CC64BCC04B59}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>2136</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>2137</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>2138</v>
-      </c>
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1">
-      <c r="A2" s="54">
+      <c r="A2" s="53">
         <v>44256</v>
       </c>
       <c r="B2" s="8">
@@ -35864,7 +36059,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="54">
+      <c r="A3" s="53">
         <v>44317</v>
       </c>
       <c r="B3">
@@ -35877,7 +36072,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>2135</v>
+        <v>2245</v>
       </c>
       <c r="B4">
         <v>1417</v>
@@ -35889,7 +36084,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>2176</v>
+        <v>2244</v>
       </c>
       <c r="B5">
         <v>1662</v>
@@ -35900,7 +36095,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>2210</v>
+        <v>2208</v>
       </c>
       <c r="B6">
         <v>1667</v>
@@ -35908,6 +36103,39 @@
       <c r="C6">
         <f>1721-B6</f>
         <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>2239</v>
+      </c>
+      <c r="B7">
+        <v>1723</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="8" customFormat="1">
+      <c r="A8" s="8" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1730</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B9">
+        <v>1734</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -36214,8 +36442,8 @@
         <v>30</v>
       </c>
       <c r="N11" s="9"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="55"/>
     </row>
     <row r="12" spans="1:19" s="8" customFormat="1">
       <c r="A12" s="8" t="s">

</xml_diff>